<commit_message>
Add T-65 and additional upgrades that increase armor rating to stat sheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This changes drastically if Raider Overhaul is installed, becoming much stronger</t>
         </r>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -74,19 +75,28 @@
     <t xml:space="preserve">Arms Lining F</t>
   </si>
   <si>
-    <t xml:space="preserve">Fully Upgraded Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level First Available in Leveled Sets</t>
+    <t xml:space="preserve">Highest Total for an Enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Upgrades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highest Total for a Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Partial Sets Are Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Full Sets Are Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level First Available on Enemies</t>
   </si>
   <si>
     <t xml:space="preserve">Level First Available as Legendary</t>
   </si>
   <si>
-    <t xml:space="preserve">Level First Available on Enemies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armor Rating</t>
+    <t xml:space="preserve">Armor</t>
   </si>
   <si>
     <t xml:space="preserve">Health</t>
@@ -120,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">X-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-65</t>
   </si>
   <si>
     <t xml:space="preserve">Ultracite</t>
@@ -132,11 +145,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,57 +168,92 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Lucida Sans"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -312,22 +361,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -338,27 +419,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,7 +536,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -468,26 +549,28 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -532,75 +615,89 @@
       <c r="S1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="V1" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="W1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
       <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>130</v>
@@ -658,16 +755,23 @@
         <f aca="false">SUM(J3,K3,M3,O3*2,Q3*2)</f>
         <v>980</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="T3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <f aca="false">S3+T3</f>
+        <v>980</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="0" t="n">
         <v>15</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>200</v>
@@ -725,16 +829,23 @@
         <f aca="false">SUM(J4,K4,M4,O4*2,Q4*2)</f>
         <v>620</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="T4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <f aca="false">S4+T4</f>
+        <v>620</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>200</v>
@@ -792,19 +903,29 @@
         <f aca="false">SUM(J5,K5,M5,O5*2,Q5*2)</f>
         <v>1100</v>
       </c>
-      <c r="T5" s="0" t="n">
+      <c r="T5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <f aca="false">S5+T5</f>
+        <v>1100</v>
+      </c>
+      <c r="V5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U5" s="0" t="n">
+      <c r="W5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="0" t="n">
         <v>20</v>
-      </c>
-      <c r="V5" s="0" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>230</v>
@@ -862,16 +983,24 @@
         <f aca="false">SUM(J6,K6,M6,O6*2,Q6*2)</f>
         <v>1280</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="T6" s="1" t="n">
+        <f aca="false">(25+40)*6</f>
+        <v>390</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <f aca="false">S6+T6</f>
+        <v>1670</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="V6" s="0" t="n">
-        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>240</v>
@@ -929,19 +1058,29 @@
         <f aca="false">SUM(J7,K7,M7,O7*2,Q7*2)</f>
         <v>1340</v>
       </c>
-      <c r="T7" s="0" t="n">
+      <c r="T7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1" t="n">
+        <f aca="false">S7+T7</f>
+        <v>1340</v>
+      </c>
+      <c r="V7" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="U7" s="0" t="n">
+      <c r="W7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="V7" s="0" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>240</v>
@@ -999,16 +1138,23 @@
         <f aca="false">SUM(J8,K8,M8,O8*2,Q8*2)</f>
         <v>1340</v>
       </c>
-      <c r="U8" s="0" t="n">
+      <c r="T8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1" t="n">
+        <f aca="false">S8+T8</f>
+        <v>1340</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="V8" s="0" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>360</v>
@@ -1066,16 +1212,23 @@
         <f aca="false">SUM(J9,K9,M9,O9*2,Q9*2)</f>
         <v>1380</v>
       </c>
-      <c r="U9" s="0" t="n">
+      <c r="T9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <f aca="false">S9+T9</f>
+        <v>1380</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y9" s="0" t="n">
         <v>40</v>
-      </c>
-      <c r="V9" s="0" t="n">
-        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>280</v>
@@ -1133,19 +1286,29 @@
         <f aca="false">SUM(J10,K10,M10,O10*2,Q10*2)</f>
         <v>1580</v>
       </c>
-      <c r="T10" s="0" t="n">
+      <c r="T10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <f aca="false">S10+T10</f>
+        <v>1580</v>
+      </c>
+      <c r="V10" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="U10" s="0" t="n">
+      <c r="W10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y10" s="0" t="n">
         <v>40</v>
-      </c>
-      <c r="V10" s="0" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>320</v>
@@ -1203,19 +1366,29 @@
         <f aca="false">SUM(J11,K11,M11,O11*2,Q11*2)</f>
         <v>1820</v>
       </c>
-      <c r="T11" s="0" t="n">
+      <c r="T11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <f aca="false">S11+T11</f>
+        <v>1820</v>
+      </c>
+      <c r="V11" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="W11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>380</v>
@@ -1273,44 +1446,52 @@
         <f aca="false">SUM(J12,K12,M12,O12*2,Q12*2)</f>
         <v>1975</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="T12" s="1" t="n">
+        <f aca="false">(80+20)*6+80</f>
+        <v>680</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <f aca="false">S12+T12</f>
+        <v>2655</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y12" s="0" t="n">
         <v>70</v>
-      </c>
-      <c r="V12" s="0" t="n">
-        <v>65</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>500</v>
+        <v>360</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>560</v>
+        <v>680</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>290</v>
+        <v>210</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>1860</v>
+        <v>1460</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>100</v>
@@ -1338,17 +1519,98 @@
       </c>
       <c r="S13" s="1" t="n">
         <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
+        <v>2060</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <f aca="false">S13+T13</f>
+        <v>2060</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
+        <v>1860</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
         <v>2460</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="T14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1" t="n">
+        <f aca="false">S14+T14</f>
+        <v>2460</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="Y14" s="0" t="n">
         <v>80</v>
-      </c>
-      <c r="V13" s="0" t="n">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -1363,8 +1625,11 @@
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J:J">
+  <conditionalFormatting sqref="J:J J1">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -1373,12 +1638,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{77D9D3D0-BBD7-4C52-8782-8529217DB06B}</x14:id>
+          <x14:id>{5FBD3910-8737-47C7-BDE5-BFA41760AC10}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S1048576">
+  <conditionalFormatting sqref="S2:S1048576">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -1387,12 +1652,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F02A87C5-1C96-4D98-81F1-D89FDE1A4FD4}</x14:id>
+          <x14:id>{C81F46B0-E3BF-41DB-9782-B3BB9163DC51}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T:T T1">
+  <conditionalFormatting sqref="U2:U1048576">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -1401,12 +1666,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D8C9598D-4145-4EB4-8384-20E66FA0E79B}</x14:id>
+          <x14:id>{D4C095DC-D5B6-4414-9D90-1824E775C036}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U:U U1">
+  <conditionalFormatting sqref="V2:Y1048576">
     <cfRule type="dataBar" priority="5">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -1415,21 +1680,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9AE7BEDE-1EC6-439B-9C99-E4F2A0192ADE}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V:V V1">
-    <cfRule type="dataBar" priority="6">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{58D258EB-4088-4193-9AB1-C9CBC0F78443}</x14:id>
+          <x14:id>{B5C05C49-6064-40C7-BF47-3FE71816C983}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1446,18 +1697,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{77D9D3D0-BBD7-4C52-8782-8529217DB06B}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>J:J</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F02A87C5-1C96-4D98-81F1-D89FDE1A4FD4}">
+          <x14:cfRule type="dataBar" id="{5FBD3910-8737-47C7-BDE5-BFA41760AC10}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1465,10 +1705,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S3:S1048576</xm:sqref>
+          <xm:sqref>J:J J1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D8C9598D-4145-4EB4-8384-20E66FA0E79B}">
+          <x14:cfRule type="dataBar" id="{C81F46B0-E3BF-41DB-9782-B3BB9163DC51}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1476,10 +1716,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>T:T T1</xm:sqref>
+          <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9AE7BEDE-1EC6-439B-9C99-E4F2A0192ADE}">
+          <x14:cfRule type="dataBar" id="{D4C095DC-D5B6-4414-9D90-1824E775C036}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1487,10 +1727,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U:U U1</xm:sqref>
+          <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{58D258EB-4088-4193-9AB1-C9CBC0F78443}">
+          <x14:cfRule type="dataBar" id="{B5C05C49-6064-40C7-BF47-3FE71816C983}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1498,7 +1738,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V:V V1</xm:sqref>
+          <xm:sqref>V2:Y1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Create a worksheet with the desired levels for each power armor set, based on their stats
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Desired State" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -42,8 +43,31 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="S4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This changes drastically if Raider Overhaul is installed, becoming much stronger</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -538,7 +562,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1638,7 +1662,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5FBD3910-8737-47C7-BDE5-BFA41760AC10}</x14:id>
+          <x14:id>{F59D78B5-4E84-4352-8A6B-1F9BE1881F4D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1652,7 +1676,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C81F46B0-E3BF-41DB-9782-B3BB9163DC51}</x14:id>
+          <x14:id>{5FBF8BBC-A595-482D-A762-6015FA4C3011}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1666,7 +1690,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D4C095DC-D5B6-4414-9D90-1824E775C036}</x14:id>
+          <x14:id>{82CEC8C3-3CB6-42D1-AF33-D4D21DDC764D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1680,7 +1704,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B5C05C49-6064-40C7-BF47-3FE71816C983}</x14:id>
+          <x14:id>{A8C095E4-72C5-4AB5-A9E0-902020D2F096}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1697,7 +1721,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5FBD3910-8737-47C7-BDE5-BFA41760AC10}">
+          <x14:cfRule type="dataBar" id="{F59D78B5-4E84-4352-8A6B-1F9BE1881F4D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1708,7 +1732,7 @@
           <xm:sqref>J:J J1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C81F46B0-E3BF-41DB-9782-B3BB9163DC51}">
+          <x14:cfRule type="dataBar" id="{5FBF8BBC-A595-482D-A762-6015FA4C3011}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1719,7 +1743,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D4C095DC-D5B6-4414-9D90-1824E775C036}">
+          <x14:cfRule type="dataBar" id="{82CEC8C3-3CB6-42D1-AF33-D4D21DDC764D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1730,7 +1754,1228 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B5C05C49-6064-40C7-BF47-3FE71816C983}">
+          <x14:cfRule type="dataBar" id="{A8C095E4-72C5-4AB5-A9E0-902020D2F096}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF0000FF"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V2:Y1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="6" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <f aca="false">SUM(B3,D3,F3*2,H3*2)</f>
+        <v>380</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <f aca="false">SUM(J3,K3,M3,O3*2,Q3*2)</f>
+        <v>980</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <f aca="false">S3+T3</f>
+        <v>980</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <f aca="false">SUM(B4,D4,F4*2,H4*2)</f>
+        <v>500</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <f aca="false">SUM(J4,K4,M4,O4*2,Q4*2)</f>
+        <v>620</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <f aca="false">S4+T4</f>
+        <v>620</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <f aca="false">SUM(B5,D5,F5*2,H5*2)</f>
+        <v>500</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <f aca="false">SUM(J5,K5,M5,O5*2,Q5*2)</f>
+        <v>1100</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <f aca="false">S5+T5</f>
+        <v>1100</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <f aca="false">SUM(B6,D6,F6*2,H6*2)</f>
+        <v>740</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <f aca="false">SUM(J6,K6,M6,O6*2,Q6*2)</f>
+        <v>1340</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <f aca="false">S6+T6</f>
+        <v>1340</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <f aca="false">SUM(B7,D7,F7*2,H7*2)</f>
+        <v>740</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <f aca="false">SUM(J7,K7,M7,O7*2,Q7*2)</f>
+        <v>1340</v>
+      </c>
+      <c r="T7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1" t="n">
+        <f aca="false">S7+T7</f>
+        <v>1340</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <f aca="false">SUM(B8,D8,F8*2,H8*2)</f>
+        <v>680</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <f aca="false">SUM(J8,K8,M8,O8*2,Q8*2)</f>
+        <v>1280</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <f aca="false">(25+40)*6</f>
+        <v>390</v>
+      </c>
+      <c r="U8" s="1" t="n">
+        <f aca="false">S8+T8</f>
+        <v>1670</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>550</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <f aca="false">SUM(B9,D9,F9*2,H9*2)</f>
+        <v>880</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P9" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <f aca="false">SUM(J9,K9,M9,O9*2,Q9*2)</f>
+        <v>1380</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <f aca="false">S9+T9</f>
+        <v>1380</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>440</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <f aca="false">SUM(B10,D10,F10*2,H10*2)</f>
+        <v>980</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <f aca="false">SUM(J10,K10,M10,O10*2,Q10*2)</f>
+        <v>1580</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <f aca="false">S10+T10</f>
+        <v>1580</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">SUM(B11,D11,F11*2,H11*2)</f>
+        <v>1220</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <f aca="false">SUM(J11,K11,M11,O11*2,Q11*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <f aca="false">S11+T11</f>
+        <v>1820</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>680</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
+        <v>1460</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <f aca="false">SUM(J12,K12,M12,O12*2,Q12*2)</f>
+        <v>2060</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <f aca="false">S12+T12</f>
+        <v>2060</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
+        <v>1375</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
+        <v>1975</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <f aca="false">(80+20)*6+80</f>
+        <v>680</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <f aca="false">S13+T13</f>
+        <v>2655</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
+        <v>1860</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
+        <v>2460</v>
+      </c>
+      <c r="T14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1" t="n">
+        <f aca="false">S14+T14</f>
+        <v>2460</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J:J">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF0000FF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7CC0FA55-C010-4266-AA40-20E590CAF722}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF0000FF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{88961BDC-54A4-4B59-A56F-736A8CA6B0B8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U1048576">
+    <cfRule type="dataBar" priority="4">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF0000FF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6771D8AB-AC55-46C1-908B-E3714FA2E65D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:Y1048576">
+    <cfRule type="dataBar" priority="5">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF0000FF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D3FF6984-E94B-4BE6-AC93-7B62193FDED1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7CC0FA55-C010-4266-AA40-20E590CAF722}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF0000FF"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J:J</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{88961BDC-54A4-4B59-A56F-736A8CA6B0B8}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF0000FF"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S2:S1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6771D8AB-AC55-46C1-908B-E3714FA2E65D}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF0000FF"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U2:U1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D3FF6984-E94B-4BE6-AC93-7B62193FDED1}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Add a level 30 synth that can spawn with Institute Power Armor
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
@@ -562,12 +562,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="X10" activeCellId="0" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1244,7 +1244,7 @@
         <v>1380</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="Y9" s="0" t="n">
         <v>40</v>
@@ -1662,7 +1662,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F59D78B5-4E84-4352-8A6B-1F9BE1881F4D}</x14:id>
+          <x14:id>{ECFCB247-FA37-4ACC-A8E3-40A5841148C9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1676,7 +1676,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5FBF8BBC-A595-482D-A762-6015FA4C3011}</x14:id>
+          <x14:id>{211937D5-1230-4B00-A71F-47E1A81C7269}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1690,7 +1690,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{82CEC8C3-3CB6-42D1-AF33-D4D21DDC764D}</x14:id>
+          <x14:id>{FBEFCA4A-4058-40EB-B823-8B9257CE12D4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1704,7 +1704,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A8C095E4-72C5-4AB5-A9E0-902020D2F096}</x14:id>
+          <x14:id>{B210DBB5-8BC0-42DF-8F85-B08D6FCF1CDA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1721,7 +1721,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F59D78B5-4E84-4352-8A6B-1F9BE1881F4D}">
+          <x14:cfRule type="dataBar" id="{ECFCB247-FA37-4ACC-A8E3-40A5841148C9}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1732,7 +1732,7 @@
           <xm:sqref>J:J J1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5FBF8BBC-A595-482D-A762-6015FA4C3011}">
+          <x14:cfRule type="dataBar" id="{211937D5-1230-4B00-A71F-47E1A81C7269}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1743,7 +1743,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{82CEC8C3-3CB6-42D1-AF33-D4D21DDC764D}">
+          <x14:cfRule type="dataBar" id="{FBEFCA4A-4058-40EB-B823-8B9257CE12D4}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1754,7 +1754,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A8C095E4-72C5-4AB5-A9E0-902020D2F096}">
+          <x14:cfRule type="dataBar" id="{B210DBB5-8BC0-42DF-8F85-B08D6FCF1CDA}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1777,12 +1777,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2883,7 +2883,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7CC0FA55-C010-4266-AA40-20E590CAF722}</x14:id>
+          <x14:id>{FAE0D08E-50FA-43FE-B1A2-10E6C98A579A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2897,7 +2897,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{88961BDC-54A4-4B59-A56F-736A8CA6B0B8}</x14:id>
+          <x14:id>{388A3148-575E-4161-83AB-62B4A7D210D1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2911,7 +2911,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6771D8AB-AC55-46C1-908B-E3714FA2E65D}</x14:id>
+          <x14:id>{B05958CF-1490-4240-8D5C-418EA066836B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2925,7 +2925,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D3FF6984-E94B-4BE6-AC93-7B62193FDED1}</x14:id>
+          <x14:id>{C36DDF56-96EC-4777-B924-322E20714FE2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2942,7 +2942,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7CC0FA55-C010-4266-AA40-20E590CAF722}">
+          <x14:cfRule type="dataBar" id="{FAE0D08E-50FA-43FE-B1A2-10E6C98A579A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2953,7 +2953,7 @@
           <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{88961BDC-54A4-4B59-A56F-736A8CA6B0B8}">
+          <x14:cfRule type="dataBar" id="{388A3148-575E-4161-83AB-62B4A7D210D1}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2964,7 +2964,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6771D8AB-AC55-46C1-908B-E3714FA2E65D}">
+          <x14:cfRule type="dataBar" id="{B05958CF-1490-4240-8D5C-418EA066836B}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2975,7 +2975,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D3FF6984-E94B-4BE6-AC93-7B62193FDED1}">
+          <x14:cfRule type="dataBar" id="{C36DDF56-96EC-4777-B924-322E20714FE2}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Balance drop levels for legendary power armor
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -135,15 +135,15 @@
     <t xml:space="preserve">T-45</t>
   </si>
   <si>
+    <t xml:space="preserve">T-51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-51c</t>
+  </si>
+  <si>
     <t xml:space="preserve">X-02</t>
   </si>
   <si>
-    <t xml:space="preserve">T-51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-51c</t>
-  </si>
-  <si>
     <t xml:space="preserve">Institute</t>
   </si>
   <si>
@@ -156,10 +156,10 @@
     <t xml:space="preserve">X-03</t>
   </si>
   <si>
+    <t xml:space="preserve">Ultracite</t>
+  </si>
+  <si>
     <t xml:space="preserve">T-65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ultracite</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X10" activeCellId="0" sqref="X10"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="Y3" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,32 +952,32 @@
         <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>500</v>
+        <v>320</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>126</v>
-      </c>
       <c r="H6" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>80</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>126</v>
       </c>
       <c r="J6" s="1" t="n">
         <f aca="false">SUM(B6,D6,F6*2,H6*2)</f>
-        <v>680</v>
+        <v>740</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>100</v>
@@ -1005,21 +1005,26 @@
       </c>
       <c r="S6" s="1" t="n">
         <f aca="false">SUM(J6,K6,M6,O6*2,Q6*2)</f>
-        <v>1280</v>
+        <v>1340</v>
       </c>
       <c r="T6" s="1" t="n">
-        <f aca="false">(25+40)*6</f>
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="U6" s="1" t="n">
         <f aca="false">S6+T6</f>
-        <v>1670</v>
+        <v>1340</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="Y6" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,12 +1094,6 @@
         <f aca="false">S7+T7</f>
         <v>1340</v>
       </c>
-      <c r="V7" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="W7" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="X7" s="0" t="n">
         <v>20</v>
       </c>
@@ -1107,32 +1106,32 @@
         <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>320</v>
+        <v>500</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E8" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="G8" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="I8" s="1" t="n">
-        <v>80</v>
+        <v>126</v>
       </c>
       <c r="J8" s="1" t="n">
         <f aca="false">SUM(B8,D8,F8*2,H8*2)</f>
-        <v>740</v>
+        <v>680</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>100</v>
@@ -1160,20 +1159,21 @@
       </c>
       <c r="S8" s="1" t="n">
         <f aca="false">SUM(J8,K8,M8,O8*2,Q8*2)</f>
-        <v>1340</v>
+        <v>1280</v>
       </c>
       <c r="T8" s="1" t="n">
-        <v>0</v>
+        <f aca="false">(25+40)*6</f>
+        <v>390</v>
       </c>
       <c r="U8" s="1" t="n">
         <f aca="false">S8+T8</f>
-        <v>1340</v>
+        <v>1670</v>
       </c>
       <c r="X8" s="0" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,32 +1490,32 @@
         <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>360</v>
+        <v>500</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>680</v>
+        <v>560</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>1460</v>
+        <v>1860</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>100</v>
@@ -1543,20 +1543,20 @@
       </c>
       <c r="S13" s="1" t="n">
         <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
-        <v>2060</v>
+        <v>2460</v>
       </c>
       <c r="T13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U13" s="1" t="n">
         <f aca="false">S13+T13</f>
-        <v>2060</v>
-      </c>
-      <c r="V13" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="W13" s="0" t="n">
-        <v>40</v>
+        <v>2460</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,32 +1564,32 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>500</v>
+        <v>360</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>560</v>
+        <v>680</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>290</v>
+        <v>210</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="J14" s="1" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1860</v>
+        <v>1460</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>100</v>
@@ -1617,20 +1617,20 @@
       </c>
       <c r="S14" s="1" t="n">
         <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
-        <v>2460</v>
+        <v>2060</v>
       </c>
       <c r="T14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U14" s="1" t="n">
         <f aca="false">S14+T14</f>
-        <v>2460</v>
-      </c>
-      <c r="X14" s="0" t="n">
-        <v>77</v>
-      </c>
-      <c r="Y14" s="0" t="n">
-        <v>80</v>
+        <v>2060</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1662,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ECFCB247-FA37-4ACC-A8E3-40A5841148C9}</x14:id>
+          <x14:id>{156038B2-2042-4540-9D16-FF34FDB8F5BF}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1676,7 +1676,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{211937D5-1230-4B00-A71F-47E1A81C7269}</x14:id>
+          <x14:id>{FA18D046-18D9-4EA6-8499-2C12FA2E64EE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1690,7 +1690,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FBEFCA4A-4058-40EB-B823-8B9257CE12D4}</x14:id>
+          <x14:id>{414EB155-A5F0-4F60-A1E3-843DD4DEF765}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1704,7 +1704,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B210DBB5-8BC0-42DF-8F85-B08D6FCF1CDA}</x14:id>
+          <x14:id>{7943B4F6-9F8A-4676-97F5-9E141A24D545}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1721,7 +1721,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ECFCB247-FA37-4ACC-A8E3-40A5841148C9}">
+          <x14:cfRule type="dataBar" id="{156038B2-2042-4540-9D16-FF34FDB8F5BF}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1732,7 +1732,7 @@
           <xm:sqref>J:J J1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{211937D5-1230-4B00-A71F-47E1A81C7269}">
+          <x14:cfRule type="dataBar" id="{FA18D046-18D9-4EA6-8499-2C12FA2E64EE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1743,7 +1743,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FBEFCA4A-4058-40EB-B823-8B9257CE12D4}">
+          <x14:cfRule type="dataBar" id="{414EB155-A5F0-4F60-A1E3-843DD4DEF765}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1754,7 +1754,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B210DBB5-8BC0-42DF-8F85-B08D6FCF1CDA}">
+          <x14:cfRule type="dataBar" id="{7943B4F6-9F8A-4676-97F5-9E141A24D545}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>240</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>240</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>230</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>360</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>500</v>
@@ -2883,7 +2883,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FAE0D08E-50FA-43FE-B1A2-10E6C98A579A}</x14:id>
+          <x14:id>{6A55FDD3-B117-411A-8651-66913B99DB3E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2897,7 +2897,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{388A3148-575E-4161-83AB-62B4A7D210D1}</x14:id>
+          <x14:id>{C6A15FB2-70B5-437B-9D64-9728AF85DB2D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2911,7 +2911,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B05958CF-1490-4240-8D5C-418EA066836B}</x14:id>
+          <x14:id>{B9BFC01A-30AA-4FCA-B0E1-AFFEACA163D2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2925,7 +2925,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C36DDF56-96EC-4777-B924-322E20714FE2}</x14:id>
+          <x14:id>{595B6FB2-D037-4472-8FAC-FAD9781A9279}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2942,7 +2942,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FAE0D08E-50FA-43FE-B1A2-10E6C98A579A}">
+          <x14:cfRule type="dataBar" id="{6A55FDD3-B117-411A-8651-66913B99DB3E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2953,7 +2953,7 @@
           <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{388A3148-575E-4161-83AB-62B4A7D210D1}">
+          <x14:cfRule type="dataBar" id="{C6A15FB2-70B5-437B-9D64-9728AF85DB2D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2964,7 +2964,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B05958CF-1490-4240-8D5C-418EA066836B}">
+          <x14:cfRule type="dataBar" id="{B9BFC01A-30AA-4FCA-B0E1-AFFEACA163D2}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2975,7 +2975,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C36DDF56-96EC-4777-B924-322E20714FE2}">
+          <x14:cfRule type="dataBar" id="{595B6FB2-D037-4472-8FAC-FAD9781A9279}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Put together a power curve for Gunner power armor to determine appropriate linings
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Desired State" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Leveled Power Increase - Gunners" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -161,6 +162,33 @@
   <si>
     <t xml:space="preserve">T-65</t>
   </si>
+  <si>
+    <t xml:space="preserve">Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-51/T-51c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting Lining:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Lining:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -278,6 +306,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -502,13 +535,13 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -530,22 +563,22 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -555,6 +588,990 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$B$1:$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$C$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-51/T-51c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$D$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-02</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$E$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$F$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$G$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-65</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$H$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="314004"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="75406654"/>
+        <c:axId val="45141557"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="75406654"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45141557"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45141557"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75406654"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>468720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>518760</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="468720" y="2243160"/>
+        <a:ext cx="7605000" cy="4277520"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -562,12 +1579,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1653,7 +2670,7 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J:J J1">
+  <conditionalFormatting sqref="J:J">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -1662,7 +2679,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{156038B2-2042-4540-9D16-FF34FDB8F5BF}</x14:id>
+          <x14:id>{D22BA549-D56C-4D82-BBA6-FB5FC0AFA01C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1676,7 +2693,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FA18D046-18D9-4EA6-8499-2C12FA2E64EE}</x14:id>
+          <x14:id>{DB5ACF91-6AB4-45B6-90D3-1752FF57908B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1690,7 +2707,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{414EB155-A5F0-4F60-A1E3-843DD4DEF765}</x14:id>
+          <x14:id>{FEE890F1-F1E6-469A-BBB5-BA34B9F59A97}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1704,7 +2721,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7943B4F6-9F8A-4676-97F5-9E141A24D545}</x14:id>
+          <x14:id>{D0E1B147-6264-439C-B593-5217E68F5044}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1721,7 +2738,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{156038B2-2042-4540-9D16-FF34FDB8F5BF}">
+          <x14:cfRule type="dataBar" id="{D22BA549-D56C-4D82-BBA6-FB5FC0AFA01C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1729,10 +2746,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J:J J1</xm:sqref>
+          <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FA18D046-18D9-4EA6-8499-2C12FA2E64EE}">
+          <x14:cfRule type="dataBar" id="{DB5ACF91-6AB4-45B6-90D3-1752FF57908B}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1743,7 +2760,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{414EB155-A5F0-4F60-A1E3-843DD4DEF765}">
+          <x14:cfRule type="dataBar" id="{FEE890F1-F1E6-469A-BBB5-BA34B9F59A97}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1754,7 +2771,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7943B4F6-9F8A-4676-97F5-9E141A24D545}">
+          <x14:cfRule type="dataBar" id="{D0E1B147-6264-439C-B593-5217E68F5044}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1782,7 +2799,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U8" activeCellId="0" sqref="U8"/>
+      <selection pane="bottomRight" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2883,7 +3900,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6A55FDD3-B117-411A-8651-66913B99DB3E}</x14:id>
+          <x14:id>{F2BF52B0-8EB9-42C7-98FF-48371AEB162C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2897,7 +3914,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C6A15FB2-70B5-437B-9D64-9728AF85DB2D}</x14:id>
+          <x14:id>{A6526B84-C0D8-419D-8175-30E77F5AF7A6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2911,7 +3928,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B9BFC01A-30AA-4FCA-B0E1-AFFEACA163D2}</x14:id>
+          <x14:id>{1D7C5C1E-F76E-4FF5-902D-2E89EE97B068}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2925,7 +3942,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{595B6FB2-D037-4472-8FAC-FAD9781A9279}</x14:id>
+          <x14:id>{DDE3AB30-8372-463C-A29A-5533D4DBE386}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2942,7 +3959,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6A55FDD3-B117-411A-8651-66913B99DB3E}">
+          <x14:cfRule type="dataBar" id="{F2BF52B0-8EB9-42C7-98FF-48371AEB162C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2953,7 +3970,7 @@
           <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C6A15FB2-70B5-437B-9D64-9728AF85DB2D}">
+          <x14:cfRule type="dataBar" id="{A6526B84-C0D8-419D-8175-30E77F5AF7A6}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2964,7 +3981,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B9BFC01A-30AA-4FCA-B0E1-AFFEACA163D2}">
+          <x14:cfRule type="dataBar" id="{1D7C5C1E-F76E-4FF5-902D-2E89EE97B068}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2975,7 +3992,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{595B6FB2-D037-4472-8FAC-FAD9781A9279}">
+          <x14:cfRule type="dataBar" id="{DDE3AB30-8372-463C-A29A-5533D4DBE386}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2989,4 +4006,218 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>860</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1040</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1160</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1220</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1460</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1460</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust the level at which X-02, X-03, and Ultracite power armor appear on enemies
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
@@ -588,7 +588,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart120.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1410,11 +1410,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="75406654"/>
-        <c:axId val="45141557"/>
+        <c:axId val="80248858"/>
+        <c:axId val="56886868"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75406654"/>
+        <c:axId val="80248858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,14 +1449,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45141557"/>
+        <c:crossAx val="56886868"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45141557"/>
+        <c:axId val="56886868"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1500,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75406654"/>
+        <c:crossAx val="80248858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1579,12 +1579,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2187,7 +2187,7 @@
         <v>1670</v>
       </c>
       <c r="X8" s="0" t="n">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="Y8" s="0" t="n">
         <v>40</v>
@@ -2496,7 +2496,7 @@
         <v>2655</v>
       </c>
       <c r="X12" s="0" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="Y12" s="0" t="n">
         <v>70</v>
@@ -2570,7 +2570,7 @@
         <v>2460</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>70</v>
@@ -2679,7 +2679,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D22BA549-D56C-4D82-BBA6-FB5FC0AFA01C}</x14:id>
+          <x14:id>{FE544282-A397-4266-B8E2-3D10D075AC5D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2693,7 +2693,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DB5ACF91-6AB4-45B6-90D3-1752FF57908B}</x14:id>
+          <x14:id>{701AED3C-A14C-4A54-A1A3-47444BC9B1B2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2707,7 +2707,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FEE890F1-F1E6-469A-BBB5-BA34B9F59A97}</x14:id>
+          <x14:id>{FFB1D8DD-29CA-4E2B-8624-1546799B9CF8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2721,7 +2721,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D0E1B147-6264-439C-B593-5217E68F5044}</x14:id>
+          <x14:id>{52D657F4-813D-4168-A8C3-8821AC30452F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2738,7 +2738,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D22BA549-D56C-4D82-BBA6-FB5FC0AFA01C}">
+          <x14:cfRule type="dataBar" id="{FE544282-A397-4266-B8E2-3D10D075AC5D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2749,7 +2749,7 @@
           <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DB5ACF91-6AB4-45B6-90D3-1752FF57908B}">
+          <x14:cfRule type="dataBar" id="{701AED3C-A14C-4A54-A1A3-47444BC9B1B2}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2760,7 +2760,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FEE890F1-F1E6-469A-BBB5-BA34B9F59A97}">
+          <x14:cfRule type="dataBar" id="{FFB1D8DD-29CA-4E2B-8624-1546799B9CF8}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2771,7 +2771,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D0E1B147-6264-439C-B593-5217E68F5044}">
+          <x14:cfRule type="dataBar" id="{52D657F4-813D-4168-A8C3-8821AC30452F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3900,7 +3900,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F2BF52B0-8EB9-42C7-98FF-48371AEB162C}</x14:id>
+          <x14:id>{38995CD3-C46B-4D47-9F2D-C8351044274B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3914,7 +3914,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A6526B84-C0D8-419D-8175-30E77F5AF7A6}</x14:id>
+          <x14:id>{6DF1872C-4728-4232-883A-BAF41F97AB4E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3928,7 +3928,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1D7C5C1E-F76E-4FF5-902D-2E89EE97B068}</x14:id>
+          <x14:id>{7FA2F495-DFBB-49B0-857C-E43FE313C72D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3942,7 +3942,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DDE3AB30-8372-463C-A29A-5533D4DBE386}</x14:id>
+          <x14:id>{92648FF8-1620-4520-9CF0-C5CD1770128A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3959,7 +3959,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F2BF52B0-8EB9-42C7-98FF-48371AEB162C}">
+          <x14:cfRule type="dataBar" id="{38995CD3-C46B-4D47-9F2D-C8351044274B}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3970,7 +3970,7 @@
           <xm:sqref>J:J</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A6526B84-C0D8-419D-8175-30E77F5AF7A6}">
+          <x14:cfRule type="dataBar" id="{6DF1872C-4728-4232-883A-BAF41F97AB4E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3981,7 +3981,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1D7C5C1E-F76E-4FF5-902D-2E89EE97B068}">
+          <x14:cfRule type="dataBar" id="{7FA2F495-DFBB-49B0-857C-E43FE313C72D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3992,7 +3992,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DDE3AB30-8372-463C-A29A-5533D4DBE386}">
+          <x14:cfRule type="dataBar" id="{92648FF8-1620-4520-9CF0-C5CD1770128A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4015,7 +4015,7 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update balancing data current state and remove desired state, since it has been achieved
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -8,9 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Current State" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Desired State" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Leveled Power Increase - Gunners" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Leveled Power Increase - Gunners" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -44,31 +43,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="S4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">This changes drastically if Raider Overhaul is installed, becoming much stronger</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -154,13 +130,13 @@
     <t xml:space="preserve">X-01</t>
   </si>
   <si>
+    <t xml:space="preserve">T-65</t>
+  </si>
+  <si>
     <t xml:space="preserve">X-03</t>
   </si>
   <si>
     <t xml:space="preserve">Ultracite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-65</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -197,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,6 +282,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -588,7 +570,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart120.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -632,6 +614,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -747,6 +730,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -862,6 +846,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -977,6 +962,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1092,6 +1078,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1207,6 +1194,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1322,6 +1310,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1410,11 +1399,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="80248858"/>
-        <c:axId val="56886868"/>
+        <c:axId val="57150747"/>
+        <c:axId val="88862748"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80248858"/>
+        <c:axId val="57150747"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,14 +1438,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56886868"/>
+        <c:crossAx val="88862748"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56886868"/>
+        <c:axId val="88862748"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1460,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1500,7 +1489,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80248858"/>
+        <c:crossAx val="57150747"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1548,9 +1537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518760</xdr:colOff>
+      <xdr:colOff>518400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1559,7 +1548,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7605000" cy="4277520"/>
+        <a:ext cx="7604640" cy="4277160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2432,32 +2421,32 @@
         <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>600</v>
+        <v>680</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>170</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>170</v>
       </c>
       <c r="J12" s="1" t="n">
         <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>1375</v>
+        <v>1460</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>100</v>
@@ -2485,21 +2474,26 @@
       </c>
       <c r="S12" s="1" t="n">
         <f aca="false">SUM(J12,K12,M12,O12*2,Q12*2)</f>
-        <v>1975</v>
+        <v>2060</v>
       </c>
       <c r="T12" s="1" t="n">
-        <f aca="false">(80+20)*6+80</f>
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="U12" s="1" t="n">
         <f aca="false">S12+T12</f>
-        <v>2655</v>
+        <v>2060</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>40</v>
       </c>
       <c r="X12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="Y12" s="0" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,32 +2501,32 @@
         <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>300</v>
+        <v>235</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>1860</v>
+        <v>1375</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>100</v>
@@ -2560,17 +2554,18 @@
       </c>
       <c r="S13" s="1" t="n">
         <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
-        <v>2460</v>
+        <v>1975</v>
       </c>
       <c r="T13" s="1" t="n">
-        <v>0</v>
+        <f aca="false">(80+20)*6+80</f>
+        <v>680</v>
       </c>
       <c r="U13" s="1" t="n">
         <f aca="false">S13+T13</f>
-        <v>2460</v>
+        <v>2655</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>70</v>
@@ -2581,32 +2576,32 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>360</v>
+        <v>500</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>680</v>
+        <v>560</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="J14" s="1" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1460</v>
+        <v>1860</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>100</v>
@@ -2634,20 +2629,20 @@
       </c>
       <c r="S14" s="1" t="n">
         <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
-        <v>2060</v>
+        <v>2460</v>
       </c>
       <c r="T14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U14" s="1" t="n">
         <f aca="false">S14+T14</f>
-        <v>2060</v>
-      </c>
-      <c r="V14" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="W14" s="0" t="n">
-        <v>40</v>
+        <v>2460</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2670,7 +2665,7 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J:J">
+  <conditionalFormatting sqref="S2:S1048576">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -2679,12 +2674,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FE544282-A397-4266-B8E2-3D10D075AC5D}</x14:id>
+          <x14:id>{E1B53946-72B9-4065-B500-3630A6A1B4D0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S1048576">
+  <conditionalFormatting sqref="U2:U1048576">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -2693,12 +2688,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{701AED3C-A14C-4A54-A1A3-47444BC9B1B2}</x14:id>
+          <x14:id>{8CBE1469-2ACD-442F-83EE-3B7611356613}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U1048576">
+  <conditionalFormatting sqref="V2:Y1048576">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -2707,21 +2702,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FFB1D8DD-29CA-4E2B-8624-1546799B9CF8}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:Y1048576">
-    <cfRule type="dataBar" priority="5">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52D657F4-813D-4168-A8C3-8821AC30452F}</x14:id>
+          <x14:id>{B7896AE9-9BC9-4B97-84DF-419C501AA09A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2738,18 +2719,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FE544282-A397-4266-B8E2-3D10D075AC5D}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FF0000FF"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>J:J</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{701AED3C-A14C-4A54-A1A3-47444BC9B1B2}">
+          <x14:cfRule type="dataBar" id="{E1B53946-72B9-4065-B500-3630A6A1B4D0}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2760,7 +2730,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FFB1D8DD-29CA-4E2B-8624-1546799B9CF8}">
+          <x14:cfRule type="dataBar" id="{8CBE1469-2ACD-442F-83EE-3B7611356613}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2771,7 +2741,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{52D657F4-813D-4168-A8C3-8821AC30452F}">
+          <x14:cfRule type="dataBar" id="{B7896AE9-9BC9-4B97-84DF-419C501AA09A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2792,1231 +2762,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B11" activeCellId="0" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="6" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <f aca="false">SUM(B3,D3,F3*2,H3*2)</f>
-        <v>380</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <f aca="false">SUM(J3,K3,M3,O3*2,Q3*2)</f>
-        <v>980</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <f aca="false">S3+T3</f>
-        <v>980</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <f aca="false">SUM(B4,D4,F4*2,H4*2)</f>
-        <v>500</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="N4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <f aca="false">SUM(J4,K4,M4,O4*2,Q4*2)</f>
-        <v>620</v>
-      </c>
-      <c r="T4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1" t="n">
-        <f aca="false">S4+T4</f>
-        <v>620</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <f aca="false">SUM(B5,D5,F5*2,H5*2)</f>
-        <v>500</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N5" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P5" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S5" s="1" t="n">
-        <f aca="false">SUM(J5,K5,M5,O5*2,Q5*2)</f>
-        <v>1100</v>
-      </c>
-      <c r="T5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1" t="n">
-        <f aca="false">S5+T5</f>
-        <v>1100</v>
-      </c>
-      <c r="V5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X5" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y5" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>240</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>320</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <f aca="false">SUM(B6,D6,F6*2,H6*2)</f>
-        <v>740</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S6" s="1" t="n">
-        <f aca="false">SUM(J6,K6,M6,O6*2,Q6*2)</f>
-        <v>1340</v>
-      </c>
-      <c r="T6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1" t="n">
-        <f aca="false">S6+T6</f>
-        <v>1340</v>
-      </c>
-      <c r="V6" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="W6" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="X6" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>240</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>320</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <f aca="false">SUM(B7,D7,F7*2,H7*2)</f>
-        <v>740</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R7" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S7" s="1" t="n">
-        <f aca="false">SUM(J7,K7,M7,O7*2,Q7*2)</f>
-        <v>1340</v>
-      </c>
-      <c r="T7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1" t="n">
-        <f aca="false">S7+T7</f>
-        <v>1340</v>
-      </c>
-      <c r="X7" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="Y7" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>230</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <f aca="false">SUM(B8,D8,F8*2,H8*2)</f>
-        <v>680</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P8" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R8" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S8" s="1" t="n">
-        <f aca="false">SUM(J8,K8,M8,O8*2,Q8*2)</f>
-        <v>1280</v>
-      </c>
-      <c r="T8" s="1" t="n">
-        <f aca="false">(25+40)*6</f>
-        <v>390</v>
-      </c>
-      <c r="U8" s="1" t="n">
-        <f aca="false">S8+T8</f>
-        <v>1670</v>
-      </c>
-      <c r="X8" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y8" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>550</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <f aca="false">SUM(B9,D9,F9*2,H9*2)</f>
-        <v>880</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P9" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R9" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <f aca="false">SUM(J9,K9,M9,O9*2,Q9*2)</f>
-        <v>1380</v>
-      </c>
-      <c r="T9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="1" t="n">
-        <f aca="false">S9+T9</f>
-        <v>1380</v>
-      </c>
-      <c r="X9" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y9" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>280</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>440</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>180</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <f aca="false">SUM(B10,D10,F10*2,H10*2)</f>
-        <v>980</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L10" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P10" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R10" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S10" s="1" t="n">
-        <f aca="false">SUM(J10,K10,M10,O10*2,Q10*2)</f>
-        <v>1580</v>
-      </c>
-      <c r="T10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="1" t="n">
-        <f aca="false">S10+T10</f>
-        <v>1580</v>
-      </c>
-      <c r="V10" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="W10" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="X10" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>320</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>560</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>220</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <f aca="false">SUM(B11,D11,F11*2,H11*2)</f>
-        <v>1220</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L11" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N11" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P11" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R11" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S11" s="1" t="n">
-        <f aca="false">SUM(J11,K11,M11,O11*2,Q11*2)</f>
-        <v>1820</v>
-      </c>
-      <c r="T11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" s="1" t="n">
-        <f aca="false">S11+T11</f>
-        <v>1820</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="W11" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="X11" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>680</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>260</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>1460</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N12" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P12" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R12" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S12" s="1" t="n">
-        <f aca="false">SUM(J12,K12,M12,O12*2,Q12*2)</f>
-        <v>2060</v>
-      </c>
-      <c r="T12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" s="1" t="n">
-        <f aca="false">S12+T12</f>
-        <v>2060</v>
-      </c>
-      <c r="V12" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="W12" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="X12" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Y12" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>380</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>600</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>235</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>190</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>190</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>1375</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N13" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P13" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R13" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
-        <v>1975</v>
-      </c>
-      <c r="T13" s="1" t="n">
-        <f aca="false">(80+20)*6+80</f>
-        <v>680</v>
-      </c>
-      <c r="U13" s="1" t="n">
-        <f aca="false">S13+T13</f>
-        <v>2655</v>
-      </c>
-      <c r="X13" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Y13" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>560</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>290</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>240</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1860</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="L14" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="N14" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="P14" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R14" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="S14" s="1" t="n">
-        <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
-        <v>2460</v>
-      </c>
-      <c r="T14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" s="1" t="n">
-        <f aca="false">S14+T14</f>
-        <v>2460</v>
-      </c>
-      <c r="X14" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Y14" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="J:J">
-    <cfRule type="dataBar" priority="2">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{38995CD3-C46B-4D47-9F2D-C8351044274B}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S1048576">
-    <cfRule type="dataBar" priority="3">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6DF1872C-4728-4232-883A-BAF41F97AB4E}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U1048576">
-    <cfRule type="dataBar" priority="4">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7FA2F495-DFBB-49B0-857C-E43FE313C72D}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:Y1048576">
-    <cfRule type="dataBar" priority="5">
-      <dataBar showValue="1" minLength="0" maxLength="100">
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{92648FF8-1620-4520-9CF0-C5CD1770128A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{38995CD3-C46B-4D47-9F2D-C8351044274B}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FF0000FF"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>J:J</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6DF1872C-4728-4232-883A-BAF41F97AB4E}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FF0000FF"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>S2:S1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7FA2F495-DFBB-49B0-857C-E43FE313C72D}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FF0000FF"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>U2:U1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{92648FF8-1620-4520-9CF0-C5CD1770128A}">
-            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FF0000FF"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>V2:Y1048576</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4045,10 +2794,10 @@
         <v>27</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add armor scaling data for all factions covered by Power Armored Enemies
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -9,7 +9,10 @@
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Leveled Power Increase - Gunners" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Leveled Power Increase - Raiders" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Leveled Power Increase - Gunners" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Leveled Power Increase - Institute" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Global Leveled Power Increase" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -142,16 +145,25 @@
     <t xml:space="preserve">Level</t>
   </si>
   <si>
-    <t xml:space="preserve">T-51/T-51c</t>
+    <t xml:space="preserve">Maximum Possible</t>
   </si>
   <si>
     <t xml:space="preserve">Starting Lining:</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Lining:</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-51/T-51c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -160,10 +172,19 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Lining:</t>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
+    <t xml:space="preserve">I-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raiders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gunners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brotherhood of Steel</t>
   </si>
 </sst>
 </file>
@@ -173,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -291,6 +312,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -570,7 +596,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -584,11 +610,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$B$1:$B$1</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T-45</c:v>
+                  <c:v>Excavator</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -624,53 +650,50 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>740</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>860</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>980</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -685,9 +708,6 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -700,11 +720,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$C$1:$C$1</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T-51/T-51c</c:v>
+                  <c:v>Raider</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -740,56 +760,53 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>860</c:v>
+                  <c:v>620</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>980</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1100</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1220</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v/>
@@ -801,9 +818,6 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -816,11 +830,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$D$1:$D$1</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-02</c:v>
+                  <c:v>T-45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -856,56 +870,53 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1040</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1160</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1280</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v/>
@@ -917,9 +928,6 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -932,11 +940,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$E$1:$E$1</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T-60</c:v>
+                  <c:v>T-51</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -972,59 +980,56 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1220</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1340</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1460</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1033,9 +1038,6 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1048,11 +1050,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$F$1:$F$1</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-01</c:v>
+                  <c:v>T-60</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1088,45 +1090,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$10</c:f>
+              <c:f>'Leveled Power Increase - Raiders'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1134,256 +1133,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1340</c:v>
+                  <c:v>980</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1460</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1580</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1700</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$G$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>T-65</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="83caff"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1580</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1820</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1940</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$H$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>X-03</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="314004"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1855</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1975</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1399,11 +1163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="57150747"/>
-        <c:axId val="88862748"/>
+        <c:axId val="33934406"/>
+        <c:axId val="76725510"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57150747"/>
+        <c:axId val="33934406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,14 +1202,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88862748"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="76725510"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88862748"/>
+        <c:axId val="76725510"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1253,2112 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57150747"/>
+        <c:crossAx val="33934406"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$B$1:$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$C$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-51/T-51c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$D$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-02</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$E$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$F$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$G$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-65</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$H$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="314004"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Starting Lining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="59075535"/>
+        <c:axId val="38413384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="59075535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38413384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38413384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59075535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Institute'!$B$1:$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>I-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Institute'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Institute'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="54323086"/>
+        <c:axId val="68272876"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="54323086"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68272876"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68272876"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54323086"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raiders</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global Leveled Power Increase'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>980</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gunners</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global Leveled Power Increase'!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Institute</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global Leveled Power Increase'!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1380</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brotherhood of Steel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global Leveled Power Increase'!$E$2:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="81772456"/>
+        <c:axId val="12991733"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="81772456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12991733"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="12991733"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Armor Rating</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81772456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1537,7 +3406,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518760</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
@@ -1548,7 +3417,112 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
+        <a:ext cx="7605000" cy="4277160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>468720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>518760</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="468720" y="2243160"/>
+        <a:ext cx="7605000" cy="4277160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>468720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>518400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="468720" y="2243160"/>
         <a:ext cx="7604640" cy="4277160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>270000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>61200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="270000" y="3157200"/>
+        <a:ext cx="8383320" cy="4715280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2674,7 +4648,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E1B53946-72B9-4065-B500-3630A6A1B4D0}</x14:id>
+          <x14:id>{B5DBEEFC-4E6D-40FE-8382-609C4F2F9A79}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2688,7 +4662,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8CBE1469-2ACD-442F-83EE-3B7611356613}</x14:id>
+          <x14:id>{2ED4E9CE-5E38-4893-B8E3-C1CD6D716648}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2702,7 +4676,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B7896AE9-9BC9-4B97-84DF-419C501AA09A}</x14:id>
+          <x14:id>{3092DC25-877F-4C7D-958E-1B9D2C4E5555}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2719,7 +4693,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E1B53946-72B9-4065-B500-3630A6A1B4D0}">
+          <x14:cfRule type="dataBar" id="{B5DBEEFC-4E6D-40FE-8382-609C4F2F9A79}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2730,7 +4704,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8CBE1469-2ACD-442F-83EE-3B7611356613}">
+          <x14:cfRule type="dataBar" id="{2ED4E9CE-5E38-4893-B8E3-C1CD6D716648}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2741,7 +4715,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B7896AE9-9BC9-4B97-84DF-419C501AA09A}">
+          <x14:cfRule type="dataBar" id="{3092DC25-877F-4C7D-958E-1B9D2C4E5555}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2762,16 +4736,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,10 +4755,158 @@
         <v>31</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>620</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">MAX(B2:I2)</f>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">MAX(B3:I3, J2)</f>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">MAX(B4:I4, J3)</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>24</v>
@@ -2798,6 +4922,9 @@
       </c>
       <c r="H1" s="0" t="s">
         <v>29</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2810,6 +4937,10 @@
       <c r="C2" s="0" t="n">
         <v>860</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">MAX(B2:I2)</f>
+        <v>860</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -2827,6 +4958,10 @@
       <c r="E3" s="0" t="n">
         <v>1100</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">MAX(B3:I3, J2)</f>
+        <v>1100</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2847,6 +4982,10 @@
       <c r="F4" s="0" t="n">
         <v>1340</v>
       </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">MAX(B4:I4, J3)</f>
+        <v>1340</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -2867,6 +5006,10 @@
       <c r="G5" s="0" t="n">
         <v>1580</v>
       </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">MAX(B5:I5, J4)</f>
+        <v>1580</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2884,6 +5027,10 @@
       <c r="H6" s="0" t="n">
         <v>1855</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">MAX(B6:I6, J5)</f>
+        <v>1855</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2898,6 +5045,10 @@
       <c r="H7" s="0" t="n">
         <v>1975</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">MAX(B7:I7, J6)</f>
+        <v>1975</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2906,57 +5057,540 @@
       <c r="G8" s="0" t="n">
         <v>1940</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">MAX(B8:I8, J7)</f>
+        <v>1975</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">MAX(B2:I2)</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">MAX(B3:I3, J2)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1180</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">MAX(B4:I4, J3)</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">MAX(B5:I5, J4)</f>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1380</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">MAX(B6:I6, J5)</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">VLOOKUP($A2, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>740</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>740</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1100</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1100</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1340</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1340</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1580</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1580</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1855</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1855</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Raiders'!$A$2:$J$9, 10, 1)</f>
+        <v>980</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <v>1975</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
+        <v>1380</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add X-02 Tesla as an option for legendary Gunners and Enclave members
* Increase X-01 Tesla lining to E and level to 65 to make room for X-02 Tesla
* Move PA_Tesla instantiation filter keyword in Power Armored Enemies Extended
* Add a Some Assembly Required patch for X-02, since the armor records were modified to add the Tesla combination
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -170,6 +170,48 @@
   </si>
   <si>
     <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">F + </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tesla</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E + </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tesla</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">F</t>
@@ -596,7 +638,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1163,11 +1205,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="33934406"/>
-        <c:axId val="76725510"/>
+        <c:axId val="4251438"/>
+        <c:axId val="98374601"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="33934406"/>
+        <c:axId val="4251438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,14 +1244,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76725510"/>
+        <c:crossAx val="98374601"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76725510"/>
+        <c:axId val="98374601"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1295,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33934406"/>
+        <c:crossAx val="4251438"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1290,7 +1332,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1304,7 +1346,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$B$1:$B$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1344,9 +1386,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1360,29 +1402,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>740</c:v>
                 </c:pt>
@@ -1408,6 +1453,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1420,7 +1468,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$C$1:$C$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1460,9 +1508,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1476,29 +1524,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>860</c:v>
                 </c:pt>
@@ -1524,6 +1575,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1536,7 +1590,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$D$1:$D$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1576,9 +1630,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1592,29 +1646,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1628,7 +1685,7 @@
                   <c:v>1280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1520</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1640,6 +1697,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1652,7 +1712,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$E$1:$E$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1692,9 +1752,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1708,29 +1768,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1744,11 +1807,11 @@
                   <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1460</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v/>
                 </c:pt>
@@ -1756,6 +1819,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1768,7 +1834,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$F$1:$F$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1808,9 +1874,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1824,29 +1890,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1860,18 +1929,21 @@
                   <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1700</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1884,7 +1956,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$G$1:$G$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1924,9 +1996,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1940,29 +2012,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1976,18 +2051,21 @@
                   <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1700</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1820</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1940</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2000,7 +2078,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$H$1:$H$1</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2040,9 +2118,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -2056,29 +2134,32 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Starting Lining:</c:v>
+                <c:pt idx="9">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$10</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2092,18 +2173,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1855</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2119,11 +2203,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="59075535"/>
-        <c:axId val="38413384"/>
+        <c:axId val="64669054"/>
+        <c:axId val="35794489"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59075535"/>
+        <c:axId val="64669054"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,14 +2242,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38413384"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="35794489"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38413384"/>
+        <c:axId val="35794489"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2293,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59075535"/>
+        <c:crossAx val="64669054"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2246,7 +2330,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2372,11 +2456,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="54323086"/>
-        <c:axId val="68272876"/>
+        <c:axId val="89207225"/>
+        <c:axId val="63226057"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54323086"/>
+        <c:axId val="89207225"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2411,14 +2495,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68272876"/>
+        <c:crossAx val="63226057"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68272876"/>
+        <c:axId val="63226057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2462,7 +2546,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54323086"/>
+        <c:crossAx val="89207225"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2499,7 +2583,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3192,11 +3276,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="81772456"/>
-        <c:axId val="12991733"/>
+        <c:axId val="84476072"/>
+        <c:axId val="41974276"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81772456"/>
+        <c:axId val="84476072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,14 +3353,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12991733"/>
+        <c:crossAx val="41974276"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12991733"/>
+        <c:axId val="41974276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3442,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81772456"/>
+        <c:crossAx val="84476072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3436,14 +3520,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>468720</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>518760</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3451,7 +3535,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="468720" y="2243160"/>
+        <a:off x="468720" y="2568240"/>
         <a:ext cx="7605000" cy="4277160"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4648,7 +4732,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B5DBEEFC-4E6D-40FE-8382-609C4F2F9A79}</x14:id>
+          <x14:id>{9EE573E7-5A54-4196-88D9-354AE89F97BF}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4662,7 +4746,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2ED4E9CE-5E38-4893-B8E3-C1CD6D716648}</x14:id>
+          <x14:id>{4F5170B0-19FE-44F2-A8B0-914FB535D073}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4676,7 +4760,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3092DC25-877F-4C7D-958E-1B9D2C4E5555}</x14:id>
+          <x14:id>{C763D677-C360-40E2-9CE8-4D66711F5F3C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4693,7 +4777,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B5DBEEFC-4E6D-40FE-8382-609C4F2F9A79}">
+          <x14:cfRule type="dataBar" id="{9EE573E7-5A54-4196-88D9-354AE89F97BF}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4704,7 +4788,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2ED4E9CE-5E38-4893-B8E3-C1CD6D716648}">
+          <x14:cfRule type="dataBar" id="{4F5170B0-19FE-44F2-A8B0-914FB535D073}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4715,7 +4799,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3092DC25-877F-4C7D-958E-1B9D2C4E5555}">
+          <x14:cfRule type="dataBar" id="{C763D677-C360-40E2-9CE8-4D66711F5F3C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4884,10 +4968,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5013,105 +5097,144 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1520</v>
       </c>
       <c r="E6" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>1460</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>1580</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1700</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>1855</v>
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">MAX(B6:I6, J5)</f>
-        <v>1855</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1460</v>
       </c>
       <c r="F7" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>1700</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>1820</v>
-      </c>
       <c r="H7" s="0" t="n">
-        <v>1975</v>
+        <v>1855</v>
       </c>
       <c r="J7" s="0" t="n">
-        <f aca="false">MAX(B7:I7, J6)</f>
-        <v>1975</v>
+        <f aca="false">MAX(B7:I7, J5)</f>
+        <v>1855</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>1700</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1855</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">MAX(B8:I8, J6)</f>
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1975</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">MAX(B9:I9, J7)</f>
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>1940</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">MAX(B8:I8, J7)</f>
+      <c r="J10" s="0" t="n">
+        <f aca="false">MAX(B10:I10, J9)</f>
         <v>1975</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B13" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>41</v>
+      <c r="H13" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5150,7 +5273,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>32</v>
@@ -5229,7 +5352,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5267,16 +5390,16 @@
         <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5297,7 +5420,7 @@
         <v>740</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>860</v>
       </c>
     </row>
@@ -5310,7 +5433,7 @@
         <v>740</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>860</v>
       </c>
     </row>
@@ -5323,7 +5446,7 @@
         <v>980</v>
       </c>
       <c r="C5" s="0" t="n">
-        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1100</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -5340,7 +5463,7 @@
         <v>980</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1100</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -5357,7 +5480,7 @@
         <v>980</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1340</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -5374,7 +5497,7 @@
         <v>980</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1340</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -5391,7 +5514,7 @@
         <v>980</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1580</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -5408,7 +5531,7 @@
         <v>980</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1580</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -5425,7 +5548,7 @@
         <v>980</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1855</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -5442,7 +5565,7 @@
         <v>980</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1855</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -5462,7 +5585,7 @@
         <v>980</v>
       </c>
       <c r="C13" s="0" t="n">
-        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -5482,7 +5605,7 @@
         <v>980</v>
       </c>
       <c r="C14" s="0" t="n">
-        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -5502,7 +5625,7 @@
         <v>980</v>
       </c>
       <c r="C15" s="0" t="n">
-        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -5522,7 +5645,7 @@
         <v>980</v>
       </c>
       <c r="C16" s="0" t="n">
-        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -5542,7 +5665,7 @@
         <v>980</v>
       </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -5562,7 +5685,7 @@
         <v>980</v>
       </c>
       <c r="C18" s="0" t="n">
-        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -5582,7 +5705,7 @@
         <v>980</v>
       </c>
       <c r="C19" s="0" t="n">
-        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$9, 10, 1)</f>
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
         <v>1975</v>
       </c>
       <c r="D19" s="0" t="n">

</xml_diff>

<commit_message>
Add Classic Advanced Power Armor to the stat sheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">X-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Advanced</t>
   </si>
   <si>
     <t xml:space="preserve">Ultracite</t>
@@ -359,6 +362,7 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -517,7 +521,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,6 +551,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,7 +627,7 @@
       <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFAECF00"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
@@ -638,7 +646,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1205,11 +1213,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="4251438"/>
-        <c:axId val="98374601"/>
+        <c:axId val="79687069"/>
+        <c:axId val="35058567"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4251438"/>
+        <c:axId val="79687069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,14 +1252,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98374601"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="35058567"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98374601"/>
+        <c:axId val="35058567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,7 +1303,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4251438"/>
+        <c:crossAx val="79687069"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,7 +1340,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1386,9 +1394,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1414,9 +1422,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1424,10 +1447,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>740</c:v>
                 </c:pt>
@@ -1456,6 +1479,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1508,9 +1546,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1536,9 +1574,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1546,10 +1599,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>860</c:v>
                 </c:pt>
@@ -1578,6 +1631,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1630,9 +1698,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1658,9 +1726,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1668,10 +1751,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1700,6 +1783,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1752,9 +1850,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1780,9 +1878,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1790,10 +1903,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1822,6 +1935,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1874,9 +2002,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1902,9 +2030,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1912,10 +2055,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1944,6 +2087,21 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1996,9 +2154,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -2024,9 +2182,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2034,10 +2207,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2063,9 +2236,24 @@
                   <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1940</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2118,9 +2306,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -2146,9 +2334,24 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2156,10 +2359,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$11</c:f>
+              <c:f>'Leveled Power Increase - Gunners'!$H$2:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2188,6 +2391,172 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Classic Advanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="aecf00"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2203,11 +2572,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="64669054"/>
-        <c:axId val="35794489"/>
+        <c:axId val="69959549"/>
+        <c:axId val="92443669"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64669054"/>
+        <c:axId val="69959549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,14 +2611,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35794489"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="92443669"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35794489"/>
+        <c:axId val="92443669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,7 +2662,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64669054"/>
+        <c:crossAx val="69959549"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2330,7 +2699,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2374,6 +2743,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2456,11 +2826,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="89207225"/>
-        <c:axId val="63226057"/>
+        <c:axId val="43412870"/>
+        <c:axId val="3371375"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89207225"/>
+        <c:axId val="43412870"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,14 +2865,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63226057"/>
+        <c:crossAx val="3371375"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63226057"/>
+        <c:axId val="3371375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,7 +2916,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89207225"/>
+        <c:crossAx val="43412870"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2583,7 +2953,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2627,6 +2997,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2796,6 +3167,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2902,28 +3274,28 @@
                   <c:v>1855</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1855</c:v>
+                  <c:v>1980</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1975</c:v>
+                  <c:v>1980</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1975</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1975</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1975</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1975</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1975</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1975</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2965,6 +3337,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3134,6 +3507,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3276,11 +3650,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84476072"/>
-        <c:axId val="41974276"/>
+        <c:axId val="12276346"/>
+        <c:axId val="30052810"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84476072"/>
+        <c:axId val="12276346"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3353,14 +3727,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41974276"/>
+        <c:crossAx val="30052810"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41974276"/>
+        <c:axId val="30052810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,7 +3787,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3442,7 +3816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84476072"/>
+        <c:crossAx val="12276346"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3490,9 +3864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518760</xdr:colOff>
+      <xdr:colOff>518400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3501,7 +3875,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7605000" cy="4277160"/>
+        <a:ext cx="7604640" cy="4276800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3520,14 +3894,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>468720</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518760</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>518400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3535,8 +3909,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="468720" y="2568240"/>
-        <a:ext cx="7605000" cy="4277160"/>
+        <a:off x="468720" y="3381120"/>
+        <a:ext cx="7882920" cy="4276800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3560,9 +3934,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3571,7 +3945,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7604640" cy="4277160"/>
+        <a:ext cx="7604280" cy="4276800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3595,9 +3969,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>61200</xdr:colOff>
+      <xdr:colOff>60840</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3606,7 +3980,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="270000" y="3157200"/>
-        <a:ext cx="8383320" cy="4715280"/>
+        <a:ext cx="8382960" cy="4714920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3624,14 +3998,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4634,32 +5008,32 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>560</v>
+        <v>710</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>140</v>
+        <v>320</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>140</v>
+        <v>320</v>
       </c>
       <c r="J14" s="1" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1860</v>
+        <v>1820</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>100</v>
@@ -4687,19 +5061,90 @@
       </c>
       <c r="S14" s="1" t="n">
         <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
-        <v>2460</v>
-      </c>
-      <c r="T14" s="1" t="n">
-        <v>0</v>
+        <v>2420</v>
       </c>
       <c r="U14" s="1" t="n">
         <f aca="false">S14+T14</f>
+        <v>2420</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <f aca="false">SUM(B15,D15,F15*2,H15*2)</f>
+        <v>1860</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <f aca="false">SUM(J15,K15,M15,O15*2,Q15*2)</f>
         <v>2460</v>
       </c>
-      <c r="X14" s="0" t="n">
+      <c r="T15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <f aca="false">S15+T15</f>
+        <v>2460</v>
+      </c>
+      <c r="X15" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="Y14" s="0" t="n">
+      <c r="Y15" s="0" t="n">
         <v>70</v>
       </c>
     </row>
@@ -4732,7 +5177,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9EE573E7-5A54-4196-88D9-354AE89F97BF}</x14:id>
+          <x14:id>{314218C0-F2AB-4169-A51C-2E2EB7D8CEF8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4746,7 +5191,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4F5170B0-19FE-44F2-A8B0-914FB535D073}</x14:id>
+          <x14:id>{2F83F7CA-70D9-4362-AAA8-AA8CF565F1D3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4760,7 +5205,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C763D677-C360-40E2-9CE8-4D66711F5F3C}</x14:id>
+          <x14:id>{89299DE7-5B6F-44FB-A222-687B86DEDD5D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4777,7 +5222,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9EE573E7-5A54-4196-88D9-354AE89F97BF}">
+          <x14:cfRule type="dataBar" id="{314218C0-F2AB-4169-A51C-2E2EB7D8CEF8}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4788,7 +5233,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4F5170B0-19FE-44F2-A8B0-914FB535D073}">
+          <x14:cfRule type="dataBar" id="{2F83F7CA-70D9-4362-AAA8-AA8CF565F1D3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4799,7 +5244,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C763D677-C360-40E2-9CE8-4D66711F5F3C}">
+          <x14:cfRule type="dataBar" id="{89299DE7-5B6F-44FB-A222-687B86DEDD5D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4836,7 +5281,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>19</v>
@@ -4854,7 +5299,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4901,54 +5346,54 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="C11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4968,29 +5413,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>24</v>
@@ -5007,8 +5453,11 @@
       <c r="H1" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="J1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5133,7 +5582,7 @@
         <v>1855</v>
       </c>
       <c r="J7" s="0" t="n">
-        <f aca="false">MAX(B7:I7, J5)</f>
+        <f aca="false">MAX(B7:I7, J6)</f>
         <v>1855</v>
       </c>
     </row>
@@ -5150,9 +5599,12 @@
       <c r="H8" s="0" t="n">
         <v>1855</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>1980</v>
+      </c>
       <c r="J8" s="0" t="n">
-        <f aca="false">MAX(B8:I8, J6)</f>
-        <v>1855</v>
+        <f aca="false">MAX(B8:I8, J7)</f>
+        <v>1980</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5168,73 +5620,142 @@
       <c r="H9" s="0" t="n">
         <v>1975</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>1980</v>
+      </c>
       <c r="J9" s="0" t="n">
-        <f aca="false">MAX(B9:I9, J7)</f>
-        <v>1975</v>
+        <f aca="false">MAX(B9:I9, J8)</f>
+        <v>1980</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1940</v>
+        <v>1820</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2100</v>
       </c>
       <c r="J10" s="0" t="n">
         <f aca="false">MAX(B10:I10, J9)</f>
-        <v>1975</v>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1940</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">MAX(B11:I11, J10)</f>
+        <v>2100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="A12" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>2220</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">MAX(B12:I12, J11)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>2220</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">MAX(B13:I13, J12)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">MAX(B14:I14, J13)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">MAX(B15:I15, J14)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="B18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="0" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5270,13 +5791,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5341,18 +5862,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -5375,7 +5896,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5387,19 +5908,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5420,7 +5941,7 @@
         <v>740</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>860</v>
       </c>
     </row>
@@ -5433,7 +5954,7 @@
         <v>740</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>860</v>
       </c>
     </row>
@@ -5446,7 +5967,7 @@
         <v>980</v>
       </c>
       <c r="C5" s="0" t="n">
-        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1100</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -5463,7 +5984,7 @@
         <v>980</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1100</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -5480,7 +6001,7 @@
         <v>980</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1340</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -5497,7 +6018,7 @@
         <v>980</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1340</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -5514,7 +6035,7 @@
         <v>980</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1580</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -5531,7 +6052,7 @@
         <v>980</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1580</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -5548,7 +6069,7 @@
         <v>980</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>1855</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -5565,8 +6086,8 @@
         <v>980</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1855</v>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>1980</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5585,8 +6106,8 @@
         <v>980</v>
       </c>
       <c r="C13" s="0" t="n">
-        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>1980</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5605,8 +6126,8 @@
         <v>980</v>
       </c>
       <c r="C14" s="0" t="n">
-        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2100</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5625,8 +6146,8 @@
         <v>980</v>
       </c>
       <c r="C15" s="0" t="n">
-        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2100</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5645,8 +6166,8 @@
         <v>980</v>
       </c>
       <c r="C16" s="0" t="n">
-        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2220</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5665,8 +6186,8 @@
         <v>980</v>
       </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2220</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5685,8 +6206,8 @@
         <v>980</v>
       </c>
       <c r="C18" s="0" t="n">
-        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2220</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
@@ -5705,8 +6226,8 @@
         <v>980</v>
       </c>
       <c r="C19" s="0" t="n">
-        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$11, 10, 1)</f>
-        <v>1975</v>
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <v>2220</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>

</xml_diff>

<commit_message>
Add balance data for Brotherhood of Steel
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Leveled Power Increase - Raiders" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Leveled Power Increase - Gunners" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Leveled Power Increase - Institute" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Global Leveled Power Increase" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Leveled Power Increase - BoS" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Global Leveled Power Increase" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -223,6 +224,21 @@
     <t xml:space="preserve">I-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Knight:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight Captain:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWKCR BPAO Replacer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raiders</t>
   </si>
   <si>
@@ -367,7 +383,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,7 +429,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -521,7 +543,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -556,6 +578,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -604,7 +634,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -646,7 +676,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1213,11 +1243,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="79687069"/>
-        <c:axId val="35058567"/>
+        <c:axId val="74759706"/>
+        <c:axId val="22067374"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79687069"/>
+        <c:axId val="74759706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,14 +1282,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35058567"/>
+        <c:crossAx val="22067374"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35058567"/>
+        <c:axId val="22067374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79687069"/>
+        <c:crossAx val="74759706"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1340,7 +1370,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2448,6 +2478,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2572,11 +2603,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="69959549"/>
-        <c:axId val="92443669"/>
+        <c:axId val="578179"/>
+        <c:axId val="25954196"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69959549"/>
+        <c:axId val="578179"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,14 +2642,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92443669"/>
+        <c:crossAx val="25954196"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92443669"/>
+        <c:axId val="25954196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2662,7 +2693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69959549"/>
+        <c:crossAx val="578179"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2699,7 +2730,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2826,11 +2857,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="43412870"/>
-        <c:axId val="3371375"/>
+        <c:axId val="49801623"/>
+        <c:axId val="72932842"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43412870"/>
+        <c:axId val="49801623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2865,14 +2896,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3371375"/>
+        <c:crossAx val="72932842"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3371375"/>
+        <c:axId val="72932842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +2947,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43412870"/>
+        <c:crossAx val="49801623"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2953,7 +2984,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2967,7 +2998,1271 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Global Leveled Power Increase'!$B$1</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-51</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-02</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$E$2:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T-65</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="314004"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$H$2:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ultracite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="aecf00"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$I$2:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="19668857"/>
+        <c:axId val="38759489"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="19668857"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38759489"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38759489"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="19668857"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global Leveled Power Increase'!$B$1:$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3137,7 +4432,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Global Leveled Power Increase'!$C$1</c:f>
+              <c:f>'Global Leveled Power Increase'!$C$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3307,7 +4602,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Global Leveled Power Increase'!$D$1</c:f>
+              <c:f>'Global Leveled Power Increase'!$D$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3477,7 +4772,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Global Leveled Power Increase'!$E$1</c:f>
+              <c:f>'Global Leveled Power Increase'!$E$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3587,55 +4882,55 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>1975</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2200</c:v>
+                  <c:v>2220</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3650,11 +4945,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="12276346"/>
-        <c:axId val="30052810"/>
+        <c:axId val="98150255"/>
+        <c:axId val="30869809"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="12276346"/>
+        <c:axId val="98150255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3727,14 +5022,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30052810"/>
+        <c:crossAx val="30869809"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30052810"/>
+        <c:axId val="30869809"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3816,7 +5111,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12276346"/>
+        <c:crossAx val="98150255"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3864,9 +5159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3875,7 +5170,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7604640" cy="4276800"/>
+        <a:ext cx="7604280" cy="4276440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3899,9 +5194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3910,7 +5205,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3381120"/>
-        <a:ext cx="7882920" cy="4276800"/>
+        <a:ext cx="7882560" cy="4276440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3934,9 +5229,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3945,7 +5240,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7604280" cy="4276800"/>
+        <a:ext cx="7603920" cy="4276440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3963,15 +5258,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>270000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:colOff>468720</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>60840</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>518040</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3979,8 +5274,43 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
+        <a:off x="468720" y="3053520"/>
+        <a:ext cx="7882560" cy="4276440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>270000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>60480</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
         <a:off x="270000" y="3157200"/>
-        <a:ext cx="8382960" cy="4714920"/>
+        <a:ext cx="8382600" cy="4714560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4005,7 +5335,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5177,7 +6507,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{314218C0-F2AB-4169-A51C-2E2EB7D8CEF8}</x14:id>
+          <x14:id>{501CC735-8D74-4000-ADF2-E83469AF2AF3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5191,7 +6521,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2F83F7CA-70D9-4362-AAA8-AA8CF565F1D3}</x14:id>
+          <x14:id>{48E3C1A1-8648-4E41-85E1-40E01C26289A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5205,7 +6535,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{89299DE7-5B6F-44FB-A222-687B86DEDD5D}</x14:id>
+          <x14:id>{4FC951F0-21C8-4097-94AF-D32DCFA7529D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5222,7 +6552,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{314218C0-F2AB-4169-A51C-2E2EB7D8CEF8}">
+          <x14:cfRule type="dataBar" id="{501CC735-8D74-4000-ADF2-E83469AF2AF3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -5233,7 +6563,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2F83F7CA-70D9-4362-AAA8-AA8CF565F1D3}">
+          <x14:cfRule type="dataBar" id="{48E3C1A1-8648-4E41-85E1-40E01C26289A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -5244,7 +6574,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{89299DE7-5B6F-44FB-A222-687B86DEDD5D}">
+          <x14:cfRule type="dataBar" id="{4FC951F0-21C8-4097-94AF-D32DCFA7529D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -5415,7 +6745,7 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -5893,10 +7223,309 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>860</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>860</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">MAX(B2:I2)</f>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B3" s="9" t="n">
+        <v>1100</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>980</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">MAX(B3:I3, J2)</f>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="n">
+        <v>1100</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">MAX(B4:I4, J3)</f>
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="n">
+        <v>1220</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">MAX(B5:I5, J4)</f>
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="n">
+        <v>1340</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1975</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">MAX(B6:I6, J5)</f>
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="I7" s="0" t="n">
+        <v>2220</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">MAX(B7:I7, J6)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="J8" s="0" t="n">
+        <f aca="false">MAX(B8:I8, J7)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="J9" s="0" t="n">
+        <f aca="false">MAX(B9:I9, J8)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="J10" s="0" t="n">
+        <f aca="false">MAX(B10:I10, J9)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="0" t="n">
+        <f aca="false">MAX(B11:I11, J10)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="J12" s="0" t="n">
+        <f aca="false">MAX(B12:I12, J11)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="J13" s="0" t="n">
+        <f aca="false">MAX(B13:I13, J12)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:C18"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5911,16 +7540,16 @@
         <v>32</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5944,6 +7573,10 @@
         <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>860</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1340</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -5957,6 +7590,10 @@
         <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
         <v>860</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1340</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -5974,6 +7611,10 @@
         <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>980</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1340</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -5991,6 +7632,10 @@
         <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1080</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1340</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -6008,6 +7653,10 @@
         <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1180</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1580</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -6025,6 +7674,10 @@
         <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1280</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1580</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -6042,6 +7695,10 @@
         <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1380</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1820</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -6059,6 +7716,10 @@
         <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1380</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1820</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -6076,6 +7737,10 @@
         <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Institute'!$A$2:$J$9, 10, 1)</f>
         <v>1380</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>1975</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -6094,7 +7759,8 @@
         <v>1380</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6114,7 +7780,8 @@
         <v>1380</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6134,7 +7801,8 @@
         <v>1380</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6154,7 +7822,8 @@
         <v>1380</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,7 +7843,8 @@
         <v>1380</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6194,7 +7864,8 @@
         <v>1380</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,7 +7885,8 @@
         <v>1380</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6234,7 +7906,8 @@
         <v>1380</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>2200</v>
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <v>2220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update balance sheet with data on the Creation Club X-02 and X-03 power armor sets
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="S4" authorId="0">
+    <comment ref="S3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -107,10 +107,10 @@
     <t xml:space="preserve">Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Excavator</t>
+    <t xml:space="preserve">Raider</t>
   </si>
   <si>
-    <t xml:space="preserve">Raider</t>
+    <t xml:space="preserve">Excavator</t>
   </si>
   <si>
     <t xml:space="preserve">T-45</t>
@@ -131,7 +131,13 @@
     <t xml:space="preserve">T-60</t>
   </si>
   <si>
+    <t xml:space="preserve">Hellfire (CC)</t>
+  </si>
+  <si>
     <t xml:space="preserve">X-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-02 (CC)</t>
   </si>
   <si>
     <t xml:space="preserve">T-65</t>
@@ -659,7 +665,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FFAECF00"/>
       <rgbColor rgb="FFFFD320"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF950E"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -669,14 +675,14 @@
       <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF4B1F6F"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart121.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1243,11 +1249,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="74759706"/>
-        <c:axId val="22067374"/>
+        <c:axId val="77357976"/>
+        <c:axId val="26073720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74759706"/>
+        <c:axId val="77357976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,14 +1288,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22067374"/>
+        <c:crossAx val="26073720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22067374"/>
+        <c:axId val="26073720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1339,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74759706"/>
+        <c:crossAx val="77357976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1370,7 +1376,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart122.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2148,7 +2154,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T-65</c:v>
+                  <c:v>X-02 (CC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2248,28 +2254,28 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1580</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1700</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1820</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1820</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1940</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -2300,7 +2306,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-03</c:v>
+                  <c:v>Hellfire (CC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2400,28 +2406,28 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1855</c:v>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1855</c:v>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1975</c:v>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -2452,7 +2458,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Classic Advanced</c:v>
+                  <c:v>T-65</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2555,6 +2561,308 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4b1f6f"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$J$2:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Classic Advanced</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff950e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - Gunners'!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - Gunners'!$K$2:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
@@ -2603,11 +2911,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="578179"/>
-        <c:axId val="25954196"/>
+        <c:axId val="42850922"/>
+        <c:axId val="98042476"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="578179"/>
+        <c:axId val="42850922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2642,14 +2950,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25954196"/>
+        <c:crossAx val="98042476"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25954196"/>
+        <c:axId val="98042476"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +3001,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578179"/>
+        <c:crossAx val="42850922"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2730,7 +3038,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart123.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2857,11 +3165,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="49801623"/>
-        <c:axId val="72932842"/>
+        <c:axId val="3619493"/>
+        <c:axId val="55530232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49801623"/>
+        <c:axId val="3619493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2896,14 +3204,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72932842"/>
+        <c:crossAx val="55530232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72932842"/>
+        <c:axId val="55530232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2947,7 +3255,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49801623"/>
+        <c:crossAx val="3619493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2984,7 +3292,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart124.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3702,7 +4010,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T-65</c:v>
+                  <c:v>X-02 (CC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3796,10 +4104,10 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1820</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v/>
@@ -3842,7 +4150,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-03</c:v>
+                  <c:v>Hellfire (CC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3936,13 +4244,13 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1580</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1975</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3982,7 +4290,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ultracite</c:v>
+                  <c:v>T-65</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4079,6 +4387,284 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X-03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4b1f6f"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$J$2:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ultracite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff950e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Leveled Power Increase - BoS'!$K$2:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
@@ -4121,11 +4707,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19668857"/>
-        <c:axId val="38759489"/>
+        <c:axId val="18440964"/>
+        <c:axId val="90889863"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19668857"/>
+        <c:axId val="18440964"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,14 +4746,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38759489"/>
+        <c:crossAx val="90889863"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38759489"/>
+        <c:axId val="90889863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4211,7 +4797,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19668857"/>
+        <c:crossAx val="18440964"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4248,7 +4834,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart125.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4945,11 +5531,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="98150255"/>
-        <c:axId val="30869809"/>
+        <c:axId val="38631021"/>
+        <c:axId val="36354668"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98150255"/>
+        <c:axId val="38631021"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5022,14 +5608,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30869809"/>
+        <c:crossAx val="36354668"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30869809"/>
+        <c:axId val="36354668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5111,7 +5697,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98150255"/>
+        <c:crossAx val="38631021"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5193,8 +5779,8 @@
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1167840</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
@@ -5205,7 +5791,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3381120"/>
-        <a:ext cx="7882560" cy="4276440"/>
+        <a:ext cx="10157760" cy="4276440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5263,8 +5849,8 @@
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1167840</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
@@ -5275,7 +5861,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3053520"/>
-        <a:ext cx="7882560" cy="4276440"/>
+        <a:ext cx="10157760" cy="4276440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5328,14 +5914,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5492,67 +6078,67 @@
         <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>50</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>50</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>50</v>
       </c>
       <c r="J3" s="1" t="n">
         <f aca="false">SUM(B3,D3,F3*2,H3*2)</f>
-        <v>380</v>
+        <v>500</v>
       </c>
       <c r="K3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L3" s="1" t="n">
-        <v>300</v>
-      </c>
       <c r="M3" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="S3" s="1" t="n">
         <f aca="false">SUM(J3,K3,M3,O3*2,Q3*2)</f>
-        <v>980</v>
+        <v>620</v>
       </c>
       <c r="T3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U3" s="1" t="n">
         <f aca="false">S3+T3</f>
-        <v>980</v>
+        <v>620</v>
       </c>
       <c r="X3" s="0" t="n">
         <v>14</v>
@@ -5566,67 +6152,67 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>100</v>
-      </c>
       <c r="D4" s="0" t="n">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>50</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>50</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>50</v>
       </c>
       <c r="J4" s="1" t="n">
         <f aca="false">SUM(B4,D4,F4*2,H4*2)</f>
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="L4" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="M4" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N4" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="S4" s="1" t="n">
         <f aca="false">SUM(J4,K4,M4,O4*2,Q4*2)</f>
-        <v>620</v>
+        <v>980</v>
       </c>
       <c r="T4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U4" s="1" t="n">
         <f aca="false">S4+T4</f>
-        <v>620</v>
+        <v>980</v>
       </c>
       <c r="X4" s="0" t="n">
         <v>14</v>
@@ -6103,56 +6689,56 @@
         <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>560</v>
+        <v>260</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1" t="n">
         <f aca="false">SUM(B11,D11,F11*2,H11*2)</f>
-        <v>1220</v>
+        <v>620</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="R11" s="1" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="S11" s="1" t="n">
         <f aca="false">SUM(J11,K11,M11,O11*2,Q11*2)</f>
@@ -6164,12 +6750,6 @@
       <c r="U11" s="1" t="n">
         <f aca="false">S11+T11</f>
         <v>1820</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="W11" s="0" t="n">
-        <v>28</v>
       </c>
       <c r="X11" s="0" t="n">
         <v>40</v>
@@ -6183,32 +6763,32 @@
         <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>360</v>
+        <v>320</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>680</v>
+        <v>560</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="E12" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>210</v>
-      </c>
       <c r="G12" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <v>210</v>
-      </c>
       <c r="I12" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="J12" s="1" t="n">
         <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>1460</v>
+        <v>1220</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>100</v>
@@ -6236,26 +6816,26 @@
       </c>
       <c r="S12" s="1" t="n">
         <f aca="false">SUM(J12,K12,M12,O12*2,Q12*2)</f>
-        <v>2060</v>
+        <v>1820</v>
       </c>
       <c r="T12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="U12" s="1" t="n">
         <f aca="false">S12+T12</f>
-        <v>2060</v>
+        <v>1820</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="W12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="X12" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="X12" s="0" t="n">
+      <c r="Y12" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="Y12" s="0" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6263,74 +6843,73 @@
         <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>380</v>
+        <v>320</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>600</v>
+        <v>560</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="G13" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <v>190</v>
-      </c>
       <c r="I13" s="1" t="n">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>1375</v>
+        <v>1220</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>100</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>100</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>100</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>100</v>
       </c>
       <c r="R13" s="1" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="S13" s="1" t="n">
         <f aca="false">SUM(J13,K13,M13,O13*2,Q13*2)</f>
-        <v>1975</v>
+        <v>1820</v>
       </c>
       <c r="T13" s="1" t="n">
-        <f aca="false">(80+20)*6+80</f>
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1" t="n">
         <f aca="false">S13+T13</f>
-        <v>2655</v>
+        <v>1820</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="Y13" s="0" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6338,32 +6917,32 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>460</v>
+        <v>360</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>710</v>
+        <v>680</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="J14" s="1" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1820</v>
+        <v>1460</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>100</v>
@@ -6391,17 +6970,26 @@
       </c>
       <c r="S14" s="1" t="n">
         <f aca="false">SUM(J14,K14,M14,O14*2,Q14*2)</f>
-        <v>2420</v>
+        <v>2060</v>
+      </c>
+      <c r="T14" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="U14" s="1" t="n">
         <f aca="false">S14+T14</f>
-        <v>2420</v>
+        <v>2060</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>40</v>
       </c>
       <c r="X14" s="0" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="Y14" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6409,32 +6997,32 @@
         <v>31</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>300</v>
+        <v>235</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="J15" s="1" t="n">
         <f aca="false">SUM(B15,D15,F15*2,H15*2)</f>
-        <v>1860</v>
+        <v>1375</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>100</v>
@@ -6462,19 +7050,168 @@
       </c>
       <c r="S15" s="1" t="n">
         <f aca="false">SUM(J15,K15,M15,O15*2,Q15*2)</f>
-        <v>2460</v>
+        <v>1975</v>
       </c>
       <c r="T15" s="1" t="n">
-        <v>0</v>
+        <f aca="false">(80+20)*6+80</f>
+        <v>680</v>
       </c>
       <c r="U15" s="1" t="n">
         <f aca="false">S15+T15</f>
+        <v>2655</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>710</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <f aca="false">SUM(B16,D16,F16*2,H16*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <f aca="false">SUM(J16,K16,M16,O16*2,Q16*2)</f>
+        <v>2420</v>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <f aca="false">S16+T16</f>
+        <v>2420</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <f aca="false">SUM(B17,D17,F17*2,H17*2)</f>
+        <v>1860</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <f aca="false">SUM(J17,K17,M17,O17*2,Q17*2)</f>
         <v>2460</v>
       </c>
-      <c r="X15" s="0" t="n">
+      <c r="T17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <f aca="false">S17+T17</f>
+        <v>2460</v>
+      </c>
+      <c r="X17" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="Y15" s="0" t="n">
+      <c r="Y17" s="0" t="n">
         <v>70</v>
       </c>
     </row>
@@ -6507,7 +7244,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{501CC735-8D74-4000-ADF2-E83469AF2AF3}</x14:id>
+          <x14:id>{1FF5C717-D080-4947-8E1D-B39BB771209E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6521,7 +7258,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{48E3C1A1-8648-4E41-85E1-40E01C26289A}</x14:id>
+          <x14:id>{C7802EF1-BBE1-418D-8468-E03F25673F72}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6535,7 +7272,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4FC951F0-21C8-4097-94AF-D32DCFA7529D}</x14:id>
+          <x14:id>{60F0226C-DB47-45A6-AD3F-271C403AFA83}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6552,7 +7289,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{501CC735-8D74-4000-ADF2-E83469AF2AF3}">
+          <x14:cfRule type="dataBar" id="{1FF5C717-D080-4947-8E1D-B39BB771209E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -6563,7 +7300,7 @@
           <xm:sqref>S2:S1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{48E3C1A1-8648-4E41-85E1-40E01C26289A}">
+          <x14:cfRule type="dataBar" id="{C7802EF1-BBE1-418D-8468-E03F25673F72}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -6574,7 +7311,7 @@
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4FC951F0-21C8-4097-94AF-D32DCFA7529D}">
+          <x14:cfRule type="dataBar" id="{60F0226C-DB47-45A6-AD3F-271C403AFA83}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -6611,13 +7348,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>21</v>
@@ -6629,7 +7366,7 @@
         <v>26</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6676,54 +7413,54 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -6743,30 +7480,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>24</v>
@@ -6775,19 +7512,25 @@
         <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>30</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6800,8 +7543,8 @@
       <c r="C2" s="0" t="n">
         <v>860</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <f aca="false">MAX(B2:I2)</f>
+      <c r="L2" s="0" t="n">
+        <f aca="false">MAX(B2:K2)</f>
         <v>860</v>
       </c>
     </row>
@@ -6821,8 +7564,8 @@
       <c r="E3" s="0" t="n">
         <v>1100</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">MAX(B3:I3, J2)</f>
+      <c r="L3" s="0" t="n">
+        <f aca="false">MAX(B3:K3, L2)</f>
         <v>1100</v>
       </c>
     </row>
@@ -6845,8 +7588,14 @@
       <c r="F4" s="0" t="n">
         <v>1340</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">MAX(B4:I4, J3)</f>
+      <c r="G4" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">MAX(B4:K4, L3)</f>
         <v>1340</v>
       </c>
     </row>
@@ -6867,10 +7616,16 @@
         <v>1460</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>1460</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="I5" s="0" t="n">
         <v>1580</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">MAX(B5:I5, J4)</f>
+      <c r="L5" s="0" t="n">
+        <f aca="false">MAX(B5:K5, L4)</f>
         <v>1580</v>
       </c>
     </row>
@@ -6888,10 +7643,16 @@
         <v>1460</v>
       </c>
       <c r="G6" s="0" t="n">
+        <v>1460</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1340</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>1580</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">MAX(B6:I6, J5)</f>
+      <c r="L6" s="0" t="n">
+        <f aca="false">MAX(B6:K6, L5)</f>
         <v>1580</v>
       </c>
     </row>
@@ -6906,13 +7667,19 @@
         <v>1580</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="I7" s="0" t="n">
         <v>1700</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>1855</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">MAX(B7:I7, J6)</f>
+      <c r="L7" s="0" t="n">
+        <f aca="false">MAX(B7:K7, L6)</f>
         <v>1855</v>
       </c>
     </row>
@@ -6923,17 +7690,23 @@
       <c r="F8" s="6" t="n">
         <v>1700</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="8" t="n">
+        <v>1580</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="I8" s="0" t="n">
         <v>1700</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>1855</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">MAX(B8:I8, J7)</f>
+      <c r="L8" s="0" t="n">
+        <f aca="false">MAX(B8:K8, L7)</f>
         <v>1980</v>
       </c>
     </row>
@@ -6945,16 +7718,22 @@
         <v>1700</v>
       </c>
       <c r="G9" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="I9" s="0" t="n">
         <v>1820</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <f aca="false">MAX(B9:I9, J8)</f>
+      <c r="L9" s="0" t="n">
+        <f aca="false">MAX(B9:K9, L8)</f>
         <v>1980</v>
       </c>
     </row>
@@ -6962,14 +7741,17 @@
       <c r="A10" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="I10" s="0" t="n">
         <v>1820</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="K10" s="0" t="n">
         <v>2100</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <f aca="false">MAX(B10:I10, J9)</f>
+      <c r="L10" s="0" t="n">
+        <f aca="false">MAX(B10:K10, L9)</f>
         <v>2100</v>
       </c>
     </row>
@@ -6977,14 +7759,17 @@
       <c r="A11" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="I11" s="0" t="n">
         <v>1940</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="K11" s="0" t="n">
         <v>2100</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <f aca="false">MAX(B11:I11, J10)</f>
+      <c r="L11" s="0" t="n">
+        <f aca="false">MAX(B11:K11, L10)</f>
         <v>2100</v>
       </c>
     </row>
@@ -6992,11 +7777,11 @@
       <c r="A12" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>2220</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <f aca="false">MAX(B12:I12, J11)</f>
+      <c r="L12" s="0" t="n">
+        <f aca="false">MAX(B12:K12, L11)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7004,11 +7789,11 @@
       <c r="A13" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="K13" s="8" t="n">
         <v>2220</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">MAX(B13:I13, J12)</f>
+      <c r="L13" s="0" t="n">
+        <f aca="false">MAX(B13:K13, L12)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7016,8 +7801,8 @@
       <c r="A14" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">MAX(B14:I14, J13)</f>
+      <c r="L14" s="0" t="n">
+        <f aca="false">MAX(B14:K14, L13)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7025,67 +7810,79 @@
       <c r="A15" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">MAX(B15:I15, J14)</f>
+      <c r="L15" s="0" t="n">
+        <f aca="false">MAX(B15:K15, L14)</f>
         <v>2220</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="D17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -7121,13 +7918,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7192,18 +7989,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -7223,24 +8020,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>21</v>
@@ -7255,19 +8052,25 @@
         <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="I1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>33</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7283,8 +8086,8 @@
       <c r="E2" s="0" t="n">
         <v>1340</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <f aca="false">MAX(B2:I2)</f>
+      <c r="L2" s="0" t="n">
+        <f aca="false">MAX(B2:K2)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7301,8 +8104,8 @@
       <c r="D3" s="0" t="n">
         <v>1280</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">MAX(B3:I3, J2)</f>
+      <c r="L3" s="0" t="n">
+        <f aca="false">MAX(B3:K3, L2)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7317,8 +8120,14 @@
       <c r="F4" s="0" t="n">
         <v>1580</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">MAX(B4:I4, J3)</f>
+      <c r="G4" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1580</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">MAX(B4:K4, L3)</f>
         <v>1580</v>
       </c>
     </row>
@@ -7330,11 +8139,11 @@
       <c r="C5" s="9" t="n">
         <v>1220</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>1820</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">MAX(B5:I5, J4)</f>
+      <c r="L5" s="0" t="n">
+        <f aca="false">MAX(B5:K5, L4)</f>
         <v>1820</v>
       </c>
     </row>
@@ -7346,11 +8155,11 @@
       <c r="C6" s="9" t="n">
         <v>1340</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">MAX(B6:I6, J5)</f>
+      <c r="L6" s="0" t="n">
+        <f aca="false">MAX(B6:K6, L5)</f>
         <v>1975</v>
       </c>
     </row>
@@ -7360,11 +8169,11 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="I7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>2220</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">MAX(B7:I7, J6)</f>
+      <c r="L7" s="0" t="n">
+        <f aca="false">MAX(B7:K7, L6)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7374,8 +8183,8 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="J8" s="0" t="n">
-        <f aca="false">MAX(B8:I8, J7)</f>
+      <c r="L8" s="0" t="n">
+        <f aca="false">MAX(B8:K8, L7)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7385,8 +8194,8 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="J9" s="0" t="n">
-        <f aca="false">MAX(B9:I9, J8)</f>
+      <c r="L9" s="0" t="n">
+        <f aca="false">MAX(B9:K9, L8)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7396,8 +8205,8 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="J10" s="0" t="n">
-        <f aca="false">MAX(B10:I10, J9)</f>
+      <c r="L10" s="0" t="n">
+        <f aca="false">MAX(B10:K10, L9)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7407,9 +8216,9 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="0" t="n">
-        <f aca="false">MAX(B11:I11, J10)</f>
+      <c r="K11" s="8"/>
+      <c r="L11" s="0" t="n">
+        <f aca="false">MAX(B11:K11, L10)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7419,8 +8228,8 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="J12" s="0" t="n">
-        <f aca="false">MAX(B12:I12, J11)</f>
+      <c r="L12" s="0" t="n">
+        <f aca="false">MAX(B12:K12, L11)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7430,8 +8239,8 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="J13" s="0" t="n">
-        <f aca="false">MAX(B13:I13, J12)</f>
+      <c r="L13" s="0" t="n">
+        <f aca="false">MAX(B13:K13, L12)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7441,64 +8250,70 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" s="10"/>
     </row>
@@ -7525,7 +8340,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7537,19 +8352,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7570,11 +8385,11 @@
         <v>740</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>860</v>
       </c>
       <c r="E3" s="0" t="n">
-        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7587,11 +8402,11 @@
         <v>740</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>860</v>
       </c>
       <c r="E4" s="0" t="n">
-        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7604,7 +8419,7 @@
         <v>980</v>
       </c>
       <c r="C5" s="0" t="n">
-        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1100</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -7612,7 +8427,7 @@
         <v>980</v>
       </c>
       <c r="E5" s="0" t="n">
-        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7625,7 +8440,7 @@
         <v>980</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1100</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -7633,7 +8448,7 @@
         <v>1080</v>
       </c>
       <c r="E6" s="0" t="n">
-        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1340</v>
       </c>
     </row>
@@ -7646,7 +8461,7 @@
         <v>980</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1340</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -7654,7 +8469,7 @@
         <v>1180</v>
       </c>
       <c r="E7" s="0" t="n">
-        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1580</v>
       </c>
     </row>
@@ -7667,7 +8482,7 @@
         <v>980</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1340</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -7675,7 +8490,7 @@
         <v>1280</v>
       </c>
       <c r="E8" s="0" t="n">
-        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1580</v>
       </c>
     </row>
@@ -7688,7 +8503,7 @@
         <v>980</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1580</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -7696,7 +8511,7 @@
         <v>1380</v>
       </c>
       <c r="E9" s="0" t="n">
-        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1820</v>
       </c>
     </row>
@@ -7709,7 +8524,7 @@
         <v>980</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1580</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -7717,7 +8532,7 @@
         <v>1380</v>
       </c>
       <c r="E10" s="0" t="n">
-        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1820</v>
       </c>
     </row>
@@ -7730,7 +8545,7 @@
         <v>980</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1855</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -7738,7 +8553,7 @@
         <v>1380</v>
       </c>
       <c r="E11" s="0" t="n">
-        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>1975</v>
       </c>
     </row>
@@ -7751,7 +8566,7 @@
         <v>980</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1980</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -7759,7 +8574,7 @@
         <v>1380</v>
       </c>
       <c r="E12" s="0" t="n">
-        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7772,7 +8587,7 @@
         <v>980</v>
       </c>
       <c r="C13" s="0" t="n">
-        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>1980</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -7780,7 +8595,7 @@
         <v>1380</v>
       </c>
       <c r="E13" s="0" t="n">
-        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7793,7 +8608,7 @@
         <v>980</v>
       </c>
       <c r="C14" s="0" t="n">
-        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2100</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -7801,7 +8616,7 @@
         <v>1380</v>
       </c>
       <c r="E14" s="0" t="n">
-        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7814,7 +8629,7 @@
         <v>980</v>
       </c>
       <c r="C15" s="0" t="n">
-        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2100</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -7822,7 +8637,7 @@
         <v>1380</v>
       </c>
       <c r="E15" s="0" t="n">
-        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A15, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7835,7 +8650,7 @@
         <v>980</v>
       </c>
       <c r="C16" s="0" t="n">
-        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2220</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -7843,7 +8658,7 @@
         <v>1380</v>
       </c>
       <c r="E16" s="0" t="n">
-        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A16, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7856,7 +8671,7 @@
         <v>980</v>
       </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2220</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -7864,7 +8679,7 @@
         <v>1380</v>
       </c>
       <c r="E17" s="0" t="n">
-        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A17, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7877,7 +8692,7 @@
         <v>980</v>
       </c>
       <c r="C18" s="0" t="n">
-        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2220</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -7885,7 +8700,7 @@
         <v>1380</v>
       </c>
       <c r="E18" s="0" t="n">
-        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A18, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>
@@ -7898,7 +8713,7 @@
         <v>980</v>
       </c>
       <c r="C19" s="0" t="n">
-        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$J$16, 10, 1)</f>
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - Gunners'!$A$2:$L$16, 12, 1)</f>
         <v>2220</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -7906,7 +8721,7 @@
         <v>1380</v>
       </c>
       <c r="E19" s="0" t="n">
-        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - BoS'!$A$2:$J$14, 10, 1)</f>
+        <f aca="false">VLOOKUP($A19, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
         <v>2220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rearrange overall balance levels based on energy resistances
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -37,7 +37,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This changes drastically if Raider Overhaul is installed, becoming much stronger</t>
         </r>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="74">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -95,6 +94,12 @@
     <t xml:space="preserve">Highest Combined Total for a Player</t>
   </si>
   <si>
+    <t xml:space="preserve">Level Highest Player Total Can Be Crafted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perks Required for Highest Player Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level Partial Sets Are Available</t>
   </si>
   <si>
@@ -119,6 +124,9 @@
     <t xml:space="preserve">Raider</t>
   </si>
   <si>
+    <t xml:space="preserve">Armorer 4 + Science 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Excavator</t>
   </si>
   <si>
@@ -131,13 +139,16 @@
     <t xml:space="preserve">T-51c</t>
   </si>
   <si>
-    <t xml:space="preserve">X-02</t>
-  </si>
-  <si>
     <t xml:space="preserve">Institute</t>
   </si>
   <si>
     <t xml:space="preserve">Quest locked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armorer 4 + Science 4 + Nuclear Physicist 3</t>
   </si>
   <si>
     <t xml:space="preserve">T-60</t>
@@ -146,25 +157,25 @@
     <t xml:space="preserve">Horse</t>
   </si>
   <si>
-    <t xml:space="preserve">Hellfire (CC)</t>
-  </si>
-  <si>
     <t xml:space="preserve">X-01</t>
   </si>
   <si>
     <t xml:space="preserve">X-02 (CC)</t>
   </si>
   <si>
-    <t xml:space="preserve">T-65</t>
+    <t xml:space="preserve">Hellfire (CC)</t>
   </si>
   <si>
     <t xml:space="preserve">X-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Classic Advanced</t>
+    <t xml:space="preserve">T-65</t>
   </si>
   <si>
     <t xml:space="preserve">Ultracite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Advanced</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -226,7 +237,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">F + </t>
     </r>
@@ -236,7 +246,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tesla</t>
     </r>
@@ -247,7 +256,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E + </t>
     </r>
@@ -257,7 +265,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tesla</t>
     </r>
@@ -304,12 +311,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -332,23 +338,16 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -423,7 +422,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -462,6 +461,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -557,7 +560,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart136.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1525,11 +1528,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="80111089"/>
-        <c:axId val="36798992"/>
+        <c:axId val="27506484"/>
+        <c:axId val="66288033"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80111089"/>
+        <c:axId val="27506484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36798992"/>
+        <c:crossAx val="66288033"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1568,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36798992"/>
+        <c:axId val="66288033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1608,7 +1611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80111089"/>
+        <c:crossAx val="27506484"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1659,7 +1662,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart137.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3073,11 +3076,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="61821661"/>
-        <c:axId val="46722795"/>
+        <c:axId val="49237055"/>
+        <c:axId val="35703292"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61821661"/>
+        <c:axId val="49237055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3108,7 +3111,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46722795"/>
+        <c:crossAx val="35703292"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3116,7 +3119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46722795"/>
+        <c:axId val="35703292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3156,7 +3159,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61821661"/>
+        <c:crossAx val="49237055"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3204,7 +3207,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart138.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3219,7 +3222,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leveled Power Increase - Instit'!$B$1:$B$1</c:f>
+              <c:f>'Leveled Power Increase - Instit'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3340,11 +3343,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="5972110"/>
-        <c:axId val="1657892"/>
+        <c:axId val="70063840"/>
+        <c:axId val="66459938"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5972110"/>
+        <c:axId val="70063840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3375,7 +3378,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1657892"/>
+        <c:crossAx val="66459938"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3383,7 +3386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1657892"/>
+        <c:axId val="66459938"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3423,7 +3426,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5972110"/>
+        <c:crossAx val="70063840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3474,7 +3477,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4717,11 +4720,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="43418221"/>
-        <c:axId val="80057224"/>
+        <c:axId val="3316534"/>
+        <c:axId val="46306350"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43418221"/>
+        <c:axId val="3316534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4752,7 +4755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80057224"/>
+        <c:crossAx val="46306350"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4760,7 +4763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80057224"/>
+        <c:axId val="46306350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4800,7 +4803,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43418221"/>
+        <c:crossAx val="3316534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4851,7 +4854,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart140.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5799,11 +5802,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="55761669"/>
-        <c:axId val="17353872"/>
+        <c:axId val="77619470"/>
+        <c:axId val="69584921"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55761669"/>
+        <c:axId val="77619470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +5871,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17353872"/>
+        <c:crossAx val="69584921"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5876,7 +5879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17353872"/>
+        <c:axId val="69584921"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5950,7 +5953,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55761669"/>
+        <c:crossAx val="77619470"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6057,7 +6060,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="468720" y="3381120"/>
+        <a:off x="468720" y="3378600"/>
         <a:ext cx="10200240" cy="4273200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -6148,13 +6151,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>260280</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>65880</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6162,7 +6165,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="260280" y="2631600"/>
+        <a:off x="260280" y="2631960"/>
         <a:ext cx="8408520" cy="4711320"/>
       </xdr:xfrm>
       <a:graphic>
@@ -6181,14 +6184,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="Y13" activeCellId="0" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6216,7 +6219,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="10.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.55"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6273,10 +6278,10 @@
       <c r="W1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="Z1" s="7" t="s">
@@ -6288,72 +6293,80 @@
       <c r="AB1" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="AC1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" s="8" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>200</v>
@@ -6426,19 +6439,25 @@
         <f aca="false">U3+V3</f>
         <v>870</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="X3" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AC3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AD3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>130</v>
@@ -6511,16 +6530,22 @@
         <f aca="false">U4+V4</f>
         <v>1770</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="X4" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="AB4" s="0" t="n">
+      <c r="AD4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>200</v>
@@ -6593,25 +6618,31 @@
         <f aca="false">U5+V5</f>
         <v>2010</v>
       </c>
-      <c r="X5" s="0" t="n">
+      <c r="X5" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="AA5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="0" t="n">
+      <c r="AB5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AA5" s="0" t="n">
+      <c r="AC5" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="AB5" s="0" t="n">
+      <c r="AD5" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>240</v>
@@ -6684,25 +6715,31 @@
         <f aca="false">U6+V6</f>
         <v>2430</v>
       </c>
-      <c r="X6" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <v>14</v>
+      <c r="X6" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="Z6" s="0" t="n">
         <v>14</v>
       </c>
       <c r="AA6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="AB6" s="0" t="n">
+      <c r="AD6" s="0" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>240</v>
@@ -6775,48 +6812,54 @@
         <f aca="false">U7+V7</f>
         <v>2430</v>
       </c>
-      <c r="AA7" s="0" t="n">
+      <c r="X7" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC7" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="AB7" s="0" t="n">
+      <c r="AD7" s="0" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>230</v>
+        <v>360</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="G8" s="1" t="n">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="J8" s="2" t="n">
         <f aca="false">SUM(B8,D8,F8*2,H8*2)</f>
-        <v>680</v>
+        <v>880</v>
       </c>
       <c r="K8" s="2" t="n">
         <f aca="false">SUM(B8:E8) + SUM(F8:I8)*2</f>
-        <v>1170</v>
+        <v>1405</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>100</v>
@@ -6825,10 +6868,10 @@
         <v>100</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>100</v>
@@ -6844,121 +6887,133 @@
       </c>
       <c r="T8" s="2" t="n">
         <f aca="false">SUM(J8,L8,N8,P8*2,R8*2)</f>
-        <v>1280</v>
+        <v>1380</v>
       </c>
       <c r="U8" s="2" t="n">
         <f aca="false">K8+SUM(L8:O8)+SUM(P8:S8)*2</f>
+        <v>2405</v>
+      </c>
+      <c r="V8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1" t="n">
+        <f aca="false">U8+V8</f>
+        <v>2405</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <f aca="false">SUM(B9,D9,F9*2,H9*2)</f>
+        <v>680</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <f aca="false">SUM(B9:E9) + SUM(F9:I9)*2</f>
+        <v>1170</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <f aca="false">SUM(J9,L9,N9,P9*2,R9*2)</f>
+        <v>1280</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <f aca="false">K9+SUM(L9:O9)+SUM(P9:S9)*2</f>
         <v>2370</v>
       </c>
-      <c r="V8" s="1" t="n">
+      <c r="V9" s="1" t="n">
         <f aca="false">(25+40)*6</f>
         <v>390</v>
       </c>
-      <c r="W8" s="1" t="n">
-        <f aca="false">U8+V8</f>
-        <v>2760</v>
-      </c>
-      <c r="Y8" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="Z8" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AA8" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB8" s="0" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>185</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <f aca="false">SUM(B9,D9,F9*2,H9*2)</f>
-        <v>880</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <f aca="false">SUM(B9:E9) + SUM(F9:I9)*2</f>
-        <v>1405</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="R9" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T9" s="2" t="n">
-        <f aca="false">SUM(J9,L9,N9,P9*2,R9*2)</f>
-        <v>1380</v>
-      </c>
-      <c r="U9" s="2" t="n">
-        <f aca="false">K9+SUM(L9:O9)+SUM(P9:S9)*2</f>
-        <v>2405</v>
-      </c>
-      <c r="V9" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W9" s="1" t="n">
         <f aca="false">U9+V9</f>
-        <v>2405</v>
-      </c>
-      <c r="Z9" s="0" t="s">
-        <v>29</v>
+        <v>2760</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="AA9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC9" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="AB9" s="0" t="n">
+      <c r="AD9" s="0" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>280</v>
@@ -7031,25 +7086,31 @@
         <f aca="false">U10+V10</f>
         <v>2825</v>
       </c>
-      <c r="X10" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>21</v>
+      <c r="X10" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="Z10" s="0" t="n">
         <v>21</v>
       </c>
       <c r="AA10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="AB10" s="0" t="n">
+      <c r="AD10" s="0" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>220</v>
@@ -7122,69 +7183,75 @@
         <f aca="false">U11+V11</f>
         <v>3070</v>
       </c>
-      <c r="AA11" s="0" t="n">
+      <c r="X11" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC11" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="E12" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="G12" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J12" s="2" t="n">
         <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>620</v>
+        <v>1220</v>
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">SUM(B12:E12) + SUM(F12:I12)*2</f>
-        <v>1170</v>
+        <v>2010</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="T12" s="2" t="n">
         <f aca="false">SUM(J12,L12,N12,P12*2,R12*2)</f>
@@ -7192,25 +7259,40 @@
       </c>
       <c r="U12" s="2" t="n">
         <f aca="false">K12+SUM(L12:O12)+SUM(P12:S12)*2</f>
-        <v>3270</v>
+        <v>3210</v>
       </c>
       <c r="V12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W12" s="1" t="n">
         <f aca="false">U12+V12</f>
-        <v>3270</v>
+        <v>3210</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>28</v>
       </c>
       <c r="AA12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC12" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="AB12" s="0" t="n">
+      <c r="AD12" s="0" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>320</v>
@@ -7266,7 +7348,7 @@
         <v>100</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T13" s="2" t="n">
         <f aca="false">SUM(J13,L13,N13,P13*2,R13*2)</f>
@@ -7274,90 +7356,87 @@
       </c>
       <c r="U13" s="2" t="n">
         <f aca="false">K13+SUM(L13:O13)+SUM(P13:S13)*2</f>
-        <v>3210</v>
+        <v>3260</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W13" s="1" t="n">
         <f aca="false">U13+V13</f>
-        <v>3210</v>
-      </c>
-      <c r="X13" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="Y13" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="Z13" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA13" s="0" t="n">
+        <v>3260</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC13" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="AB13" s="0" t="n">
+      <c r="AD13" s="0" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>1220</v>
+        <v>620</v>
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">SUM(B14:E14) + SUM(F14:I14)*2</f>
-        <v>2010</v>
+        <v>1170</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="T14" s="2" t="n">
         <f aca="false">SUM(J14,L14,N14,P14*2,R14*2)</f>
@@ -7365,57 +7444,63 @@
       </c>
       <c r="U14" s="2" t="n">
         <f aca="false">K14+SUM(L14:O14)+SUM(P14:S14)*2</f>
-        <v>3260</v>
+        <v>3270</v>
       </c>
       <c r="V14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W14" s="1" t="n">
         <f aca="false">U14+V14</f>
-        <v>3260</v>
-      </c>
-      <c r="AA14" s="0" t="n">
+        <v>3270</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC14" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="AB14" s="0" t="n">
+      <c r="AD14" s="0" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>245</v>
+        <v>130</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="J15" s="2" t="n">
         <f aca="false">SUM(B15,D15,F15*2,H15*2)</f>
-        <v>1460</v>
+        <v>1375</v>
       </c>
       <c r="K15" s="2" t="n">
         <f aca="false">SUM(B15:E15) + SUM(F15:I15)*2</f>
-        <v>2415</v>
+        <v>1685</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>100</v>
@@ -7443,70 +7528,74 @@
       </c>
       <c r="T15" s="2" t="n">
         <f aca="false">SUM(J15,L15,N15,P15*2,R15*2)</f>
-        <v>2060</v>
+        <v>1975</v>
       </c>
       <c r="U15" s="2" t="n">
         <f aca="false">K15+SUM(L15:O15)+SUM(P15:S15)*2</f>
-        <v>3615</v>
+        <v>2885</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0</v>
+        <f aca="false">(80+20)*6+80</f>
+        <v>680</v>
       </c>
       <c r="W15" s="1" t="n">
         <f aca="false">U15+V15</f>
-        <v>3615</v>
-      </c>
-      <c r="X15" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="Y15" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="Z15" s="0" t="n">
-        <v>35</v>
+        <v>3565</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="AA15" s="0" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="AB15" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>130</v>
+        <v>245</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="J16" s="2" t="n">
         <f aca="false">SUM(B16,D16,F16*2,H16*2)</f>
-        <v>1375</v>
+        <v>1460</v>
       </c>
       <c r="K16" s="2" t="n">
         <f aca="false">SUM(B16:E16) + SUM(F16:I16)*2</f>
-        <v>1685</v>
+        <v>2415</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>100</v>
@@ -7534,68 +7623,76 @@
       </c>
       <c r="T16" s="2" t="n">
         <f aca="false">SUM(J16,L16,N16,P16*2,R16*2)</f>
-        <v>1975</v>
+        <v>2060</v>
       </c>
       <c r="U16" s="2" t="n">
         <f aca="false">K16+SUM(L16:O16)+SUM(P16:S16)*2</f>
-        <v>2885</v>
+        <v>3615</v>
       </c>
       <c r="V16" s="1" t="n">
-        <f aca="false">(80+20)*6+80</f>
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="W16" s="1" t="n">
         <f aca="false">U16+V16</f>
-        <v>3565</v>
-      </c>
-      <c r="Y16" s="0" t="n">
-        <v>42</v>
+        <v>3615</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="Z16" s="0" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AA16" s="0" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="J17" s="2" t="n">
         <f aca="false">SUM(B17,D17,F17*2,H17*2)</f>
-        <v>1820</v>
+        <v>1860</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">SUM(B17:E17) + SUM(F17:I17)*2</f>
-        <v>2810</v>
+        <v>2650</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>100</v>
@@ -7623,67 +7720,70 @@
       </c>
       <c r="T17" s="2" t="n">
         <f aca="false">SUM(J17,L17,N17,P17*2,R17*2)</f>
-        <v>2420</v>
+        <v>2460</v>
       </c>
       <c r="U17" s="2" t="n">
         <f aca="false">K17+SUM(L17:O17)+SUM(P17:S17)*2</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="V17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="1" t="n">
         <f aca="false">U17+V17</f>
-        <v>4010</v>
-      </c>
-      <c r="Y17" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="Z17" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AA17" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="AB17" s="0" t="n">
+        <v>3850</v>
+      </c>
+      <c r="X17" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD17" s="0" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="J18" s="2" t="n">
         <f aca="false">SUM(B18,D18,F18*2,H18*2)</f>
-        <v>1860</v>
+        <v>1820</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">SUM(B18:E18) + SUM(F18:I18)*2</f>
-        <v>2650</v>
+        <v>2810</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>100</v>
@@ -7711,31 +7811,40 @@
       </c>
       <c r="T18" s="2" t="n">
         <f aca="false">SUM(J18,L18,N18,P18*2,R18*2)</f>
-        <v>2460</v>
+        <v>2420</v>
       </c>
       <c r="U18" s="2" t="n">
         <f aca="false">K18+SUM(L18:O18)+SUM(P18:S18)*2</f>
-        <v>3850</v>
+        <v>4010</v>
       </c>
       <c r="V18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="1" t="n">
         <f aca="false">U18+V18</f>
-        <v>3850</v>
-      </c>
-      <c r="Z18" s="10" t="s">
-        <v>29</v>
+        <v>4010</v>
+      </c>
+      <c r="X18" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="AA18" s="0" t="n">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AB18" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="AC18" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -7756,6 +7865,8 @@
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <conditionalFormatting sqref="W2:W1048576">
     <cfRule type="dataBar" priority="2">
@@ -7766,12 +7877,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2B72F2EF-BEAA-45C4-865C-F070986BCB98}</x14:id>
+          <x14:id>{42B7EBE7-9240-44F1-8646-66786D1B1FA5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:AB1048576">
+  <conditionalFormatting sqref="Z2:AD1048576">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -7780,7 +7891,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D0DCC653-1359-475F-839A-CB50F6F5ADC9}</x14:id>
+          <x14:id>{38AC5490-4DDF-4FD6-A860-E84DEB00AE3F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7794,7 +7905,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C89F9979-8BC0-43CC-81AE-587772006BFC}</x14:id>
+          <x14:id>{1BD270BF-36D9-43DB-8AA0-34D4E16A6D37}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7808,7 +7919,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7957E487-5D7E-47C5-AD22-56584751AAA7}</x14:id>
+          <x14:id>{295014CC-70F0-44C0-B363-498B5A4C7B61}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7825,7 +7936,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2B72F2EF-BEAA-45C4-865C-F070986BCB98}">
+          <x14:cfRule type="dataBar" id="{42B7EBE7-9240-44F1-8646-66786D1B1FA5}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7836,7 +7947,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D0DCC653-1359-475F-839A-CB50F6F5ADC9}">
+          <x14:cfRule type="dataBar" id="{38AC5490-4DDF-4FD6-A860-E84DEB00AE3F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7844,10 +7955,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>X2:AB1048576</xm:sqref>
+          <xm:sqref>Z2:AD1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C89F9979-8BC0-43CC-81AE-587772006BFC}">
+          <x14:cfRule type="dataBar" id="{1BD270BF-36D9-43DB-8AA0-34D4E16A6D37}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7858,7 +7969,7 @@
           <xm:sqref>T2:T1048576 U2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7957E487-5D7E-47C5-AD22-56584751AAA7}">
+          <x14:cfRule type="dataBar" id="{295014CC-70F0-44C0-B363-498B5A4C7B61}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7896,40 +8007,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,7 +8060,7 @@
         <f aca="false">220+(2*70)+(2*70)+120</f>
         <v>620</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="12" t="n">
         <f aca="false">220+(2*70)+(2*70)+120</f>
         <v>620</v>
       </c>
@@ -7962,7 +8073,7 @@
         <v>620</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7976,7 +8087,7 @@
         <f aca="false">220+(2*70)+(2*70)+120</f>
         <v>620</v>
       </c>
-      <c r="I3" s="11" t="n">
+      <c r="I3" s="12" t="n">
         <f aca="false">220+(4*82)+122</f>
         <v>670</v>
       </c>
@@ -8002,7 +8113,7 @@
         <f aca="false">240+(2*90)+(2*90)+140</f>
         <v>740</v>
       </c>
-      <c r="I4" s="11" t="n">
+      <c r="I4" s="12" t="n">
         <f aca="false">240+(4*102)+142</f>
         <v>790</v>
       </c>
@@ -8014,7 +8125,7 @@
         <v>740</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8028,7 +8139,7 @@
         <f aca="false">240+(2*90)+(2*90)+140</f>
         <v>740</v>
       </c>
-      <c r="I5" s="11" t="n">
+      <c r="I5" s="12" t="n">
         <f aca="false">240+(4*122)+162</f>
         <v>890</v>
       </c>
@@ -8065,7 +8176,7 @@
         <v>980</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8091,7 +8202,7 @@
         <v>980</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8102,7 +8213,7 @@
         <f aca="false">320+220+(4*210)</f>
         <v>1380</v>
       </c>
-      <c r="I8" s="11" t="n">
+      <c r="I8" s="12" t="n">
         <f aca="false">230+220+(4*210)</f>
         <v>1290</v>
       </c>
@@ -8114,7 +8225,7 @@
         <v>980</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8137,59 +8248,59 @@
         <v>980</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -8225,43 +8336,43 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8444,7 +8555,7 @@
       <c r="F8" s="8" t="n">
         <v>1700</v>
       </c>
-      <c r="G8" s="11" t="n">
+      <c r="G8" s="12" t="n">
         <v>1580</v>
       </c>
       <c r="H8" s="0" t="n">
@@ -8563,7 +8674,7 @@
       <c r="A13" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="K13" s="11" t="n">
+      <c r="K13" s="12" t="n">
         <v>2220</v>
       </c>
       <c r="L13" s="0" t="n">
@@ -8590,72 +8701,72 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="B18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="0" t="s">
+      <c r="I18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="K18" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -8689,13 +8800,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8760,18 +8871,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -8806,50 +8917,50 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="14" t="n">
         <v>860</v>
       </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="14" t="n">
         <v>860</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -8864,10 +8975,10 @@
       <c r="A3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="14" t="n">
         <v>1100</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="14" t="n">
         <v>980</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -8882,8 +8993,8 @@
       <c r="A4" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="n">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="n">
         <v>1100</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -8904,8 +9015,8 @@
       <c r="A5" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="n">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14" t="n">
         <v>1220</v>
       </c>
       <c r="I5" s="0" t="n">
@@ -8920,8 +9031,8 @@
       <c r="A6" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="n">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="n">
         <v>1340</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -8936,8 +9047,8 @@
       <c r="A7" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
       <c r="K7" s="0" t="n">
         <v>2220</v>
       </c>
@@ -8950,8 +9061,8 @@
       <c r="A8" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="L8" s="0" t="n">
         <f aca="false">MAX(B8:K8, L7)</f>
         <v>2220</v>
@@ -8961,8 +9072,8 @@
       <c r="A9" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="L9" s="0" t="n">
         <f aca="false">MAX(B9:K9, L8)</f>
         <v>2220</v>
@@ -8972,8 +9083,8 @@
       <c r="A10" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="L10" s="0" t="n">
         <f aca="false">MAX(B10:K10, L9)</f>
         <v>2220</v>
@@ -8983,9 +9094,9 @@
       <c r="A11" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="K11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="0" t="n">
         <f aca="false">MAX(B11:K11, L10)</f>
         <v>2220</v>
@@ -8995,8 +9106,8 @@
       <c r="A12" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="L12" s="0" t="n">
         <f aca="false">MAX(B12:K12, L11)</f>
         <v>2220</v>
@@ -9006,85 +9117,85 @@
       <c r="A13" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="L13" s="0" t="n">
         <f aca="false">MAX(B13:K13, L12)</f>
         <v>2220</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="K17" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9123,25 +9234,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Midwest Power Armor Evolution to balance spreadsheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,6 +37,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This changes drastically if Raider Overhaul is installed, becoming much stronger</t>
         </r>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="83">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -166,6 +167,9 @@
     <t xml:space="preserve">Armorer 4 + Science 4 + Nuclear Physicist 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Midwest Evolution</t>
+  </si>
+  <si>
     <t xml:space="preserve">X-01</t>
   </si>
   <si>
@@ -258,6 +262,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">F + </t>
     </r>
@@ -267,6 +272,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tesla</t>
     </r>
@@ -277,6 +283,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E + </t>
     </r>
@@ -286,12 +293,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tesla</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">I-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midwest Evo</t>
   </si>
   <si>
     <t xml:space="preserve">Knight:</t>
@@ -332,11 +343,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -359,16 +371,23 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -443,7 +462,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,7 +471,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -464,7 +483,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,10 +493,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -520,7 +535,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 3" xfId="20"/>
+    <cellStyle name="Accent 3 1" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -585,7 +600,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart281.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1568,10 +1583,10 @@
                   <c:v>1430</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1770</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2220</c:v>
+                  <c:v>1585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,11 +1601,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="27331801"/>
-        <c:axId val="95526515"/>
+        <c:axId val="25285640"/>
+        <c:axId val="42246117"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27331801"/>
+        <c:axId val="25285640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95526515"/>
+        <c:crossAx val="42246117"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95526515"/>
+        <c:axId val="42246117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1684,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27331801"/>
+        <c:crossAx val="25285640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1720,7 +1735,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart282.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3080,11 +3095,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="69415773"/>
-        <c:axId val="24139525"/>
+        <c:axId val="6216252"/>
+        <c:axId val="47799085"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69415773"/>
+        <c:axId val="6216252"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3115,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24139525"/>
+        <c:crossAx val="47799085"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3123,7 +3138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24139525"/>
+        <c:axId val="47799085"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,7 +3178,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69415773"/>
+        <c:crossAx val="6216252"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3211,7 +3226,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart283.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3347,11 +3362,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="44113594"/>
-        <c:axId val="82261013"/>
+        <c:axId val="13062684"/>
+        <c:axId val="65366029"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44113594"/>
+        <c:axId val="13062684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3382,7 +3397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82261013"/>
+        <c:crossAx val="65366029"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3390,7 +3405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82261013"/>
+        <c:axId val="65366029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3430,7 +3445,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44113594"/>
+        <c:crossAx val="13062684"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3481,7 +3496,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart284.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3553,9 +3568,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3563,36 +3578,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3600,10 +3618,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$B$2:$B$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>930</c:v>
                 </c:pt>
@@ -3611,6 +3629,9 @@
                   <c:v>1770</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1770</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2010</c:v>
                 </c:pt>
               </c:numCache>
@@ -3680,9 +3701,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3690,36 +3711,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3727,10 +3751,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$C$2:$C$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1470</c:v>
                 </c:pt>
@@ -3738,15 +3762,18 @@
                   <c:v>1710</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1950</c:v>
+                  <c:v>1710</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1950</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2190</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2430</c:v>
                 </c:pt>
               </c:numCache>
@@ -3816,9 +3843,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3826,36 +3853,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3863,10 +3893,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$D$2:$D$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2370</c:v>
                 </c:pt>
@@ -3937,9 +3967,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3947,36 +3977,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3984,10 +4017,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$E$2:$E$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2345</c:v>
                 </c:pt>
@@ -4005,7 +4038,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-01</c:v>
+                  <c:v>Midwest Evo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4058,9 +4091,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4068,36 +4101,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4105,12 +4141,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$F$2:$F$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="2">
-                  <c:v>2730</c:v>
+                  <c:v>2610</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4126,7 +4162,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X-02 (CC)</c:v>
+                  <c:v>X-01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4179,9 +4215,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4189,36 +4225,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4226,12 +4265,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$G$2:$G$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="2">
-                  <c:v>2760</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="3">
+                  <c:v>2730</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4300,9 +4339,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4310,36 +4349,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4347,11 +4389,11 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$H$2:$H$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$H$2:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="2">
+                <c:ptCount val="14"/>
+                <c:pt idx="3">
                   <c:v>2850</c:v>
                 </c:pt>
               </c:numCache>
@@ -4421,9 +4463,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4431,36 +4473,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4468,11 +4513,11 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$I$2:$I$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$I$2:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="2">
+                <c:ptCount val="14"/>
+                <c:pt idx="3">
                   <c:v>2885</c:v>
                 </c:pt>
               </c:numCache>
@@ -4542,9 +4587,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4552,36 +4597,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4589,11 +4637,11 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$J$2:$J$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$J$2:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="3">
+                <c:ptCount val="14"/>
+                <c:pt idx="4">
                   <c:v>3135</c:v>
                 </c:pt>
               </c:numCache>
@@ -4663,9 +4711,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4673,36 +4721,39 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>74</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4710,11 +4761,11 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leveled Power Increase - BoS'!$K$2:$K$14</c:f>
+              <c:f>'Leveled Power Increase - BoS'!$K$2:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="5">
+                <c:ptCount val="14"/>
+                <c:pt idx="6">
                   <c:v>3610</c:v>
                 </c:pt>
               </c:numCache>
@@ -4730,11 +4781,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17404178"/>
-        <c:axId val="91379182"/>
+        <c:axId val="14386699"/>
+        <c:axId val="62027942"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17404178"/>
+        <c:axId val="14386699"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4765,7 +4816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91379182"/>
+        <c:crossAx val="62027942"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4773,7 +4824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91379182"/>
+        <c:axId val="62027942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4813,7 +4864,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17404178"/>
+        <c:crossAx val="14386699"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4864,7 +4915,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart285.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5812,11 +5863,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="10915368"/>
-        <c:axId val="95743792"/>
+        <c:axId val="88742590"/>
+        <c:axId val="63376310"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10915368"/>
+        <c:axId val="88742590"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5881,7 +5932,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95743792"/>
+        <c:crossAx val="63376310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5889,7 +5940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95743792"/>
+        <c:axId val="63376310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5963,7 +6014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10915368"/>
+        <c:crossAx val="88742590"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6025,9 +6076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>281880</xdr:colOff>
+      <xdr:colOff>281520</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6036,7 +6087,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732040"/>
-        <a:ext cx="7637400" cy="4273200"/>
+        <a:ext cx="7646040" cy="4272840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6060,9 +6111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>39960</xdr:colOff>
+      <xdr:colOff>39600</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6071,7 +6122,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216240"/>
-        <a:ext cx="10200240" cy="4273200"/>
+        <a:ext cx="10211400" cy="4272840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6095,9 +6146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514440</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6106,7 +6157,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7641360" cy="4273200"/>
+        <a:ext cx="7651080" cy="4272840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6125,13 +6176,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>468720</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1164600</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:colOff>1164240</xdr:colOff>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -6140,8 +6191,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="468720" y="3053520"/>
-        <a:ext cx="10200240" cy="4273200"/>
+        <a:off x="468720" y="3216240"/>
+        <a:ext cx="10211400" cy="4272840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6165,9 +6216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6176,7 +6227,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2631960"/>
-        <a:ext cx="8408520" cy="4711320"/>
+        <a:ext cx="8411760" cy="4710960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6194,17 +6245,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE18"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD13" activeCellId="0" sqref="AD13"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -6216,7 +6267,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.83"/>
@@ -6232,10 +6283,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="49.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="49.8"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6310,60 +6361,60 @@
       <c r="AD1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="true" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="T2" s="5"/>
@@ -6377,7 +6428,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
-      <c r="AE2" s="8"/>
+      <c r="AE2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -6469,7 +6520,7 @@
       <c r="AD3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AE3" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6560,7 +6611,7 @@
       <c r="AD4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AE4" s="11"/>
+      <c r="AE4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -6658,7 +6709,7 @@
       <c r="AD5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AE5" s="11"/>
+      <c r="AE5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -6756,7 +6807,7 @@
       <c r="AD6" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="AE6" s="11"/>
+      <c r="AE6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -6845,7 +6896,7 @@
       <c r="AD7" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="AE7" s="11"/>
+      <c r="AE7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -6937,7 +6988,7 @@
       <c r="AD8" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="AE8" s="11"/>
+      <c r="AE8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -7035,7 +7086,7 @@
       <c r="AD9" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="AE9" s="11" t="s">
+      <c r="AE9" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7123,7 +7174,7 @@
       <c r="AC10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="AE10" s="11"/>
+      <c r="AE10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -7203,7 +7254,7 @@
       <c r="X11" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="Y11" s="12" t="s">
+      <c r="Y11" s="11" t="s">
         <v>38</v>
       </c>
       <c r="AA11" s="0" t="n">
@@ -7218,43 +7269,43 @@
       <c r="AD11" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="AE11" s="11"/>
+      <c r="AE11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>140</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>110</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>110</v>
       </c>
       <c r="J12" s="2" t="n">
         <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>1220</v>
+        <v>1100</v>
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">SUM(B12:E12) + SUM(F12:I12)*2</f>
-        <v>2010</v>
+        <v>1890</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>100</v>
@@ -7282,18 +7333,18 @@
       </c>
       <c r="T12" s="2" t="n">
         <f aca="false">SUM(J12,L12,N12,P12*2,R12*2)</f>
-        <v>1820</v>
+        <v>1700</v>
       </c>
       <c r="U12" s="2" t="n">
         <f aca="false">K12+SUM(L12:O12)+SUM(P12:S12)*2</f>
-        <v>3210</v>
+        <v>3090</v>
       </c>
       <c r="V12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W12" s="1" t="n">
         <f aca="false">U12+V12</f>
-        <v>3210</v>
+        <v>3090</v>
       </c>
       <c r="X12" s="1" t="n">
         <v>39</v>
@@ -7301,22 +7352,15 @@
       <c r="Y12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z12" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA12" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AB12" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AC12" s="0" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE12" s="11"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -7376,7 +7420,7 @@
         <v>100</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="T13" s="2" t="n">
         <f aca="false">SUM(J13,L13,N13,P13*2,R13*2)</f>
@@ -7384,14 +7428,14 @@
       </c>
       <c r="U13" s="2" t="n">
         <f aca="false">K13+SUM(L13:O13)+SUM(P13:S13)*2</f>
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W13" s="1" t="n">
         <f aca="false">U13+V13</f>
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="X13" s="1" t="n">
         <v>39</v>
@@ -7399,73 +7443,82 @@
       <c r="Y13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="Z13" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="AC13" s="0" t="n">
         <v>32</v>
       </c>
       <c r="AD13" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="AE13" s="11"/>
+      <c r="AE13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="E14" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="G14" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>620</v>
+        <v>1220</v>
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">SUM(B14:E14) + SUM(F14:I14)*2</f>
-        <v>1170</v>
+        <v>2010</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="T14" s="2" t="n">
         <f aca="false">SUM(J14,L14,N14,P14*2,R14*2)</f>
@@ -7473,14 +7526,14 @@
       </c>
       <c r="U14" s="2" t="n">
         <f aca="false">K14+SUM(L14:O14)+SUM(P14:S14)*2</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="V14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W14" s="1" t="n">
         <f aca="false">U14+V14</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="X14" s="1" t="n">
         <v>39</v>
@@ -7494,239 +7547,230 @@
       <c r="AD14" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="AE14" s="11"/>
+      <c r="AE14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>380</v>
+        <v>220</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="J15" s="2" t="n">
         <f aca="false">SUM(B15,D15,F15*2,H15*2)</f>
-        <v>1375</v>
+        <v>620</v>
       </c>
       <c r="K15" s="2" t="n">
         <f aca="false">SUM(B15:E15) + SUM(F15:I15)*2</f>
-        <v>1685</v>
+        <v>1170</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R15" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="T15" s="2" t="n">
         <f aca="false">SUM(J15,L15,N15,P15*2,R15*2)</f>
-        <v>1975</v>
+        <v>1820</v>
       </c>
       <c r="U15" s="2" t="n">
         <f aca="false">K15+SUM(L15:O15)+SUM(P15:S15)*2</f>
+        <v>3270</v>
+      </c>
+      <c r="V15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <f aca="false">U15+V15</f>
+        <v>3270</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <f aca="false">SUM(B16,D16,F16*2,H16*2)</f>
+        <v>1375</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <f aca="false">SUM(B16:E16) + SUM(F16:I16)*2</f>
+        <v>1685</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <f aca="false">SUM(J16,L16,N16,P16*2,R16*2)</f>
+        <v>1975</v>
+      </c>
+      <c r="U16" s="2" t="n">
+        <f aca="false">K16+SUM(L16:O16)+SUM(P16:S16)*2</f>
         <v>2885</v>
       </c>
-      <c r="V15" s="1" t="n">
+      <c r="V16" s="1" t="n">
         <f aca="false">(80+20)*6+80</f>
         <v>680</v>
       </c>
-      <c r="W15" s="1" t="n">
-        <f aca="false">U15+V15</f>
-        <v>3565</v>
-      </c>
-      <c r="X15" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="Y15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA15" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AB15" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC15" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="AD15" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE15" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>245</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>260</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="J16" s="2" t="n">
-        <f aca="false">SUM(B16,D16,F16*2,H16*2)</f>
-        <v>1460</v>
-      </c>
-      <c r="K16" s="2" t="n">
-        <f aca="false">SUM(B16:E16) + SUM(F16:I16)*2</f>
-        <v>2415</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="O16" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q16" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="R16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S16" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T16" s="2" t="n">
-        <f aca="false">SUM(J16,L16,N16,P16*2,R16*2)</f>
-        <v>2060</v>
-      </c>
-      <c r="U16" s="2" t="n">
-        <f aca="false">K16+SUM(L16:O16)+SUM(P16:S16)*2</f>
-        <v>3615</v>
-      </c>
-      <c r="V16" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W16" s="1" t="n">
         <f aca="false">U16+V16</f>
-        <v>3615</v>
+        <v>3565</v>
       </c>
       <c r="X16" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z16" s="0" t="n">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="AA16" s="0" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AC16" s="0" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="AD16" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AE16" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="AE16" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>500</v>
+        <v>360</v>
       </c>
       <c r="C17" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>210</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E17" s="1" t="n">
+      <c r="G17" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>290</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>110</v>
-      </c>
       <c r="H17" s="0" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="J17" s="2" t="n">
         <f aca="false">SUM(B17,D17,F17*2,H17*2)</f>
-        <v>1860</v>
+        <v>1460</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">SUM(B17:E17) + SUM(F17:I17)*2</f>
-        <v>2650</v>
+        <v>2415</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>100</v>
@@ -7754,18 +7798,18 @@
       </c>
       <c r="T17" s="2" t="n">
         <f aca="false">SUM(J17,L17,N17,P17*2,R17*2)</f>
-        <v>2460</v>
+        <v>2060</v>
       </c>
       <c r="U17" s="2" t="n">
         <f aca="false">K17+SUM(L17:O17)+SUM(P17:S17)*2</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="V17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="1" t="n">
         <f aca="false">U17+V17</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="X17" s="1" t="n">
         <v>39</v>
@@ -7773,54 +7817,58 @@
       <c r="Y17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB17" s="11" t="s">
-        <v>33</v>
+      <c r="Z17" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>35</v>
       </c>
       <c r="AC17" s="0" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AD17" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AE17" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="AE17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="J18" s="2" t="n">
         <f aca="false">SUM(B18,D18,F18*2,H18*2)</f>
-        <v>1820</v>
+        <v>1860</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">SUM(B18:E18) + SUM(F18:I18)*2</f>
-        <v>2810</v>
+        <v>2650</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>100</v>
@@ -7848,18 +7896,18 @@
       </c>
       <c r="T18" s="2" t="n">
         <f aca="false">SUM(J18,L18,N18,P18*2,R18*2)</f>
-        <v>2420</v>
+        <v>2460</v>
       </c>
       <c r="U18" s="2" t="n">
         <f aca="false">K18+SUM(L18:O18)+SUM(P18:S18)*2</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="V18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="1" t="n">
         <f aca="false">U18+V18</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="X18" s="1" t="n">
         <v>39</v>
@@ -7867,11 +7915,8 @@
       <c r="Y18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA18" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AB18" s="0" t="n">
-        <v>42</v>
+      <c r="AB18" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="AC18" s="0" t="n">
         <v>46</v>
@@ -7879,7 +7924,104 @@
       <c r="AD18" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="AE18" s="11"/>
+      <c r="AE18" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <f aca="false">SUM(B19,D19,F19*2,H19*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <f aca="false">SUM(B19:E19) + SUM(F19:I19)*2</f>
+        <v>2810</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T19" s="2" t="n">
+        <f aca="false">SUM(J19,L19,N19,P19*2,R19*2)</f>
+        <v>2420</v>
+      </c>
+      <c r="U19" s="2" t="n">
+        <f aca="false">K19+SUM(L19:O19)+SUM(P19:S19)*2</f>
+        <v>4010</v>
+      </c>
+      <c r="V19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1" t="n">
+        <f aca="false">U19+V19</f>
+        <v>4010</v>
+      </c>
+      <c r="X19" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC19" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD19" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AE19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -7916,7 +8058,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{647D50E5-EAB6-4F9F-92F0-B0FDBE93A994}</x14:id>
+          <x14:id>{76B0DD9A-A255-4D8E-9B54-30247851BEE2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7930,7 +8072,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A1D5B07B-FD9F-4247-813F-7312224FED57}</x14:id>
+          <x14:id>{6B547010-7970-4BE7-A0FD-424E1578FFB7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7944,7 +8086,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{47634BCD-EE7E-4C7A-B9D4-D988F66FA327}</x14:id>
+          <x14:id>{133CF4C4-A090-4A30-A6A9-873AB812D7B7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7958,7 +8100,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F74D1F8E-A048-448C-9AF6-8300108DD0B6}</x14:id>
+          <x14:id>{853FA494-BE72-4A94-A51C-95B8BBE09290}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7975,7 +8117,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{647D50E5-EAB6-4F9F-92F0-B0FDBE93A994}">
+          <x14:cfRule type="dataBar" id="{76B0DD9A-A255-4D8E-9B54-30247851BEE2}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7986,7 +8128,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A1D5B07B-FD9F-4247-813F-7312224FED57}">
+          <x14:cfRule type="dataBar" id="{6B547010-7970-4BE7-A0FD-424E1578FFB7}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -7997,7 +8139,7 @@
           <xm:sqref>Z2:AD1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{47634BCD-EE7E-4C7A-B9D4-D988F66FA327}">
+          <x14:cfRule type="dataBar" id="{133CF4C4-A090-4A30-A6A9-873AB812D7B7}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8008,7 +8150,7 @@
           <xm:sqref>T2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F74D1F8E-A048-448C-9AF6-8300108DD0B6}">
+          <x14:cfRule type="dataBar" id="{853FA494-BE72-4A94-A51C-95B8BBE09290}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8035,7 +8177,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.83"/>
@@ -8045,41 +8187,41 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>54</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8098,7 +8240,7 @@
       <c r="H2" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I2" s="13" t="n">
+      <c r="I2" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B2-570)/6</f>
         <v>690</v>
       </c>
@@ -8111,7 +8253,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8124,7 +8266,7 @@
       <c r="H3" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I3" s="13" t="n">
+      <c r="I3" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B3-570)/6</f>
         <v>730</v>
       </c>
@@ -8149,7 +8291,7 @@
       <c r="H4" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B4-570)/6</f>
         <v>1050</v>
       </c>
@@ -8174,7 +8316,7 @@
       <c r="H5" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B5-570)/6</f>
         <v>1090</v>
       </c>
@@ -8200,7 +8342,7 @@
         <f aca="false">F6</f>
         <v>1625</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I6" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B6-570)/6</f>
         <v>1390</v>
       </c>
@@ -8212,7 +8354,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8225,7 +8367,7 @@
       <c r="H7" s="0" t="n">
         <v>1625</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I7" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B7-570)/6</f>
         <v>1430</v>
       </c>
@@ -8251,9 +8393,9 @@
         <f aca="false">G8</f>
         <v>2010</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$13:$E$13)+(2*SUM('Power Armor Sets'!$F$13:$G$13))+(2*SUM('Power Armor Sets'!$H$15:$I$15))+($B8-570)/6</f>
-        <v>1770</v>
+        <v>1610</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">MAX(B8:I8)</f>
@@ -8263,7 +8405,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8277,9 +8419,9 @@
         <f aca="false">G8+270</f>
         <v>2280</v>
       </c>
-      <c r="I9" s="13" t="n">
+      <c r="I9" s="12" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$16:$E$16)+(2*SUM('Power Armor Sets'!$F$16:$G$16))+(2*SUM('Power Armor Sets'!$H$16:$I$16))+($B9-570)/6</f>
-        <v>2220</v>
+        <v>1585</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">MAX(B9:I9)</f>
@@ -8289,62 +8431,62 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="13"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>59</v>
+      <c r="A13" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -8370,7 +8512,7 @@
       <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
@@ -8378,45 +8520,45 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.12"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>53</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -8579,10 +8721,10 @@
       <c r="A7" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="8" t="n">
         <v>2970</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="8" t="n">
         <v>2970</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -8685,7 +8827,7 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="K12" s="13"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="0" t="n">
         <f aca="false">MAX(B12:K12, L11)</f>
         <v>3530</v>
@@ -8709,73 +8851,73 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>59</v>
+      <c r="A16" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>61</v>
+      <c r="A17" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -8801,21 +8943,21 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>52</v>
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8879,19 +9021,19 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>59</v>
+      <c r="A10" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>61</v>
+      <c r="A11" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -8911,65 +9053,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.55"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>52</v>
+      <c r="K1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="14" t="n">
         <v>930</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="14" t="n">
         <v>1470</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -8987,10 +9129,10 @@
       <c r="A3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="14" t="n">
         <v>1770</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="14" t="n">
         <v>1710</v>
       </c>
       <c r="L3" s="0" t="n">
@@ -9000,54 +9142,56 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B4" s="15" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C4" s="15" t="n">
-        <v>1950</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="14" t="n">
+        <v>1770</v>
+      </c>
+      <c r="C4" s="14" t="n">
+        <v>1710</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2730</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>2760</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>2850</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>2885</v>
+        <v>2610</v>
       </c>
       <c r="L4" s="0" t="n">
         <f aca="false">MAX(B4:K4, L3)</f>
-        <v>2885</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15" t="n">
+        <v>32</v>
+      </c>
+      <c r="B5" s="14" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C5" s="14" t="n">
         <v>1950</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>3135</v>
+      <c r="G5" s="0" t="n">
+        <v>2730</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2850</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>2885</v>
       </c>
       <c r="L5" s="0" t="n">
-        <f aca="false">MAX(B5:K5, L4)</f>
-        <v>3135</v>
+        <f aca="false">MAX(B5:K5, L3)</f>
+        <v>2885</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="n">
-        <v>2190</v>
+        <v>39</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="n">
+        <v>1950</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>3135</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">MAX(B6:K6, L5)</f>
@@ -9056,26 +9200,28 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="n">
-        <v>2430</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>3610</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="n">
+        <v>2190</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">MAX(B7:K7, L6)</f>
-        <v>3610</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="n">
+        <v>2430</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>3610</v>
+      </c>
       <c r="L8" s="0" t="n">
         <f aca="false">MAX(B8:K8, L7)</f>
         <v>3610</v>
@@ -9083,10 +9229,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>67</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="L9" s="0" t="n">
         <f aca="false">MAX(B9:K9, L8)</f>
         <v>3610</v>
@@ -9094,10 +9240,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>74</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="L10" s="0" t="n">
         <f aca="false">MAX(B10:K10, L9)</f>
         <v>3610</v>
@@ -9105,11 +9251,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>81</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="K11" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="L11" s="0" t="n">
         <f aca="false">MAX(B11:K11, L10)</f>
         <v>3610</v>
@@ -9117,10 +9262,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>88</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="0" t="n">
         <f aca="false">MAX(B12:K12, L11)</f>
         <v>3610</v>
@@ -9128,91 +9274,108 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+        <v>88</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="L13" s="0" t="n">
         <f aca="false">MAX(B13:K13, L12)</f>
         <v>3610</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="L14" s="0" t="n">
+        <f aca="false">MAX(B14:K14, L13)</f>
+        <v>3610</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>66</v>
-      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>72</v>
+      <c r="B16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>72</v>
+      <c r="C17" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="16"/>
+      <c r="A18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -9236,7 +9399,7 @@
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
@@ -9246,26 +9409,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>80</v>
+      <c r="G1" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9281,7 +9444,7 @@
         <v>870</v>
       </c>
       <c r="G2" s="0" t="n">
-        <f aca="false">VLOOKUP($A2, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A2, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>2370</v>
       </c>
     </row>
@@ -9306,7 +9469,7 @@
         <v>1470</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A3, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>2370</v>
       </c>
     </row>
@@ -9335,7 +9498,7 @@
         <v>1605</v>
       </c>
       <c r="G4" s="0" t="n">
-        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A4, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>2370</v>
       </c>
     </row>
@@ -9364,7 +9527,7 @@
         <v>2005</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A5, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>2885</v>
       </c>
     </row>
@@ -9393,7 +9556,7 @@
         <v>2405</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A6, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3135</v>
       </c>
     </row>
@@ -9422,7 +9585,7 @@
         <v>2405</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A7, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3135</v>
       </c>
     </row>
@@ -9451,7 +9614,7 @@
         <v>2405</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A8, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9480,7 +9643,7 @@
         <v>2405</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A9, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9509,7 +9672,7 @@
         <v>2405</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A10, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9538,7 +9701,7 @@
         <v>2405</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A11, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9567,7 +9730,7 @@
         <v>2405</v>
       </c>
       <c r="G12" s="0" t="n">
-        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A12, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9596,7 +9759,7 @@
         <v>2405</v>
       </c>
       <c r="G13" s="0" t="n">
-        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A13, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>
@@ -9625,7 +9788,7 @@
         <v>2405</v>
       </c>
       <c r="G14" s="0" t="n">
-        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - BoS'!$A$2:$L$14, 12, 1)</f>
+        <f aca="false">VLOOKUP($A14, 'Leveled Power Increase - BoS'!$A$2:$L$15, 12, 1)</f>
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Midwest Power Armor Evolution as a legendary drop
Adjust level it's available as a legendary so it doesn't have fewer levels it's available in its tier
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -600,7 +600,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1601,11 +1601,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="25285640"/>
-        <c:axId val="42246117"/>
+        <c:axId val="10608517"/>
+        <c:axId val="74957088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25285640"/>
+        <c:axId val="10608517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42246117"/>
+        <c:crossAx val="74957088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1644,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42246117"/>
+        <c:axId val="74957088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,7 +1684,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25285640"/>
+        <c:crossAx val="10608517"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1735,7 +1735,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3095,11 +3095,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="6216252"/>
-        <c:axId val="47799085"/>
+        <c:axId val="48180507"/>
+        <c:axId val="73488421"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6216252"/>
+        <c:axId val="48180507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47799085"/>
+        <c:crossAx val="73488421"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47799085"/>
+        <c:axId val="73488421"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3178,7 +3178,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6216252"/>
+        <c:crossAx val="48180507"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3226,7 +3226,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3362,11 +3362,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="13062684"/>
-        <c:axId val="65366029"/>
+        <c:axId val="5571946"/>
+        <c:axId val="73340402"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13062684"/>
+        <c:axId val="5571946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3397,7 +3397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65366029"/>
+        <c:crossAx val="73340402"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3405,7 +3405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65366029"/>
+        <c:axId val="73340402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3445,7 +3445,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13062684"/>
+        <c:crossAx val="5571946"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3496,7 +3496,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4781,11 +4781,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="14386699"/>
-        <c:axId val="62027942"/>
+        <c:axId val="62990108"/>
+        <c:axId val="61199886"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14386699"/>
+        <c:axId val="62990108"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4816,7 +4816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62027942"/>
+        <c:crossAx val="61199886"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4824,7 +4824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62027942"/>
+        <c:axId val="61199886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4864,7 +4864,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14386699"/>
+        <c:crossAx val="62990108"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4915,7 +4915,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5863,11 +5863,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="88742590"/>
-        <c:axId val="63376310"/>
+        <c:axId val="33055427"/>
+        <c:axId val="15323346"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88742590"/>
+        <c:axId val="33055427"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5932,7 +5932,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63376310"/>
+        <c:crossAx val="15323346"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5940,7 +5940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63376310"/>
+        <c:axId val="15323346"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6014,7 +6014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88742590"/>
+        <c:crossAx val="33055427"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6252,7 +6252,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="AD13" activeCellId="0" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7359,7 +7359,7 @@
         <v>29</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8058,7 +8058,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{76B0DD9A-A255-4D8E-9B54-30247851BEE2}</x14:id>
+          <x14:id>{DE6823E1-E899-4DD2-B224-73EB5DC2B96A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8072,7 +8072,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6B547010-7970-4BE7-A0FD-424E1578FFB7}</x14:id>
+          <x14:id>{3039251F-7312-4886-AFB9-D0E3007ECF31}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8086,7 +8086,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{133CF4C4-A090-4A30-A6A9-873AB812D7B7}</x14:id>
+          <x14:id>{823F38E4-C062-4E87-8D60-E7D03FC08E10}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8100,7 +8100,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{853FA494-BE72-4A94-A51C-95B8BBE09290}</x14:id>
+          <x14:id>{92C86ADD-DCC5-415A-B2E0-34F8E856BF51}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8117,7 +8117,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{76B0DD9A-A255-4D8E-9B54-30247851BEE2}">
+          <x14:cfRule type="dataBar" id="{DE6823E1-E899-4DD2-B224-73EB5DC2B96A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8128,7 +8128,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6B547010-7970-4BE7-A0FD-424E1578FFB7}">
+          <x14:cfRule type="dataBar" id="{3039251F-7312-4886-AFB9-D0E3007ECF31}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8139,7 +8139,7 @@
           <xm:sqref>Z2:AD1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{133CF4C4-A090-4A30-A6A9-873AB812D7B7}">
+          <x14:cfRule type="dataBar" id="{823F38E4-C062-4E87-8D60-E7D03FC08E10}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8150,7 +8150,7 @@
           <xm:sqref>T2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{853FA494-BE72-4A94-A51C-95B8BBE09290}">
+          <x14:cfRule type="dataBar" id="{92C86ADD-DCC5-415A-B2E0-34F8E856BF51}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Add balancing data for all power armor sets in the repair patcher
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -222,6 +222,30 @@
   </si>
   <si>
     <t xml:space="preserve">Classic Advanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Shift Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberty Prime Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Captain Cosmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spartan Battle Suit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TES-51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submersible Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction Power Armor</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -492,7 +516,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -539,6 +563,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -634,7 +666,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart196.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1635,11 +1667,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="42723954"/>
-        <c:axId val="72229452"/>
+        <c:axId val="11022568"/>
+        <c:axId val="37907003"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42723954"/>
+        <c:axId val="11022568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1702,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72229452"/>
+        <c:crossAx val="37907003"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1678,7 +1710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72229452"/>
+        <c:axId val="37907003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1750,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42723954"/>
+        <c:crossAx val="11022568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1769,7 +1801,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart197.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3167,6 +3199,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3299,6 +3332,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3387,11 +3421,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="98042040"/>
-        <c:axId val="28670403"/>
+        <c:axId val="66891590"/>
+        <c:axId val="35424757"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98042040"/>
+        <c:axId val="66891590"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3422,7 +3456,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28670403"/>
+        <c:crossAx val="35424757"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3430,7 +3464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28670403"/>
+        <c:axId val="35424757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3470,7 +3504,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98042040"/>
+        <c:crossAx val="66891590"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3518,7 +3552,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart198.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart93.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3654,11 +3688,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="14898893"/>
-        <c:axId val="48259916"/>
+        <c:axId val="13030816"/>
+        <c:axId val="94683015"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14898893"/>
+        <c:axId val="13030816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3689,7 +3723,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48259916"/>
+        <c:crossAx val="94683015"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3697,7 +3731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48259916"/>
+        <c:axId val="94683015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3737,7 +3771,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14898893"/>
+        <c:crossAx val="13030816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3788,7 +3822,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart199.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart94.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5069,6 +5103,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -5151,11 +5186,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="75880279"/>
-        <c:axId val="80191320"/>
+        <c:axId val="51471438"/>
+        <c:axId val="52263011"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75880279"/>
+        <c:axId val="51471438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5186,7 +5221,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80191320"/>
+        <c:crossAx val="52263011"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5194,7 +5229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80191320"/>
+        <c:axId val="52263011"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5234,7 +5269,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75880279"/>
+        <c:crossAx val="51471438"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5285,7 +5320,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart200.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart95.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6233,11 +6268,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="59954739"/>
-        <c:axId val="51105968"/>
+        <c:axId val="19546644"/>
+        <c:axId val="86951482"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59954739"/>
+        <c:axId val="19546644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6302,7 +6337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51105968"/>
+        <c:crossAx val="86951482"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6310,7 +6345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51105968"/>
+        <c:axId val="86951482"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6384,7 +6419,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59954739"/>
+        <c:crossAx val="19546644"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6446,9 +6481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>280080</xdr:colOff>
+      <xdr:colOff>279360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6457,7 +6492,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732040"/>
-        <a:ext cx="7675560" cy="4271400"/>
+        <a:ext cx="7692840" cy="4270680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6481,9 +6516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>382320</xdr:colOff>
+      <xdr:colOff>381600</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6492,7 +6527,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10249920" cy="4271400"/>
+        <a:ext cx="10274760" cy="4270680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6516,9 +6551,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>512640</xdr:colOff>
+      <xdr:colOff>511920</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6527,7 +6562,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7685280" cy="4271400"/>
+        <a:ext cx="7705080" cy="4270680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6551,9 +6586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>71640</xdr:colOff>
+      <xdr:colOff>70920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6562,7 +6597,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10249920" cy="4271400"/>
+        <a:ext cx="10271880" cy="4270680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6586,9 +6621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>64080</xdr:colOff>
+      <xdr:colOff>63360</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6597,7 +6632,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2631960"/>
-        <a:ext cx="8423640" cy="4709520"/>
+        <a:ext cx="8430480" cy="4708800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6615,19 +6650,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.83"/>
@@ -8769,6 +8804,662 @@
       </c>
       <c r="AE23" s="10"/>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <f aca="false">SUM(B24,D24,F24*2,H24*2)</f>
+        <v>980</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <f aca="false">SUM(B24:E24) + SUM(F24:I24)*2</f>
+        <v>1625</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S24" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T24" s="12" t="n">
+        <f aca="false">SUM(J24,L24,N24,P24*2,R24*2)</f>
+        <v>1580</v>
+      </c>
+      <c r="U24" s="12" t="n">
+        <f aca="false">K24+SUM(L24:O24)+SUM(P24:S24)*2</f>
+        <v>2825</v>
+      </c>
+      <c r="V24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="13" t="n">
+        <f aca="false">U24+V24</f>
+        <v>2825</v>
+      </c>
+      <c r="X24" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <f aca="false">SUM(B25,D25,F25*2,H25*2)</f>
+        <v>835</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <f aca="false">SUM(B25:E25) + SUM(F25:I25)*2</f>
+        <v>1400</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S25" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T25" s="12" t="n">
+        <f aca="false">SUM(J25,L25,N25,P25*2,R25*2)</f>
+        <v>1435</v>
+      </c>
+      <c r="U25" s="12" t="n">
+        <f aca="false">K25+SUM(L25:O25)+SUM(P25:S25)*2</f>
+        <v>2600</v>
+      </c>
+      <c r="V25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="13" t="n">
+        <f aca="false">U25+V25</f>
+        <v>2600</v>
+      </c>
+      <c r="X25" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <f aca="false">SUM(B26,D26,F26*2,H26*2)</f>
+        <v>1460</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <f aca="false">SUM(B26:E26) + SUM(F26:I26)*2</f>
+        <v>2395</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q26" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T26" s="12" t="n">
+        <f aca="false">SUM(J26,L26,N26,P26*2,R26*2)</f>
+        <v>2060</v>
+      </c>
+      <c r="U26" s="12" t="n">
+        <f aca="false">K26+SUM(L26:O26)+SUM(P26:S26)*2</f>
+        <v>3595</v>
+      </c>
+      <c r="V26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="13" t="n">
+        <f aca="false">U26+V26</f>
+        <v>3595</v>
+      </c>
+      <c r="X26" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <f aca="false">SUM(B27,D27,F27*2,H27*2)</f>
+        <v>980</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <f aca="false">SUM(B27:E27) + SUM(F27:I27)*2</f>
+        <v>1625</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T27" s="12" t="n">
+        <f aca="false">SUM(J27,L27,N27,P27*2,R27*2)</f>
+        <v>1580</v>
+      </c>
+      <c r="U27" s="12" t="n">
+        <f aca="false">K27+SUM(L27:O27)+SUM(P27:S27)*2</f>
+        <v>2825</v>
+      </c>
+      <c r="V27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="13" t="n">
+        <f aca="false">U27+V27</f>
+        <v>2825</v>
+      </c>
+      <c r="X27" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <f aca="false">SUM(B28,D28,F28*2,H28*2)</f>
+        <v>1185</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <f aca="false">SUM(B28:E28) + SUM(F28:I28)*2</f>
+        <v>2010</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T28" s="12" t="n">
+        <f aca="false">SUM(J28,L28,N28,P28*2,R28*2)</f>
+        <v>1785</v>
+      </c>
+      <c r="U28" s="12" t="n">
+        <f aca="false">K28+SUM(L28:O28)+SUM(P28:S28)*2</f>
+        <v>3210</v>
+      </c>
+      <c r="V28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="13" t="n">
+        <f aca="false">U28+V28</f>
+        <v>3210</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <f aca="false">SUM(B29,D29,F29*2,H29*2)</f>
+        <v>1220</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <f aca="false">SUM(B29:E29) + SUM(F29:I29)*2</f>
+        <v>2010</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T29" s="12" t="n">
+        <f aca="false">SUM(J29,L29,N29,P29*2,R29*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="U29" s="12" t="n">
+        <f aca="false">K29+SUM(L29:O29)+SUM(P29:S29)*2</f>
+        <v>3210</v>
+      </c>
+      <c r="V29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" s="13" t="n">
+        <f aca="false">U29+V29</f>
+        <v>3210</v>
+      </c>
+      <c r="X29" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <f aca="false">SUM(B30,D30,F30*2,H30*2)</f>
+        <v>1080</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <f aca="false">SUM(B30:E30) + SUM(F30:I30)*2</f>
+        <v>1770</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q30" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T30" s="12" t="n">
+        <f aca="false">SUM(J30,L30,N30,P30*2,R30*2)</f>
+        <v>1680</v>
+      </c>
+      <c r="U30" s="12" t="n">
+        <f aca="false">K30+SUM(L30:O30)+SUM(P30:S30)*2</f>
+        <v>2970</v>
+      </c>
+      <c r="V30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" s="13" t="n">
+        <f aca="false">U30+V30</f>
+        <v>2970</v>
+      </c>
+      <c r="X30" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <f aca="false">SUM(B31,D31,F31*2,H31*2)</f>
+        <v>980</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <f aca="false">SUM(B31:E31) + SUM(F31:I31)*2</f>
+        <v>1625</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T31" s="12" t="n">
+        <f aca="false">SUM(J31,L31,N31,P31*2,R31*2)</f>
+        <v>1580</v>
+      </c>
+      <c r="U31" s="12" t="n">
+        <f aca="false">K31+SUM(L31:O31)+SUM(P31:S31)*2</f>
+        <v>2825</v>
+      </c>
+      <c r="V31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" s="13" t="n">
+        <f aca="false">U31+V31</f>
+        <v>2825</v>
+      </c>
+      <c r="X31" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="A1:A2"/>
@@ -8795,7 +9486,7 @@
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AE1:AE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="W2:W1048576">
+  <conditionalFormatting sqref="W32:W1048576 W2:W23">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -8804,7 +9495,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{806C96E0-AFF2-45B8-A223-D85AD085FCD2}</x14:id>
+          <x14:id>{5923D784-DA83-4425-A887-9F42D72585BE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8818,12 +9509,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C420284D-4C11-42BD-AB3C-E873D6312AA2}</x14:id>
+          <x14:id>{79CCE221-6C69-4C4B-90BD-26A0487650E7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:U1048576">
+  <conditionalFormatting sqref="T32:U1048576 T2:U23">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -8832,7 +9523,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7AD6E630-9DA0-4567-AA52-CB869BB2429D}</x14:id>
+          <x14:id>{BACFD341-508D-407D-89FA-D08EC08D3096}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8846,7 +9537,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7A9F1C27-2DEB-4072-808C-CB759C9D9C88}</x14:id>
+          <x14:id>{45872254-5327-4240-AC45-ECE4ED6FD577}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8860,7 +9551,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{513D5D9F-5038-4B9F-9318-A25A46D56D53}</x14:id>
+          <x14:id>{FFC43643-A7D0-4816-98C5-925D2DCDB2DB}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8874,7 +9565,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EA385ECE-81A3-4C2D-B522-301B5CAD2CFB}</x14:id>
+          <x14:id>{1A8AF0EE-F5E5-4627-9BCB-B46350A1ED14}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8888,7 +9579,49 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{76D761B4-54D9-4FF5-A460-3BDCE4BC7061}</x14:id>
+          <x14:id>{784471DB-D8C4-461E-8865-98B75556E694}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T24:T31">
+    <cfRule type="dataBar" priority="9">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{988C3535-A290-41F4-919F-BC4CF16178BE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U24:U31">
+    <cfRule type="dataBar" priority="10">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CDD49A8D-DC97-4B33-8715-E0364BE01F33}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W24:W31">
+    <cfRule type="dataBar" priority="11">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EFA0ADB6-A7E8-45AB-B731-C741129A4EFD}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8905,7 +9638,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{806C96E0-AFF2-45B8-A223-D85AD085FCD2}">
+          <x14:cfRule type="dataBar" id="{5923D784-DA83-4425-A887-9F42D72585BE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8913,10 +9646,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W2:W1048576</xm:sqref>
+          <xm:sqref>W32:W1048576 W2:W23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C420284D-4C11-42BD-AB3C-E873D6312AA2}">
+          <x14:cfRule type="dataBar" id="{79CCE221-6C69-4C4B-90BD-26A0487650E7}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8927,7 +9660,7 @@
           <xm:sqref>Z2:AA1048576 AB2:AD19 AB21:AD1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7AD6E630-9DA0-4567-AA52-CB869BB2429D}">
+          <x14:cfRule type="dataBar" id="{BACFD341-508D-407D-89FA-D08EC08D3096}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8935,10 +9668,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>T2:U1048576</xm:sqref>
+          <xm:sqref>T32:U1048576 T2:U23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7A9F1C27-2DEB-4072-808C-CB759C9D9C88}">
+          <x14:cfRule type="dataBar" id="{45872254-5327-4240-AC45-ECE4ED6FD577}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8949,7 +9682,7 @@
           <xm:sqref>J2:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{513D5D9F-5038-4B9F-9318-A25A46D56D53}">
+          <x14:cfRule type="dataBar" id="{FFC43643-A7D0-4816-98C5-925D2DCDB2DB}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8960,7 +9693,7 @@
           <xm:sqref>AB20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EA385ECE-81A3-4C2D-B522-301B5CAD2CFB}">
+          <x14:cfRule type="dataBar" id="{1A8AF0EE-F5E5-4627-9BCB-B46350A1ED14}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8971,7 +9704,7 @@
           <xm:sqref>AC20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{76D761B4-54D9-4FF5-A460-3BDCE4BC7061}">
+          <x14:cfRule type="dataBar" id="{784471DB-D8C4-461E-8865-98B75556E694}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8980,6 +9713,39 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>AD20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{988C3535-A290-41F4-919F-BC4CF16178BE}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>T24:T31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CDD49A8D-DC97-4B33-8715-E0364BE01F33}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U24:U31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EFA0ADB6-A7E8-45AB-B731-C741129A4EFD}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W24:W31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8998,7 +9764,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.83"/>
@@ -9009,7 +9775,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>28</v>
@@ -9027,22 +9793,22 @@
         <v>36</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9061,7 +9827,7 @@
       <c r="H2" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I2" s="12" t="n">
+      <c r="I2" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B2-570)/6</f>
         <v>690</v>
       </c>
@@ -9074,7 +9840,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9087,7 +9853,7 @@
       <c r="H3" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I3" s="12" t="n">
+      <c r="I3" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B3-570)/6</f>
         <v>730</v>
       </c>
@@ -9112,7 +9878,7 @@
       <c r="H4" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I4" s="12" t="n">
+      <c r="I4" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B4-570)/6</f>
         <v>930</v>
       </c>
@@ -9137,7 +9903,7 @@
       <c r="H5" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B5-570)/6</f>
         <v>970</v>
       </c>
@@ -9163,7 +9929,7 @@
         <f aca="false">F6</f>
         <v>1625</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B6-570)/6</f>
         <v>1390</v>
       </c>
@@ -9175,7 +9941,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9188,7 +9954,7 @@
       <c r="H7" s="0" t="n">
         <v>1625</v>
       </c>
-      <c r="I7" s="12" t="n">
+      <c r="I7" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B7-570)/6</f>
         <v>1430</v>
       </c>
@@ -9214,7 +9980,7 @@
         <f aca="false">G8</f>
         <v>2010</v>
       </c>
-      <c r="I8" s="12" t="n">
+      <c r="I8" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$13:$E$13)+(2*SUM('Power Armor Sets'!$F$13:$G$13))+(2*SUM('Power Armor Sets'!$H$15:$I$15))+($B8-570)/6</f>
         <v>1830</v>
       </c>
@@ -9226,7 +9992,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9240,7 +10006,7 @@
         <f aca="false">G8+270</f>
         <v>2280</v>
       </c>
-      <c r="I9" s="12" t="n">
+      <c r="I9" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$16:$E$16)+(2*SUM('Power Armor Sets'!$F$16:$G$16))+(2*SUM('Power Armor Sets'!$H$16:$I$16))+($B9-570)/6</f>
         <v>1890</v>
       </c>
@@ -9252,62 +10018,62 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="12"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -9333,7 +10099,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -9343,7 +10109,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>29</v>
@@ -9352,7 +10118,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>39</v>
@@ -9382,10 +10148,10 @@
         <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9672,8 +10438,8 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="0" t="n">
         <f aca="false">MAX(B12:L12, N11)</f>
         <v>3530</v>
@@ -9698,88 +10464,88 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="M16" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="13"/>
+      <c r="M18" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9804,7 +10570,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -9812,13 +10578,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9883,18 +10649,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -9920,7 +10686,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -9929,12 +10695,12 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -9944,7 +10710,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>44</v>
@@ -9965,17 +10731,17 @@
         <v>55</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="17" t="n">
         <v>930</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="17" t="n">
         <v>1470</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -9993,10 +10759,10 @@
       <c r="A3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="17" t="n">
         <v>1770</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="17" t="n">
         <v>1710</v>
       </c>
       <c r="M3" s="0" t="n">
@@ -10008,10 +10774,10 @@
       <c r="A4" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="17" t="n">
         <v>1770</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="17" t="n">
         <v>1710</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -10026,10 +10792,10 @@
       <c r="A5" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="17" t="n">
         <v>2010</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="17" t="n">
         <v>1950</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -10050,8 +10816,8 @@
       <c r="A6" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="n">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="n">
         <v>1950</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -10066,8 +10832,8 @@
       <c r="A7" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="n">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="n">
         <v>2190</v>
       </c>
       <c r="K7" s="0" t="n">
@@ -10082,8 +10848,8 @@
       <c r="A8" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15" t="n">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="n">
         <v>2430</v>
       </c>
       <c r="L8" s="0" t="n">
@@ -10098,8 +10864,8 @@
       <c r="A9" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="M9" s="0" t="n">
         <f aca="false">MAX(B9:L9, M8)</f>
         <v>3610</v>
@@ -10109,8 +10875,8 @@
       <c r="A10" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
       <c r="M10" s="0" t="n">
         <f aca="false">MAX(B10:L10, M9)</f>
         <v>3610</v>
@@ -10120,8 +10886,8 @@
       <c r="A11" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="M11" s="0" t="n">
         <f aca="false">MAX(B11:L11, M10)</f>
         <v>3610</v>
@@ -10131,9 +10897,9 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="L12" s="12"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="0" t="n">
         <f aca="false">MAX(B12:L12, M11)</f>
         <v>3610</v>
@@ -10143,8 +10909,8 @@
       <c r="A13" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="M13" s="0" t="n">
         <f aca="false">MAX(B13:L13, M12)</f>
         <v>3610</v>
@@ -10154,91 +10920,91 @@
       <c r="A14" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="M14" s="0" t="n">
         <f aca="false">MAX(B14:L14, M13)</f>
         <v>3610</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="F16" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="F17" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="F18" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="G18" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="16"/>
+      <c r="B19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10266,7 +11032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
@@ -10277,25 +11043,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Enclave Power Armor to balancing sheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Power Armor Sets" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="102">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve">Construction Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enclave Power Armor</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -666,7 +669,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1667,11 +1670,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="60663628"/>
-        <c:axId val="66070617"/>
+        <c:axId val="5361038"/>
+        <c:axId val="31790877"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60663628"/>
+        <c:axId val="5361038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1705,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66070617"/>
+        <c:crossAx val="31790877"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1710,7 +1713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66070617"/>
+        <c:axId val="31790877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1753,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60663628"/>
+        <c:crossAx val="5361038"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1801,7 +1804,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3424,11 +3427,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="36389062"/>
-        <c:axId val="63833575"/>
+        <c:axId val="64144204"/>
+        <c:axId val="80925128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36389062"/>
+        <c:axId val="64144204"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3459,7 +3462,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63833575"/>
+        <c:crossAx val="80925128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3467,7 +3470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63833575"/>
+        <c:axId val="80925128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3507,7 +3510,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36389062"/>
+        <c:crossAx val="64144204"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3555,7 +3558,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3691,11 +3694,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="85643686"/>
-        <c:axId val="8671527"/>
+        <c:axId val="52508192"/>
+        <c:axId val="20896844"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85643686"/>
+        <c:axId val="52508192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,7 +3729,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8671527"/>
+        <c:crossAx val="20896844"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3734,7 +3737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8671527"/>
+        <c:axId val="20896844"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3774,7 +3777,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85643686"/>
+        <c:crossAx val="52508192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3825,7 +3828,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5189,11 +5192,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="95857765"/>
-        <c:axId val="14491319"/>
+        <c:axId val="74531072"/>
+        <c:axId val="2475686"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95857765"/>
+        <c:axId val="74531072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5224,7 +5227,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14491319"/>
+        <c:crossAx val="2475686"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5232,7 +5235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14491319"/>
+        <c:axId val="2475686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5272,7 +5275,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95857765"/>
+        <c:crossAx val="74531072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5323,7 +5326,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6271,11 +6274,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="15672911"/>
-        <c:axId val="72603673"/>
+        <c:axId val="1461076"/>
+        <c:axId val="82703208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15672911"/>
+        <c:axId val="1461076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6340,7 +6343,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72603673"/>
+        <c:crossAx val="82703208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6348,7 +6351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72603673"/>
+        <c:axId val="82703208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6422,7 +6425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15672911"/>
+        <c:crossAx val="1461076"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6484,9 +6487,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>278640</xdr:colOff>
+      <xdr:colOff>278280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6495,7 +6498,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732040"/>
-        <a:ext cx="7709760" cy="4269960"/>
+        <a:ext cx="7718400" cy="4269600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6519,9 +6522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6530,7 +6533,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10299240" cy="4269960"/>
+        <a:ext cx="10311480" cy="4269600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6554,9 +6557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>511200</xdr:colOff>
+      <xdr:colOff>510840</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6565,7 +6568,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7724520" cy="4269960"/>
+        <a:ext cx="7734240" cy="4269600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6589,9 +6592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>70200</xdr:colOff>
+      <xdr:colOff>69840</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6600,7 +6603,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10294200" cy="4269960"/>
+        <a:ext cx="10305000" cy="4269600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6624,9 +6627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>62640</xdr:colOff>
+      <xdr:colOff>62280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6635,7 +6638,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2631960"/>
-        <a:ext cx="8437680" cy="4708080"/>
+        <a:ext cx="8440920" cy="4707720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6653,17 +6656,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z5" activeCellId="0" sqref="Z5"/>
+      <selection pane="bottomRight" activeCell="Z30" activeCellId="0" sqref="Z30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -9484,6 +9487,103 @@
         <v>26</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <f aca="false">SUM(B32,D32,F32*2,H32*2)</f>
+        <v>1220</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <f aca="false">SUM(B32:E32) + SUM(F32:I32)*2</f>
+        <v>2010</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S32" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T32" s="12" t="n">
+        <f aca="false">SUM(J32,L32,N32,P32*2,R32*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="U32" s="12" t="n">
+        <f aca="false">K32+SUM(L32:O32)+SUM(P32:S32)*2</f>
+        <v>3210</v>
+      </c>
+      <c r="V32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" s="13" t="n">
+        <f aca="false">U32+V32</f>
+        <v>3210</v>
+      </c>
+      <c r="X32" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA32" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB32" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC32" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD32" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="A1:A2"/>
@@ -9510,7 +9610,7 @@
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AE1:AE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="W32:W1048576 W2:W23">
+  <conditionalFormatting sqref="W33:W1048576 W2:W23">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9519,12 +9619,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B2687040-A0F5-44E1-8AD2-C425BE905D20}</x14:id>
+          <x14:id>{CD1189FA-E47E-471A-A7E8-4B3E8EFC40EA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:AA1048576 AB2:AD19 AB21:AD1048576">
+  <conditionalFormatting sqref="Z33:AA1048576 AB2:AD19 AB33:AD1048576 Z2:AA31 AB21:AD31">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9533,12 +9633,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B3DFE46A-9998-4797-9933-3EC98A36CF5E}</x14:id>
+          <x14:id>{3365F077-8D39-4693-95D9-8825C8822AE9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T32:U1048576 T2:U23">
+  <conditionalFormatting sqref="T33:U1048576 T2:U23">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9547,7 +9647,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D0AB1978-F739-4FC8-8FD0-7983C64AD0DF}</x14:id>
+          <x14:id>{F696BEEB-C62D-4AB0-9097-63824DD2298E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9561,7 +9661,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B9A2593E-DF44-45D8-947E-EA3858811CAF}</x14:id>
+          <x14:id>{B66BC4C4-5ADC-4D6A-BC40-401BC41DFA92}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9575,7 +9675,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{98DF1B77-A62F-496E-AC45-BF785D9F438B}</x14:id>
+          <x14:id>{4F5645EB-F541-44E8-B3D0-BE1B82286051}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9589,7 +9689,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C9A0D04F-2FE5-4AB0-B642-DACD61E48A75}</x14:id>
+          <x14:id>{F15E0020-DC60-434D-BAEB-54F0A79D65BE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9603,12 +9703,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4961C4E2-F0F3-4BC7-BB8D-5F1BA377D7B3}</x14:id>
+          <x14:id>{EF468A90-DC59-44F6-A2A0-A086BA60A2FE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T24:T31">
+  <conditionalFormatting sqref="T24:T32">
     <cfRule type="dataBar" priority="9">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9617,12 +9717,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C070C816-8C5B-4A16-A1C4-7F60ADB08A37}</x14:id>
+          <x14:id>{93278639-2F5B-4595-9140-E6B3EC2C1FFC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U24:U31">
+  <conditionalFormatting sqref="U24:U32">
     <cfRule type="dataBar" priority="10">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9631,12 +9731,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DD2B507F-267B-49D3-A779-BE49ACBB8C69}</x14:id>
+          <x14:id>{C66335FC-A6F5-4572-8B33-FF7D4F854E64}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W24:W31">
+  <conditionalFormatting sqref="W24:W32">
     <cfRule type="dataBar" priority="11">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9645,7 +9745,77 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BD40CCAA-8BF4-4330-ABA1-18316920B824}</x14:id>
+          <x14:id>{57B6C180-152D-456F-8E7C-19CD7320A39F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z32">
+    <cfRule type="dataBar" priority="12">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B79BDFD0-1D40-422A-888F-11E24F964070}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA32">
+    <cfRule type="dataBar" priority="13">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3600A5D7-8187-463E-AF60-3DBD186C8182}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB32">
+    <cfRule type="dataBar" priority="14">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C77DA585-4FC0-4747-8221-BD15E7218E35}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC32">
+    <cfRule type="dataBar" priority="15">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{70585478-4CA0-4CF0-A320-1F4FFCE19E6A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD32">
+    <cfRule type="dataBar" priority="16">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E8761C99-8A71-4BA0-AA71-8B8F7B1DB8C3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9662,7 +9832,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B2687040-A0F5-44E1-8AD2-C425BE905D20}">
+          <x14:cfRule type="dataBar" id="{CD1189FA-E47E-471A-A7E8-4B3E8EFC40EA}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9670,10 +9840,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W32:W1048576 W2:W23</xm:sqref>
+          <xm:sqref>W33:W1048576 W2:W23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B3DFE46A-9998-4797-9933-3EC98A36CF5E}">
+          <x14:cfRule type="dataBar" id="{3365F077-8D39-4693-95D9-8825C8822AE9}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9681,10 +9851,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Z2:AA1048576 AB2:AD19 AB21:AD1048576</xm:sqref>
+          <xm:sqref>Z33:AA1048576 AB2:AD19 AB33:AD1048576 Z2:AA31 AB21:AD31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D0AB1978-F739-4FC8-8FD0-7983C64AD0DF}">
+          <x14:cfRule type="dataBar" id="{F696BEEB-C62D-4AB0-9097-63824DD2298E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9692,10 +9862,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>T32:U1048576 T2:U23</xm:sqref>
+          <xm:sqref>T33:U1048576 T2:U23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B9A2593E-DF44-45D8-947E-EA3858811CAF}">
+          <x14:cfRule type="dataBar" id="{B66BC4C4-5ADC-4D6A-BC40-401BC41DFA92}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9706,7 +9876,7 @@
           <xm:sqref>J2:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{98DF1B77-A62F-496E-AC45-BF785D9F438B}">
+          <x14:cfRule type="dataBar" id="{4F5645EB-F541-44E8-B3D0-BE1B82286051}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9717,7 +9887,7 @@
           <xm:sqref>AB20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C9A0D04F-2FE5-4AB0-B642-DACD61E48A75}">
+          <x14:cfRule type="dataBar" id="{F15E0020-DC60-434D-BAEB-54F0A79D65BE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9728,7 +9898,7 @@
           <xm:sqref>AC20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4961C4E2-F0F3-4BC7-BB8D-5F1BA377D7B3}">
+          <x14:cfRule type="dataBar" id="{EF468A90-DC59-44F6-A2A0-A086BA60A2FE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9739,7 +9909,7 @@
           <xm:sqref>AD20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C070C816-8C5B-4A16-A1C4-7F60ADB08A37}">
+          <x14:cfRule type="dataBar" id="{93278639-2F5B-4595-9140-E6B3EC2C1FFC}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9747,10 +9917,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>T24:T31</xm:sqref>
+          <xm:sqref>T24:T32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DD2B507F-267B-49D3-A779-BE49ACBB8C69}">
+          <x14:cfRule type="dataBar" id="{C66335FC-A6F5-4572-8B33-FF7D4F854E64}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9758,10 +9928,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U24:U31</xm:sqref>
+          <xm:sqref>U24:U32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BD40CCAA-8BF4-4330-ABA1-18316920B824}">
+          <x14:cfRule type="dataBar" id="{57B6C180-152D-456F-8E7C-19CD7320A39F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9769,7 +9939,62 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W24:W31</xm:sqref>
+          <xm:sqref>W24:W32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B79BDFD0-1D40-422A-888F-11E24F964070}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Z32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3600A5D7-8187-463E-AF60-3DBD186C8182}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AA32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C77DA585-4FC0-4747-8221-BD15E7218E35}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AB32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{70585478-4CA0-4CF0-A320-1F4FFCE19E6A}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AC32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E8761C99-8A71-4BA0-AA71-8B8F7B1DB8C3}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AD32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9788,7 +10013,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.83"/>
@@ -9799,7 +10024,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>28</v>
@@ -9817,22 +10042,22 @@
         <v>36</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9864,7 +10089,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9965,7 +10190,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10016,7 +10241,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10042,7 +10267,7 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10050,54 +10275,54 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -10119,11 +10344,11 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -10133,7 +10358,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>29</v>
@@ -10142,7 +10367,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>39</v>
@@ -10172,10 +10397,10 @@
         <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10491,40 +10716,40 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M16" s="15" t="s">
         <v>53</v>
@@ -10532,43 +10757,43 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10597,7 +10822,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -10605,13 +10830,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10676,18 +10901,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -10713,7 +10938,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -10722,7 +10947,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>29</v>
@@ -10737,7 +10962,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>44</v>
@@ -10758,7 +10983,7 @@
         <v>55</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10960,76 +11185,76 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>92</v>
-      </c>
       <c r="C17" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="L18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="18"/>
     </row>
@@ -11059,7 +11284,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
@@ -11070,25 +11295,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add SE-01 to the balancing sheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="103">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t xml:space="preserve">Enclave Power Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-01</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -519,7 +522,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,6 +576,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1670,11 +1677,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="5361038"/>
-        <c:axId val="31790877"/>
+        <c:axId val="81123328"/>
+        <c:axId val="91138450"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5361038"/>
+        <c:axId val="81123328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1712,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31790877"/>
+        <c:crossAx val="91138450"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1713,7 +1720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31790877"/>
+        <c:axId val="91138450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1760,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5361038"/>
+        <c:crossAx val="81123328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3427,11 +3434,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="64144204"/>
-        <c:axId val="80925128"/>
+        <c:axId val="30415600"/>
+        <c:axId val="32701849"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64144204"/>
+        <c:axId val="30415600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3462,7 +3469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80925128"/>
+        <c:crossAx val="32701849"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3470,7 +3477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80925128"/>
+        <c:axId val="32701849"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +3517,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64144204"/>
+        <c:crossAx val="30415600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3694,11 +3701,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="52508192"/>
-        <c:axId val="20896844"/>
+        <c:axId val="45547115"/>
+        <c:axId val="46454211"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52508192"/>
+        <c:axId val="45547115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,7 +3736,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20896844"/>
+        <c:crossAx val="46454211"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3737,7 +3744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20896844"/>
+        <c:axId val="46454211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3784,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52508192"/>
+        <c:crossAx val="45547115"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5192,11 +5199,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="74531072"/>
-        <c:axId val="2475686"/>
+        <c:axId val="84112194"/>
+        <c:axId val="42930903"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74531072"/>
+        <c:axId val="84112194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5227,7 +5234,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2475686"/>
+        <c:crossAx val="42930903"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5235,7 +5242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2475686"/>
+        <c:axId val="42930903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5275,7 +5282,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74531072"/>
+        <c:crossAx val="84112194"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6274,11 +6281,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="1461076"/>
-        <c:axId val="82703208"/>
+        <c:axId val="93298184"/>
+        <c:axId val="22110683"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1461076"/>
+        <c:axId val="93298184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6343,7 +6350,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82703208"/>
+        <c:crossAx val="22110683"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6351,7 +6358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82703208"/>
+        <c:axId val="22110683"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6425,7 +6432,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1461076"/>
+        <c:crossAx val="93298184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6487,9 +6494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>278280</xdr:colOff>
+      <xdr:colOff>277920</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6498,7 +6505,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732040"/>
-        <a:ext cx="7718400" cy="4269600"/>
+        <a:ext cx="7722360" cy="4269240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6522,9 +6529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6533,7 +6540,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10311480" cy="4269600"/>
+        <a:ext cx="10317600" cy="4269240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6557,9 +6564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>510840</xdr:colOff>
+      <xdr:colOff>510480</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6568,7 +6575,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7734240" cy="4269600"/>
+        <a:ext cx="7738920" cy="4269240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6592,9 +6599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>69840</xdr:colOff>
+      <xdr:colOff>69480</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6603,7 +6610,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10305000" cy="4269600"/>
+        <a:ext cx="10310400" cy="4269240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6627,9 +6634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>62280</xdr:colOff>
+      <xdr:colOff>61920</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6638,7 +6645,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2631960"/>
-        <a:ext cx="8440920" cy="4707720"/>
+        <a:ext cx="8442720" cy="4707360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6656,17 +6663,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z30" activeCellId="0" sqref="Z30"/>
+      <selection pane="bottomRight" activeCell="AE33" activeCellId="0" sqref="AE33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -9584,6 +9591,103 @@
         <v>28</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="J33" s="14" t="n">
+        <f aca="false">SUM(B33,D33,F33*2,H33*2)</f>
+        <v>1100</v>
+      </c>
+      <c r="K33" s="14" t="n">
+        <f aca="false">SUM(B33:E33) + SUM(F33:I33)*2</f>
+        <v>1410</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T33" s="12" t="n">
+        <f aca="false">SUM(J33,L33,N33,P33*2,R33*2)</f>
+        <v>1700</v>
+      </c>
+      <c r="U33" s="12" t="n">
+        <f aca="false">K33+SUM(L33:O33)+SUM(P33:S33)*2</f>
+        <v>2610</v>
+      </c>
+      <c r="V33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" s="13" t="n">
+        <f aca="false">U33+V33</f>
+        <v>2610</v>
+      </c>
+      <c r="X33" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z33" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA33" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB33" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC33" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD33" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="A1:A2"/>
@@ -9610,7 +9714,7 @@
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AE1:AE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="W33:W1048576 W2:W23">
+  <conditionalFormatting sqref="W34:W1048576 W2:W23">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9619,12 +9723,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CD1189FA-E47E-471A-A7E8-4B3E8EFC40EA}</x14:id>
+          <x14:id>{25495032-12BB-4290-9224-C8D1F92CC2F8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z33:AA1048576 AB2:AD19 AB33:AD1048576 Z2:AA31 AB21:AD31">
+  <conditionalFormatting sqref="Z34:AA1048576 AB2:AD19 AB34:AD1048576 Z2:AA31 AB21:AD31">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9633,12 +9737,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3365F077-8D39-4693-95D9-8825C8822AE9}</x14:id>
+          <x14:id>{CCCC223C-F784-4FCF-8EFF-96F46691D384}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T33:U1048576 T2:U23">
+  <conditionalFormatting sqref="T34:U1048576 T2:U23">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9647,12 +9751,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F696BEEB-C62D-4AB0-9097-63824DD2298E}</x14:id>
+          <x14:id>{3AB37E69-8D59-41AA-AF99-2DE57EC2B9F6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K1048576">
+  <conditionalFormatting sqref="J34:K1048576 J2:K32">
     <cfRule type="dataBar" priority="5">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="min" val="0"/>
@@ -9661,7 +9765,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B66BC4C4-5ADC-4D6A-BC40-401BC41DFA92}</x14:id>
+          <x14:id>{FFEA2D9F-12BC-423C-8BA0-E0D1FFD877FE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9675,7 +9779,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4F5645EB-F541-44E8-B3D0-BE1B82286051}</x14:id>
+          <x14:id>{854FB636-7C83-4075-AF55-334A36FBA0A8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9689,7 +9793,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F15E0020-DC60-434D-BAEB-54F0A79D65BE}</x14:id>
+          <x14:id>{9EE14A71-B3C2-4925-9DE6-A693288C87FC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9703,7 +9807,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EF468A90-DC59-44F6-A2A0-A086BA60A2FE}</x14:id>
+          <x14:id>{BCCDE176-1291-4313-A6BC-BA5C34B97F8D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9717,7 +9821,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{93278639-2F5B-4595-9140-E6B3EC2C1FFC}</x14:id>
+          <x14:id>{F91123E0-AC68-4500-9E58-4330BAEC1C4F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9731,7 +9835,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C66335FC-A6F5-4572-8B33-FF7D4F854E64}</x14:id>
+          <x14:id>{AB9D8D2D-A756-4851-A18E-B3B2702B8B90}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9745,7 +9849,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{57B6C180-152D-456F-8E7C-19CD7320A39F}</x14:id>
+          <x14:id>{80CBC4A3-A6F0-46FF-9E1F-6383E09FAE4C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9759,7 +9863,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B79BDFD0-1D40-422A-888F-11E24F964070}</x14:id>
+          <x14:id>{CB1BB09D-F17F-446B-8292-2C15C063E7F9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9773,7 +9877,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3600A5D7-8187-463E-AF60-3DBD186C8182}</x14:id>
+          <x14:id>{EE7496F2-82C1-468F-B930-6049DFD53790}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9787,7 +9891,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C77DA585-4FC0-4747-8221-BD15E7218E35}</x14:id>
+          <x14:id>{D8F8FE6E-FC21-4D2F-86B0-37A0AD11824E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9801,7 +9905,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{70585478-4CA0-4CF0-A320-1F4FFCE19E6A}</x14:id>
+          <x14:id>{8B2930CF-CE13-488F-84F9-11F389708AEE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9815,7 +9919,147 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E8761C99-8A71-4BA0-AA71-8B8F7B1DB8C3}</x14:id>
+          <x14:id>{9FAF606C-7C3F-47EF-9F1C-7DAD63F49A4F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="dataBar" priority="17">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8A7CE098-8612-4BA4-9353-BA5372651020}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
+    <cfRule type="dataBar" priority="18">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{198C41CF-B246-4A3B-B7DE-E04CD7FDFF17}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T33">
+    <cfRule type="dataBar" priority="19">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5DF4685F-C0F4-478B-86D1-6491E0C5A845}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U33">
+    <cfRule type="dataBar" priority="20">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6AAC807D-3171-4E87-926F-30CE90DF7531}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W33">
+    <cfRule type="dataBar" priority="21">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DD5C4815-27CF-4AA3-A425-4BCD9044E9D1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z33">
+    <cfRule type="dataBar" priority="22">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{497084D7-91A0-4541-8280-984F6C5691B3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA33">
+    <cfRule type="dataBar" priority="23">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EA3CFBFD-BAE9-4738-B19B-A4EC999B5FC2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB33">
+    <cfRule type="dataBar" priority="24">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A04961C0-BFB1-4059-851F-F0FE867DD56F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC33">
+    <cfRule type="dataBar" priority="25">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E0907271-76C4-4D22-9F71-38F075F48BC6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD33">
+    <cfRule type="dataBar" priority="26">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5983B0"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2D1ABF78-EC66-444E-9B47-9027EA29E34B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9832,7 +10076,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CD1189FA-E47E-471A-A7E8-4B3E8EFC40EA}">
+          <x14:cfRule type="dataBar" id="{25495032-12BB-4290-9224-C8D1F92CC2F8}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9840,10 +10084,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W33:W1048576 W2:W23</xm:sqref>
+          <xm:sqref>W34:W1048576 W2:W23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3365F077-8D39-4693-95D9-8825C8822AE9}">
+          <x14:cfRule type="dataBar" id="{CCCC223C-F784-4FCF-8EFF-96F46691D384}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9851,10 +10095,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Z33:AA1048576 AB2:AD19 AB33:AD1048576 Z2:AA31 AB21:AD31</xm:sqref>
+          <xm:sqref>Z34:AA1048576 AB2:AD19 AB34:AD1048576 Z2:AA31 AB21:AD31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F696BEEB-C62D-4AB0-9097-63824DD2298E}">
+          <x14:cfRule type="dataBar" id="{3AB37E69-8D59-41AA-AF99-2DE57EC2B9F6}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9862,10 +10106,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>T33:U1048576 T2:U23</xm:sqref>
+          <xm:sqref>T34:U1048576 T2:U23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B66BC4C4-5ADC-4D6A-BC40-401BC41DFA92}">
+          <x14:cfRule type="dataBar" id="{FFEA2D9F-12BC-423C-8BA0-E0D1FFD877FE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9873,10 +10117,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J2:K1048576</xm:sqref>
+          <xm:sqref>J34:K1048576 J2:K32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4F5645EB-F541-44E8-B3D0-BE1B82286051}">
+          <x14:cfRule type="dataBar" id="{854FB636-7C83-4075-AF55-334A36FBA0A8}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9887,7 +10131,7 @@
           <xm:sqref>AB20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F15E0020-DC60-434D-BAEB-54F0A79D65BE}">
+          <x14:cfRule type="dataBar" id="{9EE14A71-B3C2-4925-9DE6-A693288C87FC}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9898,7 +10142,7 @@
           <xm:sqref>AC20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EF468A90-DC59-44F6-A2A0-A086BA60A2FE}">
+          <x14:cfRule type="dataBar" id="{BCCDE176-1291-4313-A6BC-BA5C34B97F8D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9909,7 +10153,7 @@
           <xm:sqref>AD20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{93278639-2F5B-4595-9140-E6B3EC2C1FFC}">
+          <x14:cfRule type="dataBar" id="{F91123E0-AC68-4500-9E58-4330BAEC1C4F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9920,7 +10164,7 @@
           <xm:sqref>T24:T32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C66335FC-A6F5-4572-8B33-FF7D4F854E64}">
+          <x14:cfRule type="dataBar" id="{AB9D8D2D-A756-4851-A18E-B3B2702B8B90}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9931,7 +10175,7 @@
           <xm:sqref>U24:U32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{57B6C180-152D-456F-8E7C-19CD7320A39F}">
+          <x14:cfRule type="dataBar" id="{80CBC4A3-A6F0-46FF-9E1F-6383E09FAE4C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9942,7 +10186,7 @@
           <xm:sqref>W24:W32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B79BDFD0-1D40-422A-888F-11E24F964070}">
+          <x14:cfRule type="dataBar" id="{CB1BB09D-F17F-446B-8292-2C15C063E7F9}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9953,7 +10197,7 @@
           <xm:sqref>Z32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3600A5D7-8187-463E-AF60-3DBD186C8182}">
+          <x14:cfRule type="dataBar" id="{EE7496F2-82C1-468F-B930-6049DFD53790}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9964,7 +10208,7 @@
           <xm:sqref>AA32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C77DA585-4FC0-4747-8221-BD15E7218E35}">
+          <x14:cfRule type="dataBar" id="{D8F8FE6E-FC21-4D2F-86B0-37A0AD11824E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9975,7 +10219,7 @@
           <xm:sqref>AB32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{70585478-4CA0-4CF0-A320-1F4FFCE19E6A}">
+          <x14:cfRule type="dataBar" id="{8B2930CF-CE13-488F-84F9-11F389708AEE}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9986,7 +10230,7 @@
           <xm:sqref>AC32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E8761C99-8A71-4BA0-AA71-8B8F7B1DB8C3}">
+          <x14:cfRule type="dataBar" id="{9FAF606C-7C3F-47EF-9F1C-7DAD63F49A4F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9995,6 +10239,116 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>AD32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8A7CE098-8612-4BA4-9353-BA5372651020}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{198C41CF-B246-4A3B-B7DE-E04CD7FDFF17}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5DF4685F-C0F4-478B-86D1-6491E0C5A845}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>T33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6AAC807D-3171-4E87-926F-30CE90DF7531}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DD5C4815-27CF-4AA3-A425-4BCD9044E9D1}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{497084D7-91A0-4541-8280-984F6C5691B3}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Z33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EA3CFBFD-BAE9-4738-B19B-A4EC999B5FC2}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AA33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A04961C0-BFB1-4059-851F-F0FE867DD56F}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AB33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E0907271-76C4-4D22-9F71-38F075F48BC6}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AC33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2D1ABF78-EC66-444E-9B47-9027EA29E34B}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FF5983B0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AD33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -10013,7 +10367,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.83"/>
@@ -10024,7 +10378,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>28</v>
@@ -10042,22 +10396,22 @@
         <v>36</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10076,7 +10430,7 @@
       <c r="H2" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I2" s="14" t="n">
+      <c r="I2" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B2-570)/6</f>
         <v>690</v>
       </c>
@@ -10089,7 +10443,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10102,7 +10456,7 @@
       <c r="H3" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I3" s="14" t="n">
+      <c r="I3" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B3-570)/6</f>
         <v>730</v>
       </c>
@@ -10127,7 +10481,7 @@
       <c r="H4" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I4" s="14" t="n">
+      <c r="I4" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B4-570)/6</f>
         <v>930</v>
       </c>
@@ -10152,7 +10506,7 @@
       <c r="H5" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I5" s="14" t="n">
+      <c r="I5" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B5-570)/6</f>
         <v>970</v>
       </c>
@@ -10178,7 +10532,7 @@
         <f aca="false">F6</f>
         <v>1625</v>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B6-570)/6</f>
         <v>1390</v>
       </c>
@@ -10190,7 +10544,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10203,7 +10557,7 @@
       <c r="H7" s="0" t="n">
         <v>1625</v>
       </c>
-      <c r="I7" s="14" t="n">
+      <c r="I7" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B7-570)/6</f>
         <v>1430</v>
       </c>
@@ -10229,7 +10583,7 @@
         <f aca="false">G8</f>
         <v>2010</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$13:$E$13)+(2*SUM('Power Armor Sets'!$F$13:$G$13))+(2*SUM('Power Armor Sets'!$H$15:$I$15))+($B8-570)/6</f>
         <v>1830</v>
       </c>
@@ -10241,7 +10595,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10255,7 +10609,7 @@
         <f aca="false">G8+270</f>
         <v>2280</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="15" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$16:$E$16)+(2*SUM('Power Armor Sets'!$F$16:$G$16))+(2*SUM('Power Armor Sets'!$H$16:$I$16))+($B9-570)/6</f>
         <v>1890</v>
       </c>
@@ -10267,62 +10621,62 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="14"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -10348,7 +10702,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -10358,7 +10712,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>29</v>
@@ -10367,7 +10721,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>39</v>
@@ -10397,10 +10751,10 @@
         <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10690,8 +11044,8 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="0" t="n">
         <f aca="false">MAX(B12:L12, N11)</f>
         <v>3530</v>
@@ -10716,88 +11070,88 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="M16" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="15"/>
+      <c r="M18" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10822,7 +11176,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -10830,13 +11184,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10901,18 +11255,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -10938,7 +11292,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -10947,12 +11301,12 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -10962,7 +11316,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>44</v>
@@ -10983,17 +11337,17 @@
         <v>55</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="n">
+      <c r="B2" s="18" t="n">
         <v>930</v>
       </c>
-      <c r="C2" s="17" t="n">
+      <c r="C2" s="18" t="n">
         <v>1470</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -11011,10 +11365,10 @@
       <c r="A3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="n">
+      <c r="B3" s="18" t="n">
         <v>1770</v>
       </c>
-      <c r="C3" s="17" t="n">
+      <c r="C3" s="18" t="n">
         <v>1710</v>
       </c>
       <c r="M3" s="0" t="n">
@@ -11026,10 +11380,10 @@
       <c r="A4" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="18" t="n">
         <v>1770</v>
       </c>
-      <c r="C4" s="17" t="n">
+      <c r="C4" s="18" t="n">
         <v>1710</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -11044,10 +11398,10 @@
       <c r="A5" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="17" t="n">
+      <c r="B5" s="18" t="n">
         <v>2010</v>
       </c>
-      <c r="C5" s="17" t="n">
+      <c r="C5" s="18" t="n">
         <v>1950</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -11068,8 +11422,8 @@
       <c r="A6" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17" t="n">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="n">
         <v>1950</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -11084,8 +11438,8 @@
       <c r="A7" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17" t="n">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="n">
         <v>2190</v>
       </c>
       <c r="K7" s="0" t="n">
@@ -11100,8 +11454,8 @@
       <c r="A8" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="n">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="n">
         <v>2430</v>
       </c>
       <c r="L8" s="0" t="n">
@@ -11116,8 +11470,8 @@
       <c r="A9" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
       <c r="M9" s="0" t="n">
         <f aca="false">MAX(B9:L9, M8)</f>
         <v>3610</v>
@@ -11127,8 +11481,8 @@
       <c r="A10" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="M10" s="0" t="n">
         <f aca="false">MAX(B10:L10, M9)</f>
         <v>3610</v>
@@ -11138,8 +11492,8 @@
       <c r="A11" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
       <c r="M11" s="0" t="n">
         <f aca="false">MAX(B11:L11, M10)</f>
         <v>3610</v>
@@ -11149,9 +11503,9 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="L12" s="14"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="L12" s="15"/>
       <c r="M12" s="0" t="n">
         <f aca="false">MAX(B12:L12, M11)</f>
         <v>3610</v>
@@ -11161,8 +11515,8 @@
       <c r="A13" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
       <c r="M13" s="0" t="n">
         <f aca="false">MAX(B13:L13, M12)</f>
         <v>3610</v>
@@ -11172,91 +11526,91 @@
       <c r="A14" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
       <c r="M14" s="0" t="n">
         <f aca="false">MAX(B14:L14, M13)</f>
         <v>3610</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>93</v>
+      <c r="B16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>93</v>
+      <c r="C17" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="L18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="18"/>
+      <c r="B19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11284,7 +11638,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
@@ -11295,25 +11649,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Synth Power Armor to the balance sheet
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="104">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">SE-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synth Power Armor</t>
   </si>
   <si>
     <t xml:space="preserve">Level</t>
@@ -522,7 +525,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -576,10 +579,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,7 +675,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1677,11 +1676,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="81123328"/>
-        <c:axId val="91138450"/>
+        <c:axId val="5403534"/>
+        <c:axId val="39829682"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81123328"/>
+        <c:axId val="5403534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1711,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91138450"/>
+        <c:crossAx val="39829682"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1720,7 +1719,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91138450"/>
+        <c:axId val="39829682"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,7 +1759,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81123328"/>
+        <c:crossAx val="5403534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1811,7 +1810,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3434,11 +3433,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="30415600"/>
-        <c:axId val="32701849"/>
+        <c:axId val="26895073"/>
+        <c:axId val="67328381"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30415600"/>
+        <c:axId val="26895073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,7 +3468,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32701849"/>
+        <c:crossAx val="67328381"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3477,7 +3476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32701849"/>
+        <c:axId val="67328381"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,7 +3516,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30415600"/>
+        <c:crossAx val="26895073"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3565,7 +3564,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3701,11 +3700,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45547115"/>
-        <c:axId val="46454211"/>
+        <c:axId val="71637688"/>
+        <c:axId val="61065115"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45547115"/>
+        <c:axId val="71637688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,7 +3735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46454211"/>
+        <c:crossAx val="61065115"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3744,7 +3743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46454211"/>
+        <c:axId val="61065115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3784,7 +3783,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45547115"/>
+        <c:crossAx val="71637688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3835,7 +3834,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5199,11 +5198,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84112194"/>
-        <c:axId val="42930903"/>
+        <c:axId val="87939479"/>
+        <c:axId val="13483733"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84112194"/>
+        <c:axId val="87939479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5234,7 +5233,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42930903"/>
+        <c:crossAx val="13483733"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5242,7 +5241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42930903"/>
+        <c:axId val="13483733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5282,7 +5281,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84112194"/>
+        <c:crossAx val="87939479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5333,7 +5332,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6281,11 +6280,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="93298184"/>
-        <c:axId val="22110683"/>
+        <c:axId val="79560735"/>
+        <c:axId val="53814348"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93298184"/>
+        <c:axId val="79560735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6350,7 +6349,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22110683"/>
+        <c:crossAx val="53814348"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6358,7 +6357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22110683"/>
+        <c:axId val="53814348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6432,7 +6431,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93298184"/>
+        <c:crossAx val="79560735"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6494,9 +6493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>277920</xdr:colOff>
+      <xdr:colOff>277560</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6505,7 +6504,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732040"/>
-        <a:ext cx="7722360" cy="4269240"/>
+        <a:ext cx="7731000" cy="4268880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6529,9 +6528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>380160</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6540,7 +6539,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10317600" cy="4269240"/>
+        <a:ext cx="10329840" cy="4268880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6564,9 +6563,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>510480</xdr:colOff>
+      <xdr:colOff>510120</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6575,7 +6574,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7738920" cy="4269240"/>
+        <a:ext cx="7749000" cy="4268880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6599,9 +6598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>69480</xdr:colOff>
+      <xdr:colOff>69120</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6610,7 +6609,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216600"/>
-        <a:ext cx="10310400" cy="4269240"/>
+        <a:ext cx="10321560" cy="4268880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6634,9 +6633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>61920</xdr:colOff>
+      <xdr:colOff>61560</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6645,7 +6644,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2631960"/>
-        <a:ext cx="8442720" cy="4707360"/>
+        <a:ext cx="8445960" cy="4707000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6663,17 +6662,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE33" activeCellId="0" sqref="AE33"/>
+      <selection pane="bottomRight" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -9619,11 +9618,11 @@
       <c r="I33" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="J33" s="14" t="n">
+      <c r="J33" s="12" t="n">
         <f aca="false">SUM(B33,D33,F33*2,H33*2)</f>
         <v>1100</v>
       </c>
-      <c r="K33" s="14" t="n">
+      <c r="K33" s="12" t="n">
         <f aca="false">SUM(B33:E33) + SUM(F33:I33)*2</f>
         <v>1410</v>
       </c>
@@ -9686,6 +9685,35 @@
       </c>
       <c r="AD33" s="0" t="n">
         <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -9723,7 +9751,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{25495032-12BB-4290-9224-C8D1F92CC2F8}</x14:id>
+          <x14:id>{808EDC33-4012-417B-ADA0-12FEA3153B4C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9737,7 +9765,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CCCC223C-F784-4FCF-8EFF-96F46691D384}</x14:id>
+          <x14:id>{30D8B36B-5990-40D7-A36D-6BE0A06465B4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9751,7 +9779,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3AB37E69-8D59-41AA-AF99-2DE57EC2B9F6}</x14:id>
+          <x14:id>{B7446259-52B3-44AB-A745-CF831F6E6B27}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9765,7 +9793,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FFEA2D9F-12BC-423C-8BA0-E0D1FFD877FE}</x14:id>
+          <x14:id>{70C7B993-A460-4438-98A5-AD31DDDB5355}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9779,7 +9807,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{854FB636-7C83-4075-AF55-334A36FBA0A8}</x14:id>
+          <x14:id>{A32250F0-D92F-451E-AED1-7EE7D9DA95FD}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9793,7 +9821,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9EE14A71-B3C2-4925-9DE6-A693288C87FC}</x14:id>
+          <x14:id>{6470C49C-009F-4929-A45B-50365512F25D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9807,7 +9835,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BCCDE176-1291-4313-A6BC-BA5C34B97F8D}</x14:id>
+          <x14:id>{8239898D-9129-4BEA-9AF4-416932F4478C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9821,7 +9849,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F91123E0-AC68-4500-9E58-4330BAEC1C4F}</x14:id>
+          <x14:id>{92B4ECD2-FA3B-4D90-BB95-70B4C922DE90}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9835,7 +9863,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AB9D8D2D-A756-4851-A18E-B3B2702B8B90}</x14:id>
+          <x14:id>{C9FBB874-2548-407F-95DD-77F8F6BE9DC2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9849,7 +9877,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{80CBC4A3-A6F0-46FF-9E1F-6383E09FAE4C}</x14:id>
+          <x14:id>{F18F2031-D0E5-4B36-9D6D-46A0B755E419}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9863,7 +9891,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CB1BB09D-F17F-446B-8292-2C15C063E7F9}</x14:id>
+          <x14:id>{E0A99F21-5F2B-49FB-9E2A-706F3831108F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9877,7 +9905,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EE7496F2-82C1-468F-B930-6049DFD53790}</x14:id>
+          <x14:id>{79E282D8-3837-4657-B33C-249CB745D5AA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9891,7 +9919,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D8F8FE6E-FC21-4D2F-86B0-37A0AD11824E}</x14:id>
+          <x14:id>{D7865811-EAD3-4DF6-B4FA-FD1A1F91D950}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9905,7 +9933,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8B2930CF-CE13-488F-84F9-11F389708AEE}</x14:id>
+          <x14:id>{0032F9BE-EE74-4430-ABAC-7065EFF0E864}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9919,7 +9947,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9FAF606C-7C3F-47EF-9F1C-7DAD63F49A4F}</x14:id>
+          <x14:id>{67CA108F-301C-4248-BAB7-FF54A8AD835E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9933,7 +9961,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8A7CE098-8612-4BA4-9353-BA5372651020}</x14:id>
+          <x14:id>{3E9E20DE-7F69-4926-A3E4-EEC73B6B4D00}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9947,7 +9975,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{198C41CF-B246-4A3B-B7DE-E04CD7FDFF17}</x14:id>
+          <x14:id>{E5F0557B-A1F2-4BD7-96EA-5B7B707BD694}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9961,7 +9989,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5DF4685F-C0F4-478B-86D1-6491E0C5A845}</x14:id>
+          <x14:id>{90AE89D8-9E5F-412D-8C3C-E440F3A1F215}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9975,7 +10003,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6AAC807D-3171-4E87-926F-30CE90DF7531}</x14:id>
+          <x14:id>{4D6CE7C7-82CC-4E34-8FDA-D022FCCD4C3A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9989,7 +10017,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DD5C4815-27CF-4AA3-A425-4BCD9044E9D1}</x14:id>
+          <x14:id>{5AB0672C-37E6-41EB-A4C7-1B856C1D8498}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10003,7 +10031,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{497084D7-91A0-4541-8280-984F6C5691B3}</x14:id>
+          <x14:id>{9C95ECFF-C956-4059-BF75-397E4665D4E5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10017,7 +10045,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EA3CFBFD-BAE9-4738-B19B-A4EC999B5FC2}</x14:id>
+          <x14:id>{FE1F6D3B-C69C-40D3-8225-144237C41FD7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10031,7 +10059,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A04961C0-BFB1-4059-851F-F0FE867DD56F}</x14:id>
+          <x14:id>{73AAF0FA-3CFA-48B4-99F4-70E8B75C93B9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10045,7 +10073,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E0907271-76C4-4D22-9F71-38F075F48BC6}</x14:id>
+          <x14:id>{10AE85C5-B474-42E5-B344-80225A78607C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10059,7 +10087,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2D1ABF78-EC66-444E-9B47-9027EA29E34B}</x14:id>
+          <x14:id>{E7C959B2-3914-49AB-A653-7140E96056C5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10076,7 +10104,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{25495032-12BB-4290-9224-C8D1F92CC2F8}">
+          <x14:cfRule type="dataBar" id="{808EDC33-4012-417B-ADA0-12FEA3153B4C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10087,7 +10115,7 @@
           <xm:sqref>W34:W1048576 W2:W23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CCCC223C-F784-4FCF-8EFF-96F46691D384}">
+          <x14:cfRule type="dataBar" id="{30D8B36B-5990-40D7-A36D-6BE0A06465B4}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10098,7 +10126,7 @@
           <xm:sqref>Z34:AA1048576 AB2:AD19 AB34:AD1048576 Z2:AA31 AB21:AD31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3AB37E69-8D59-41AA-AF99-2DE57EC2B9F6}">
+          <x14:cfRule type="dataBar" id="{B7446259-52B3-44AB-A745-CF831F6E6B27}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10109,7 +10137,7 @@
           <xm:sqref>T34:U1048576 T2:U23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FFEA2D9F-12BC-423C-8BA0-E0D1FFD877FE}">
+          <x14:cfRule type="dataBar" id="{70C7B993-A460-4438-98A5-AD31DDDB5355}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10120,7 +10148,7 @@
           <xm:sqref>J34:K1048576 J2:K32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{854FB636-7C83-4075-AF55-334A36FBA0A8}">
+          <x14:cfRule type="dataBar" id="{A32250F0-D92F-451E-AED1-7EE7D9DA95FD}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10131,7 +10159,7 @@
           <xm:sqref>AB20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9EE14A71-B3C2-4925-9DE6-A693288C87FC}">
+          <x14:cfRule type="dataBar" id="{6470C49C-009F-4929-A45B-50365512F25D}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10142,7 +10170,7 @@
           <xm:sqref>AC20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BCCDE176-1291-4313-A6BC-BA5C34B97F8D}">
+          <x14:cfRule type="dataBar" id="{8239898D-9129-4BEA-9AF4-416932F4478C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10153,7 +10181,7 @@
           <xm:sqref>AD20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F91123E0-AC68-4500-9E58-4330BAEC1C4F}">
+          <x14:cfRule type="dataBar" id="{92B4ECD2-FA3B-4D90-BB95-70B4C922DE90}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10164,7 +10192,7 @@
           <xm:sqref>T24:T32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AB9D8D2D-A756-4851-A18E-B3B2702B8B90}">
+          <x14:cfRule type="dataBar" id="{C9FBB874-2548-407F-95DD-77F8F6BE9DC2}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10175,7 +10203,7 @@
           <xm:sqref>U24:U32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{80CBC4A3-A6F0-46FF-9E1F-6383E09FAE4C}">
+          <x14:cfRule type="dataBar" id="{F18F2031-D0E5-4B36-9D6D-46A0B755E419}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10186,7 +10214,7 @@
           <xm:sqref>W24:W32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CB1BB09D-F17F-446B-8292-2C15C063E7F9}">
+          <x14:cfRule type="dataBar" id="{E0A99F21-5F2B-49FB-9E2A-706F3831108F}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10197,7 +10225,7 @@
           <xm:sqref>Z32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EE7496F2-82C1-468F-B930-6049DFD53790}">
+          <x14:cfRule type="dataBar" id="{79E282D8-3837-4657-B33C-249CB745D5AA}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10208,7 +10236,7 @@
           <xm:sqref>AA32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D8F8FE6E-FC21-4D2F-86B0-37A0AD11824E}">
+          <x14:cfRule type="dataBar" id="{D7865811-EAD3-4DF6-B4FA-FD1A1F91D950}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10219,7 +10247,7 @@
           <xm:sqref>AB32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8B2930CF-CE13-488F-84F9-11F389708AEE}">
+          <x14:cfRule type="dataBar" id="{0032F9BE-EE74-4430-ABAC-7065EFF0E864}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10230,7 +10258,7 @@
           <xm:sqref>AC32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9FAF606C-7C3F-47EF-9F1C-7DAD63F49A4F}">
+          <x14:cfRule type="dataBar" id="{67CA108F-301C-4248-BAB7-FF54A8AD835E}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10241,7 +10269,7 @@
           <xm:sqref>AD32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8A7CE098-8612-4BA4-9353-BA5372651020}">
+          <x14:cfRule type="dataBar" id="{3E9E20DE-7F69-4926-A3E4-EEC73B6B4D00}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10252,7 +10280,7 @@
           <xm:sqref>J33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{198C41CF-B246-4A3B-B7DE-E04CD7FDFF17}">
+          <x14:cfRule type="dataBar" id="{E5F0557B-A1F2-4BD7-96EA-5B7B707BD694}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10263,7 +10291,7 @@
           <xm:sqref>K33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5DF4685F-C0F4-478B-86D1-6491E0C5A845}">
+          <x14:cfRule type="dataBar" id="{90AE89D8-9E5F-412D-8C3C-E440F3A1F215}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10274,7 +10302,7 @@
           <xm:sqref>T33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6AAC807D-3171-4E87-926F-30CE90DF7531}">
+          <x14:cfRule type="dataBar" id="{4D6CE7C7-82CC-4E34-8FDA-D022FCCD4C3A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10285,7 +10313,7 @@
           <xm:sqref>U33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DD5C4815-27CF-4AA3-A425-4BCD9044E9D1}">
+          <x14:cfRule type="dataBar" id="{5AB0672C-37E6-41EB-A4C7-1B856C1D8498}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10296,7 +10324,7 @@
           <xm:sqref>W33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{497084D7-91A0-4541-8280-984F6C5691B3}">
+          <x14:cfRule type="dataBar" id="{9C95ECFF-C956-4059-BF75-397E4665D4E5}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10307,7 +10335,7 @@
           <xm:sqref>Z33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EA3CFBFD-BAE9-4738-B19B-A4EC999B5FC2}">
+          <x14:cfRule type="dataBar" id="{FE1F6D3B-C69C-40D3-8225-144237C41FD7}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10318,7 +10346,7 @@
           <xm:sqref>AA33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A04961C0-BFB1-4059-851F-F0FE867DD56F}">
+          <x14:cfRule type="dataBar" id="{73AAF0FA-3CFA-48B4-99F4-70E8B75C93B9}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10329,7 +10357,7 @@
           <xm:sqref>AB33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E0907271-76C4-4D22-9F71-38F075F48BC6}">
+          <x14:cfRule type="dataBar" id="{10AE85C5-B474-42E5-B344-80225A78607C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10340,7 +10368,7 @@
           <xm:sqref>AC33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2D1ABF78-EC66-444E-9B47-9027EA29E34B}">
+          <x14:cfRule type="dataBar" id="{E7C959B2-3914-49AB-A653-7140E96056C5}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10367,7 +10395,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.83"/>
@@ -10378,7 +10406,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>28</v>
@@ -10396,22 +10424,22 @@
         <v>36</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10430,7 +10458,7 @@
       <c r="H2" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I2" s="15" t="n">
+      <c r="I2" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B2-570)/6</f>
         <v>690</v>
       </c>
@@ -10443,7 +10471,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10456,7 +10484,7 @@
       <c r="H3" s="0" t="n">
         <v>870</v>
       </c>
-      <c r="I3" s="15" t="n">
+      <c r="I3" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B3-570)/6</f>
         <v>730</v>
       </c>
@@ -10481,7 +10509,7 @@
       <c r="H4" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I4" s="15" t="n">
+      <c r="I4" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B4-570)/6</f>
         <v>930</v>
       </c>
@@ -10506,7 +10534,7 @@
       <c r="H5" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="I5" s="15" t="n">
+      <c r="I5" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B5-570)/6</f>
         <v>970</v>
       </c>
@@ -10532,7 +10560,7 @@
         <f aca="false">F6</f>
         <v>1625</v>
       </c>
-      <c r="I6" s="15" t="n">
+      <c r="I6" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B6-570)/6</f>
         <v>1390</v>
       </c>
@@ -10544,7 +10572,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10557,7 +10585,7 @@
       <c r="H7" s="0" t="n">
         <v>1625</v>
       </c>
-      <c r="I7" s="15" t="n">
+      <c r="I7" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B7-570)/6</f>
         <v>1430</v>
       </c>
@@ -10583,7 +10611,7 @@
         <f aca="false">G8</f>
         <v>2010</v>
       </c>
-      <c r="I8" s="15" t="n">
+      <c r="I8" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$13:$E$13)+(2*SUM('Power Armor Sets'!$F$13:$G$13))+(2*SUM('Power Armor Sets'!$H$15:$I$15))+($B8-570)/6</f>
         <v>1830</v>
       </c>
@@ -10595,7 +10623,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10609,7 +10637,7 @@
         <f aca="false">G8+270</f>
         <v>2280</v>
       </c>
-      <c r="I9" s="15" t="n">
+      <c r="I9" s="14" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$16:$E$16)+(2*SUM('Power Armor Sets'!$F$16:$G$16))+(2*SUM('Power Armor Sets'!$H$16:$I$16))+($B9-570)/6</f>
         <v>1890</v>
       </c>
@@ -10621,62 +10649,62 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="15"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>80</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -10702,7 +10730,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -10712,7 +10740,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>29</v>
@@ -10721,7 +10749,7 @@
         <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>39</v>
@@ -10751,10 +10779,10 @@
         <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11044,8 +11072,8 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="0" t="n">
         <f aca="false">MAX(B12:L12, N11)</f>
         <v>3530</v>
@@ -11070,88 +11098,88 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="16"/>
+      <c r="M18" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11176,7 +11204,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -11184,13 +11212,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11255,18 +11283,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -11292,7 +11320,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -11301,12 +11329,12 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -11316,7 +11344,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>44</v>
@@ -11337,17 +11365,17 @@
         <v>55</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="n">
+      <c r="B2" s="17" t="n">
         <v>930</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="17" t="n">
         <v>1470</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -11365,10 +11393,10 @@
       <c r="A3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="n">
+      <c r="B3" s="17" t="n">
         <v>1770</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="C3" s="17" t="n">
         <v>1710</v>
       </c>
       <c r="M3" s="0" t="n">
@@ -11380,10 +11408,10 @@
       <c r="A4" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="17" t="n">
         <v>1770</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="C4" s="17" t="n">
         <v>1710</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -11398,10 +11426,10 @@
       <c r="A5" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="17" t="n">
         <v>2010</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="17" t="n">
         <v>1950</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -11422,8 +11450,8 @@
       <c r="A6" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="n">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="n">
         <v>1950</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -11438,8 +11466,8 @@
       <c r="A7" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="n">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="n">
         <v>2190</v>
       </c>
       <c r="K7" s="0" t="n">
@@ -11454,8 +11482,8 @@
       <c r="A8" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="n">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="n">
         <v>2430</v>
       </c>
       <c r="L8" s="0" t="n">
@@ -11470,8 +11498,8 @@
       <c r="A9" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="M9" s="0" t="n">
         <f aca="false">MAX(B9:L9, M8)</f>
         <v>3610</v>
@@ -11481,8 +11509,8 @@
       <c r="A10" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
       <c r="M10" s="0" t="n">
         <f aca="false">MAX(B10:L10, M9)</f>
         <v>3610</v>
@@ -11492,8 +11520,8 @@
       <c r="A11" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="M11" s="0" t="n">
         <f aca="false">MAX(B11:L11, M10)</f>
         <v>3610</v>
@@ -11503,9 +11531,9 @@
       <c r="A12" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="L12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="0" t="n">
         <f aca="false">MAX(B12:L12, M11)</f>
         <v>3610</v>
@@ -11515,8 +11543,8 @@
       <c r="A13" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="M13" s="0" t="n">
         <f aca="false">MAX(B13:L13, M12)</f>
         <v>3610</v>
@@ -11526,91 +11554,91 @@
       <c r="A14" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="M14" s="0" t="n">
         <f aca="false">MAX(B14:L14, M13)</f>
         <v>3610</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>94</v>
+      <c r="B16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>94</v>
+      <c r="C17" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>94</v>
+        <v>97</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="L18" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="19"/>
+      <c r="B19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11638,7 +11666,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
@@ -11649,25 +11677,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Industrialist Power Armor to balancing data
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="123">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -133,6 +133,9 @@
     <t xml:space="preserve">Much higher stats are available with Raider Overhaul</t>
   </si>
   <si>
+    <t xml:space="preserve">Industrialist Power Armor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Excavator</t>
   </si>
   <si>
@@ -166,10 +169,16 @@
     <t xml:space="preserve">Armorer 4 + Science 4 + Nuclear Physicist 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Higher tier because player upgrades allow for much higher stats</t>
+  </si>
+  <si>
     <t xml:space="preserve">Institute</t>
   </si>
   <si>
     <t xml:space="preserve">Quest locked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higher tier because each piece is equivalent to T-60, but the head and chest have the stats of only one piece</t>
   </si>
   <si>
     <t xml:space="preserve">T-51</t>
@@ -184,13 +193,13 @@
     <t xml:space="preserve">Red Shift Power Armor</t>
   </si>
   <si>
+    <t xml:space="preserve">Quantum T-47R</t>
+  </si>
+  <si>
     <t xml:space="preserve">SE-01</t>
   </si>
   <si>
     <t xml:space="preserve">Higher tier because of the very high physical defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantum T-47R</t>
   </si>
   <si>
     <t xml:space="preserve">T-47R</t>
@@ -244,6 +253,9 @@
     <t xml:space="preserve">Legendaries available at vendor only</t>
   </si>
   <si>
+    <t xml:space="preserve">Spartan Battle Suit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diving Power Armor</t>
   </si>
   <si>
@@ -256,16 +268,10 @@
     <t xml:space="preserve">Soviet Power Armor</t>
   </si>
   <si>
-    <t xml:space="preserve">Spartan Battle Suit</t>
-  </si>
-  <si>
     <t xml:space="preserve">TES-51</t>
   </si>
   <si>
     <t xml:space="preserve">X-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synth Power Armor</t>
   </si>
   <si>
     <t xml:space="preserve">X-02 (Black Devil)</t>
@@ -275,6 +281,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cannot be upgraded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synth Power Armor</t>
   </si>
   <si>
     <t xml:space="preserve">X-02 (CC)</t>
@@ -702,7 +711,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart136.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1667,28 +1676,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>690</c:v>
+                  <c:v>710</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>730</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>770</c:v>
+                  <c:v>870</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>810</c:v>
+                  <c:v>910</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>910</c:v>
+                  <c:v>970</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>950</c:v>
+                  <c:v>1010</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1140</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1340</c:v>
+                  <c:v>1380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1703,11 +1712,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8221635"/>
-        <c:axId val="83817712"/>
+        <c:axId val="83751279"/>
+        <c:axId val="15889737"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8221635"/>
+        <c:axId val="83751279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,7 +1747,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83817712"/>
+        <c:crossAx val="15889737"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1746,7 +1755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83817712"/>
+        <c:axId val="15889737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1795,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8221635"/>
+        <c:crossAx val="83751279"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1837,7 +1846,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart137.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3460,11 +3469,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="48885354"/>
-        <c:axId val="63820776"/>
+        <c:axId val="94704909"/>
+        <c:axId val="37819175"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48885354"/>
+        <c:axId val="94704909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3495,7 +3504,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63820776"/>
+        <c:crossAx val="37819175"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3503,7 +3512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63820776"/>
+        <c:axId val="37819175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,7 +3552,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48885354"/>
+        <c:crossAx val="94704909"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3591,7 +3600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart138.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3727,11 +3736,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="83605482"/>
-        <c:axId val="22297127"/>
+        <c:axId val="13121501"/>
+        <c:axId val="91690563"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83605482"/>
+        <c:axId val="13121501"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3762,7 +3771,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22297127"/>
+        <c:crossAx val="91690563"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3770,7 +3779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22297127"/>
+        <c:axId val="91690563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3810,7 +3819,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83605482"/>
+        <c:crossAx val="13121501"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3861,7 +3870,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5225,11 +5234,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19835707"/>
-        <c:axId val="74756025"/>
+        <c:axId val="54902611"/>
+        <c:axId val="52391616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19835707"/>
+        <c:axId val="54902611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5260,7 +5269,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74756025"/>
+        <c:crossAx val="52391616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5268,7 +5277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74756025"/>
+        <c:axId val="52391616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5308,7 +5317,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19835707"/>
+        <c:crossAx val="54902611"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5359,7 +5368,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart125.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart140.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6307,11 +6316,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="10704532"/>
-        <c:axId val="47899067"/>
+        <c:axId val="92375491"/>
+        <c:axId val="10256908"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10704532"/>
+        <c:axId val="92375491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6376,7 +6385,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47899067"/>
+        <c:crossAx val="10256908"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6384,7 +6393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47899067"/>
+        <c:axId val="10256908"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6458,7 +6467,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10704532"/>
+        <c:crossAx val="92375491"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6689,14 +6698,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE49"/>
+  <dimension ref="A1:AE50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC32" activeCellId="0" sqref="AC32"/>
+      <selection pane="bottomRight" activeCell="AA18" activeCellId="0" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6973,81 +6982,72 @@
         <v>28</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2" t="n">
         <f aca="false">SUM(B4,D4,F4*2,H4*2)</f>
-        <v>380</v>
+        <v>610</v>
       </c>
       <c r="K4" s="2" t="n">
         <f aca="false">SUM(B4:E4) + SUM(F4:I4)*2</f>
-        <v>570</v>
+        <v>860</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="T4" s="2" t="n">
         <f aca="false">SUM(J4,L4,N4,P4*2,R4*2)</f>
-        <v>980</v>
+        <v>730</v>
       </c>
       <c r="U4" s="2" t="n">
         <f aca="false">K4+SUM(L4:O4)+SUM(P4:S4)*2</f>
-        <v>1770</v>
-      </c>
-      <c r="V4" s="1" t="n">
-        <v>0</v>
+        <v>980</v>
       </c>
       <c r="W4" s="1" t="n">
         <f aca="false">U4+V4</f>
-        <v>1770</v>
-      </c>
-      <c r="X4" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>26</v>
+        <v>980</v>
       </c>
       <c r="AC4" s="0" t="n">
         <v>11</v>
@@ -7055,43 +7055,42 @@
       <c r="AD4" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AE4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="n">
         <f aca="false">SUM(B5,D5,F5*2,H5*2)</f>
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">SUM(B5:E5) + SUM(F5:I5)*2</f>
-        <v>810</v>
+        <v>570</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>100</v>
@@ -7119,15 +7118,24 @@
       </c>
       <c r="T5" s="2" t="n">
         <f aca="false">SUM(J5,L5,N5,P5*2,R5*2)</f>
-        <v>1100</v>
+        <v>980</v>
       </c>
       <c r="U5" s="2" t="n">
         <f aca="false">K5+SUM(L5:O5)+SUM(P5:S5)*2</f>
-        <v>2010</v>
+        <v>1770</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="n">
         <f aca="false">U5+V5</f>
-        <v>2010</v>
+        <v>1770</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AC5" s="0" t="n">
         <v>11</v>
@@ -7135,6 +7143,7 @@
       <c r="AD5" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="AE5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -7283,71 +7292,52 @@
         <f aca="false">K7+SUM(L7:O7)+SUM(P7:S7)*2</f>
         <v>2010</v>
       </c>
-      <c r="V7" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W7" s="1" t="n">
         <f aca="false">U7+V7</f>
         <v>2010</v>
       </c>
-      <c r="X7" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="0" t="n">
-        <v>7</v>
-      </c>
       <c r="AC7" s="0" t="n">
         <v>11</v>
       </c>
       <c r="AD7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AE7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>60</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J8" s="2" t="n">
         <f aca="false">SUM(B8,D8,F8*2,H8*2)</f>
-        <v>540</v>
+        <v>500</v>
       </c>
       <c r="K8" s="2" t="n">
         <f aca="false">SUM(B8:E8) + SUM(F8:I8)*2</f>
-        <v>830</v>
+        <v>810</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>100</v>
@@ -7375,18 +7365,18 @@
       </c>
       <c r="T8" s="2" t="n">
         <f aca="false">SUM(J8,L8,N8,P8*2,R8*2)</f>
-        <v>1140</v>
+        <v>1100</v>
       </c>
       <c r="U8" s="2" t="n">
         <f aca="false">K8+SUM(L8:O8)+SUM(P8:S8)*2</f>
-        <v>2030</v>
+        <v>2010</v>
       </c>
       <c r="V8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W8" s="1" t="n">
         <f aca="false">U8+V8</f>
-        <v>2030</v>
+        <v>2010</v>
       </c>
       <c r="X8" s="1" t="n">
         <v>39</v>
@@ -7394,12 +7384,22 @@
       <c r="Y8" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="Z8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="AC8" s="0" t="n">
         <v>11</v>
       </c>
       <c r="AD8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="AE8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -7424,18 +7424,18 @@
         <v>35</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J9" s="2" t="n">
         <f aca="false">SUM(B9,D9,F9*2,H9*2)</f>
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">SUM(B9:E9) + SUM(F9:I9)*2</f>
-        <v>870</v>
+        <v>830</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>100</v>
@@ -7463,18 +7463,18 @@
       </c>
       <c r="T9" s="2" t="n">
         <f aca="false">SUM(J9,L9,N9,P9*2,R9*2)</f>
-        <v>1160</v>
+        <v>1140</v>
       </c>
       <c r="U9" s="2" t="n">
         <f aca="false">K9+SUM(L9:O9)+SUM(P9:S9)*2</f>
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="V9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W9" s="1" t="n">
         <f aca="false">U9+V9</f>
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="X9" s="1" t="n">
         <v>39</v>
@@ -7490,40 +7490,40 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>110</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>60</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>35</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>35</v>
       </c>
       <c r="J10" s="2" t="n">
         <f aca="false">SUM(B10,D10,F10*2,H10*2)</f>
-        <v>675</v>
+        <v>560</v>
       </c>
       <c r="K10" s="2" t="n">
         <f aca="false">SUM(B10:E10) + SUM(F10:I10)*2</f>
-        <v>985</v>
+        <v>870</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>100</v>
@@ -7551,18 +7551,18 @@
       </c>
       <c r="T10" s="2" t="n">
         <f aca="false">SUM(J10,L10,N10,P10*2,R10*2)</f>
-        <v>1275</v>
+        <v>1160</v>
       </c>
       <c r="U10" s="2" t="n">
         <f aca="false">K10+SUM(L10:O10)+SUM(P10:S10)*2</f>
-        <v>2185</v>
+        <v>2070</v>
       </c>
       <c r="V10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W10" s="1" t="n">
         <f aca="false">U10+V10</f>
-        <v>2185</v>
+        <v>2070</v>
       </c>
       <c r="X10" s="1" t="n">
         <v>39</v>
@@ -7578,40 +7578,40 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>60</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J11" s="2" t="n">
         <f aca="false">SUM(B11,D11,F11*2,H11*2)</f>
-        <v>740</v>
+        <v>675</v>
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">SUM(B11:E11) + SUM(F11:I11)*2</f>
-        <v>1050</v>
+        <v>985</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>100</v>
@@ -7639,18 +7639,18 @@
       </c>
       <c r="T11" s="2" t="n">
         <f aca="false">SUM(J11,L11,N11,P11*2,R11*2)</f>
-        <v>1340</v>
+        <v>1275</v>
       </c>
       <c r="U11" s="2" t="n">
         <f aca="false">K11+SUM(L11:O11)+SUM(P11:S11)*2</f>
-        <v>2250</v>
+        <v>2185</v>
       </c>
       <c r="V11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W11" s="1" t="n">
         <f aca="false">U11+V11</f>
-        <v>2250</v>
+        <v>2185</v>
       </c>
       <c r="X11" s="1" t="n">
         <v>39</v>
@@ -7658,54 +7658,48 @@
       <c r="Y11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB11" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="AC11" s="0" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="AD11" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="AE11" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="B12" s="0" t="n">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J12" s="2" t="n">
         <f aca="false">SUM(B12,D12,F12*2,H12*2)</f>
-        <v>680</v>
+        <v>740</v>
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">SUM(B12:E12) + SUM(F12:I12)*2</f>
-        <v>1170</v>
+        <v>1050</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>100</v>
@@ -7733,77 +7727,73 @@
       </c>
       <c r="T12" s="2" t="n">
         <f aca="false">SUM(J12,L12,N12,P12*2,R12*2)</f>
-        <v>1280</v>
+        <v>1340</v>
       </c>
       <c r="U12" s="2" t="n">
         <f aca="false">K12+SUM(L12:O12)+SUM(P12:S12)*2</f>
-        <v>2370</v>
+        <v>2250</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="W12" s="1" t="n">
         <f aca="false">U12+V12</f>
-        <v>3210</v>
+        <v>2250</v>
       </c>
       <c r="X12" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="Y12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="Z12" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AA12" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AB12" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AC12" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD12" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AE12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="B13" s="0" t="n">
-        <v>360</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="J13" s="2" t="n">
         <f aca="false">SUM(B13,D13,F13*2,H13*2)</f>
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">SUM(B13:E13) + SUM(F13:I13)*2</f>
-        <v>1405</v>
+        <v>1170</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>100</v>
@@ -7812,10 +7802,10 @@
         <v>100</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>100</v>
@@ -7831,27 +7821,33 @@
       </c>
       <c r="T13" s="2" t="n">
         <f aca="false">SUM(J13,L13,N13,P13*2,R13*2)</f>
-        <v>1380</v>
+        <v>1280</v>
       </c>
       <c r="U13" s="2" t="n">
         <f aca="false">K13+SUM(L13:O13)+SUM(P13:S13)*2</f>
-        <v>2405</v>
+        <v>2370</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="W13" s="1" t="n">
         <f aca="false">U13+V13</f>
-        <v>2405</v>
+        <v>3210</v>
       </c>
       <c r="X13" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="Y13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Y13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB13" s="0" t="s">
-        <v>40</v>
+      <c r="Z13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>21</v>
       </c>
       <c r="AC13" s="0" t="n">
         <v>25</v>
@@ -7859,43 +7855,45 @@
       <c r="AD13" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="AE13" s="10"/>
+      <c r="AE13" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">SUM(B14,D14,F14*2,H14*2)</f>
-        <v>740</v>
+        <v>880</v>
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">SUM(B14:E14) + SUM(F14:I14)*2</f>
-        <v>1230</v>
+        <v>1405</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>100</v>
@@ -7904,10 +7902,10 @@
         <v>100</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>100</v>
@@ -7923,18 +7921,18 @@
       </c>
       <c r="T14" s="2" t="n">
         <f aca="false">SUM(J14,L14,N14,P14*2,R14*2)</f>
-        <v>1340</v>
+        <v>1380</v>
       </c>
       <c r="U14" s="2" t="n">
         <f aca="false">K14+SUM(L14:O14)+SUM(P14:S14)*2</f>
-        <v>2430</v>
+        <v>2405</v>
       </c>
       <c r="V14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W14" s="1" t="n">
         <f aca="false">U14+V14</f>
-        <v>2430</v>
+        <v>2405</v>
       </c>
       <c r="X14" s="1" t="n">
         <v>39</v>
@@ -7942,26 +7940,22 @@
       <c r="Y14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z14" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="AA14" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="AB14" s="0" t="n">
-        <v>14</v>
+      <c r="AB14" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="AC14" s="0" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AD14" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="AE14" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>240</v>
@@ -8039,6 +8033,15 @@
       </c>
       <c r="Y15" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="AC15" s="0" t="n">
         <v>18</v>
@@ -8050,39 +8053,39 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J16" s="2" t="n">
         <f aca="false">SUM(B16,D16,F16*2,H16*2)</f>
-        <v>825</v>
+        <v>740</v>
       </c>
       <c r="K16" s="2" t="n">
         <f aca="false">SUM(B16:E16) + SUM(F16:I16)*2</f>
-        <v>1380</v>
+        <v>1230</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>100</v>
@@ -8110,15 +8113,24 @@
       </c>
       <c r="T16" s="2" t="n">
         <f aca="false">SUM(J16,L16,N16,P16*2,R16*2)</f>
-        <v>1425</v>
+        <v>1340</v>
       </c>
       <c r="U16" s="2" t="n">
         <f aca="false">K16+SUM(L16:O16)+SUM(P16:S16)*2</f>
-        <v>2580</v>
+        <v>2430</v>
+      </c>
+      <c r="V16" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="W16" s="1" t="n">
         <f aca="false">U16+V16</f>
-        <v>2580</v>
+        <v>2430</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AC16" s="0" t="n">
         <v>18</v>
@@ -8126,19 +8138,20 @@
       <c r="AD16" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="AE16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>175</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>100</v>
@@ -8147,21 +8160,21 @@
         <v>100</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I17" s="1" t="n">
         <v>70</v>
       </c>
       <c r="J17" s="2" t="n">
         <f aca="false">SUM(B17,D17,F17*2,H17*2)</f>
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">SUM(B17:E17) + SUM(F17:I17)*2</f>
-        <v>1400</v>
+        <v>1380</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>100</v>
@@ -8189,61 +8202,58 @@
       </c>
       <c r="T17" s="2" t="n">
         <f aca="false">SUM(J17,L17,N17,P17*2,R17*2)</f>
-        <v>1435</v>
+        <v>1425</v>
       </c>
       <c r="U17" s="2" t="n">
         <f aca="false">K17+SUM(L17:O17)+SUM(P17:S17)*2</f>
-        <v>2600</v>
-      </c>
-      <c r="V17" s="1" t="n">
-        <v>0</v>
+        <v>2580</v>
       </c>
       <c r="W17" s="1" t="n">
         <f aca="false">U17+V17</f>
-        <v>2600</v>
-      </c>
-      <c r="X17" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>26</v>
+        <v>2580</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="J18" s="2" t="n">
         <f aca="false">SUM(B18,D18,F18*2,H18*2)</f>
-        <v>1100</v>
+        <v>835</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">SUM(B18:E18) + SUM(F18:I18)*2</f>
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>100</v>
@@ -8271,47 +8281,29 @@
       </c>
       <c r="T18" s="2" t="n">
         <f aca="false">SUM(J18,L18,N18,P18*2,R18*2)</f>
-        <v>1700</v>
+        <v>1435</v>
       </c>
       <c r="U18" s="2" t="n">
         <f aca="false">K18+SUM(L18:O18)+SUM(P18:S18)*2</f>
-        <v>2610</v>
+        <v>2600</v>
       </c>
       <c r="V18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="1" t="n">
         <f aca="false">U18+V18</f>
-        <v>2610</v>
+        <v>2600</v>
       </c>
       <c r="X18" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="Z18" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AA18" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AB18" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AC18" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD18" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AE18" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>320</v>
@@ -8384,39 +8376,39 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="J20" s="2" t="n">
         <f aca="false">SUM(B20,D20,F20*2,H20*2)</f>
-        <v>740</v>
+        <v>1100</v>
       </c>
       <c r="K20" s="2" t="n">
         <f aca="false">SUM(B20:E20) + SUM(F20:I20)*2</f>
-        <v>1530</v>
+        <v>1410</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>100</v>
@@ -8444,58 +8436,79 @@
       </c>
       <c r="T20" s="2" t="n">
         <f aca="false">SUM(J20,L20,N20,P20*2,R20*2)</f>
-        <v>1340</v>
+        <v>1700</v>
       </c>
       <c r="U20" s="2" t="n">
         <f aca="false">K20+SUM(L20:O20)+SUM(P20:S20)*2</f>
-        <v>2730</v>
+        <v>2610</v>
+      </c>
+      <c r="V20" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="W20" s="1" t="n">
         <f aca="false">U20+V20</f>
-        <v>2730</v>
+        <v>2610</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>21</v>
       </c>
       <c r="AC20" s="0" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AD20" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="AE20" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J21" s="2" t="n">
         <f aca="false">SUM(B21,D21,F21*2,H21*2)</f>
-        <v>980</v>
+        <v>740</v>
       </c>
       <c r="K21" s="2" t="n">
         <f aca="false">SUM(B21:E21) + SUM(F21:I21)*2</f>
-        <v>1625</v>
+        <v>1530</v>
       </c>
       <c r="L21" s="0" t="n">
         <v>100</v>
@@ -8523,26 +8536,26 @@
       </c>
       <c r="T21" s="2" t="n">
         <f aca="false">SUM(J21,L21,N21,P21*2,R21*2)</f>
-        <v>1580</v>
+        <v>1340</v>
       </c>
       <c r="U21" s="2" t="n">
         <f aca="false">K21+SUM(L21:O21)+SUM(P21:S21)*2</f>
-        <v>2825</v>
+        <v>2730</v>
       </c>
       <c r="W21" s="1" t="n">
         <f aca="false">U21+V21</f>
-        <v>2825</v>
+        <v>2730</v>
       </c>
       <c r="AC21" s="0" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="AD21" s="0" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>280</v>
@@ -8608,23 +8621,20 @@
         <f aca="false">K22+SUM(L22:O22)+SUM(P22:S22)*2</f>
         <v>2825</v>
       </c>
-      <c r="V22" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W22" s="1" t="n">
         <f aca="false">U22+V22</f>
         <v>2825</v>
       </c>
-      <c r="X22" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>26</v>
+      <c r="AC22" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>280</v>
@@ -8703,16 +8713,10 @@
       <c r="Y23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC23" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD23" s="0" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>280</v>
@@ -8800,7 +8804,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>280</v>
@@ -8866,10 +8870,19 @@
         <f aca="false">K25+SUM(L25:O25)+SUM(P25:S25)*2</f>
         <v>2825</v>
       </c>
+      <c r="V25" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="W25" s="1" t="n">
         <f aca="false">U25+V25</f>
         <v>2825</v>
       </c>
+      <c r="X25" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AC25" s="0" t="n">
         <v>25</v>
       </c>
@@ -8879,7 +8892,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>280</v>
@@ -8949,10 +8962,16 @@
         <f aca="false">U26+V26</f>
         <v>2825</v>
       </c>
+      <c r="AC26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD26" s="0" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>280</v>
@@ -9018,73 +9037,46 @@
         <f aca="false">K27+SUM(L27:O27)+SUM(P27:S27)*2</f>
         <v>2825</v>
       </c>
-      <c r="V27" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W27" s="1" t="n">
         <f aca="false">U27+V27</f>
         <v>2825</v>
       </c>
-      <c r="X27" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z27" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AA27" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AB27" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AC27" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD27" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AE27" s="10" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>380</v>
+        <v>280</v>
       </c>
       <c r="C28" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="F28" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>235</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>190</v>
-      </c>
       <c r="G28" s="1" t="n">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="J28" s="2" t="n">
         <f aca="false">SUM(B28,D28,F28*2,H28*2)</f>
-        <v>1375</v>
+        <v>980</v>
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">SUM(B28:E28) + SUM(F28:I28)*2</f>
-        <v>1685</v>
+        <v>1625</v>
       </c>
       <c r="L28" s="0" t="n">
         <v>100</v>
@@ -9112,165 +9104,177 @@
       </c>
       <c r="T28" s="2" t="n">
         <f aca="false">SUM(J28,L28,N28,P28*2,R28*2)</f>
-        <v>1975</v>
+        <v>1580</v>
       </c>
       <c r="U28" s="2" t="n">
         <f aca="false">K28+SUM(L28:O28)+SUM(P28:S28)*2</f>
+        <v>2825</v>
+      </c>
+      <c r="V28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1" t="n">
+        <f aca="false">U28+V28</f>
+        <v>2825</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE28" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <f aca="false">SUM(B29,D29,F29*2,H29*2)</f>
+        <v>1375</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <f aca="false">SUM(B29:E29) + SUM(F29:I29)*2</f>
+        <v>1685</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <f aca="false">SUM(J29,L29,N29,P29*2,R29*2)</f>
+        <v>1975</v>
+      </c>
+      <c r="U29" s="2" t="n">
+        <f aca="false">K29+SUM(L29:O29)+SUM(P29:S29)*2</f>
         <v>2885</v>
       </c>
-      <c r="V28" s="1" t="n">
+      <c r="V29" s="1" t="n">
         <f aca="false">(80+20)*6+80</f>
         <v>680</v>
       </c>
-      <c r="W28" s="1" t="n">
-        <f aca="false">U28+V28</f>
-        <v>3565</v>
-      </c>
-      <c r="X28" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="Y28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA28" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AB28" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC28" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="AD28" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE28" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="J29" s="2" t="n">
-        <f aca="false">SUM(B29,D29,F29*2,H29*2)</f>
-        <v>1080</v>
-      </c>
-      <c r="K29" s="2" t="n">
-        <f aca="false">SUM(B29:E29) + SUM(F29:I29)*2</f>
-        <v>1770</v>
-      </c>
-      <c r="L29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="N29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="O29" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="P29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q29" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="R29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S29" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T29" s="2" t="n">
-        <f aca="false">SUM(J29,L29,N29,P29*2,R29*2)</f>
-        <v>1680</v>
-      </c>
-      <c r="U29" s="2" t="n">
-        <f aca="false">K29+SUM(L29:O29)+SUM(P29:S29)*2</f>
-        <v>2970</v>
-      </c>
-      <c r="V29" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W29" s="1" t="n">
         <f aca="false">U29+V29</f>
-        <v>2970</v>
+        <v>3565</v>
       </c>
       <c r="X29" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="Y29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Y29" s="1" t="s">
-        <v>26</v>
+      <c r="AA29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB29" s="0" t="n">
+        <v>28</v>
       </c>
       <c r="AC29" s="0" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AD29" s="0" t="n">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="AE29" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>165</v>
+        <v>250</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="J30" s="2" t="n">
         <f aca="false">SUM(B30,D30,F30*2,H30*2)</f>
-        <v>1280</v>
+        <v>1080</v>
       </c>
       <c r="K30" s="2" t="n">
         <f aca="false">SUM(B30:E30) + SUM(F30:I30)*2</f>
-        <v>1800</v>
+        <v>1770</v>
       </c>
       <c r="L30" s="0" t="n">
         <v>100</v>
@@ -9298,180 +9302,182 @@
       </c>
       <c r="T30" s="2" t="n">
         <f aca="false">SUM(J30,L30,N30,P30*2,R30*2)</f>
-        <v>1880</v>
+        <v>1680</v>
       </c>
       <c r="U30" s="2" t="n">
         <f aca="false">K30+SUM(L30:O30)+SUM(P30:S30)*2</f>
-        <v>3000</v>
+        <v>2970</v>
+      </c>
+      <c r="V30" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="W30" s="1" t="n">
         <f aca="false">U30+V30</f>
-        <v>3000</v>
-      </c>
-      <c r="AE30" s="10" t="s">
-        <v>58</v>
+        <v>2970</v>
+      </c>
+      <c r="X30" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>220</v>
+        <v>330</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="J31" s="2" t="n">
         <f aca="false">SUM(B31,D31,F31*2,H31*2)</f>
-        <v>540</v>
+        <v>1280</v>
       </c>
       <c r="K31" s="2" t="n">
         <f aca="false">SUM(B31:E31) + SUM(F31:I31)*2</f>
-        <v>970</v>
+        <v>1800</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R31" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S31" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="T31" s="2" t="n">
         <f aca="false">SUM(J31,L31,N31,P31*2,R31*2)</f>
-        <v>1740</v>
+        <v>1880</v>
       </c>
       <c r="U31" s="2" t="n">
         <f aca="false">K31+SUM(L31:O31)+SUM(P31:S31)*2</f>
-        <v>3070</v>
-      </c>
-      <c r="V31" s="1" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="W31" s="1" t="n">
         <f aca="false">U31+V31</f>
-        <v>3070</v>
-      </c>
-      <c r="X31" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC31" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AE31" s="10"/>
+        <v>3000</v>
+      </c>
+      <c r="AE31" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="J32" s="2" t="n">
         <f aca="false">SUM(B32,D32,F32*2,H32*2)</f>
-        <v>1100</v>
+        <v>540</v>
       </c>
       <c r="K32" s="2" t="n">
         <f aca="false">SUM(B32:E32) + SUM(F32:I32)*2</f>
-        <v>1890</v>
+        <v>970</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M32" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="P32" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R32" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S32" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="T32" s="2" t="n">
         <f aca="false">SUM(J32,L32,N32,P32*2,R32*2)</f>
-        <v>1700</v>
+        <v>1740</v>
       </c>
       <c r="U32" s="2" t="n">
         <f aca="false">K32+SUM(L32:O32)+SUM(P32:S32)*2</f>
-        <v>3090</v>
+        <v>3070</v>
       </c>
       <c r="V32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W32" s="1" t="n">
         <f aca="false">U32+V32</f>
-        <v>3090</v>
+        <v>3070</v>
       </c>
       <c r="X32" s="1" t="n">
         <v>39</v>
@@ -9479,19 +9485,14 @@
       <c r="Y32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB32" s="0" t="n">
+      <c r="AC32" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="AC32" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="AD32" s="0" t="n">
-        <v>21</v>
-      </c>
+      <c r="AE32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>300</v>
@@ -9577,47 +9578,44 @@
         <v>29</v>
       </c>
       <c r="AD33" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AE33" s="0" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>140</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>110</v>
       </c>
       <c r="J34" s="2" t="n">
         <f aca="false">SUM(B34,D34,F34*2,H34*2)</f>
-        <v>1220</v>
+        <v>1100</v>
       </c>
       <c r="K34" s="2" t="n">
         <f aca="false">SUM(B34:E34) + SUM(F34:I34)*2</f>
-        <v>2010</v>
+        <v>1890</v>
       </c>
       <c r="L34" s="0" t="n">
         <v>100</v>
@@ -9645,54 +9643,69 @@
       </c>
       <c r="T34" s="2" t="n">
         <f aca="false">SUM(J34,L34,N34,P34*2,R34*2)</f>
-        <v>1820</v>
+        <v>1700</v>
       </c>
       <c r="U34" s="2" t="n">
         <f aca="false">K34+SUM(L34:O34)+SUM(P34:S34)*2</f>
-        <v>3210</v>
+        <v>3090</v>
+      </c>
+      <c r="V34" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="W34" s="1" t="n">
         <f aca="false">U34+V34</f>
-        <v>3210</v>
+        <v>3090</v>
+      </c>
+      <c r="X34" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB34" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="AC34" s="0" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AD34" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="AE34" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>320</v>
+        <v>365</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="J35" s="2" t="n">
         <f aca="false">SUM(B35,D35,F35*2,H35*2)</f>
-        <v>1220</v>
+        <v>1185</v>
       </c>
       <c r="K35" s="2" t="n">
         <f aca="false">SUM(B35:E35) + SUM(F35:I35)*2</f>
@@ -9724,7 +9737,7 @@
       </c>
       <c r="T35" s="2" t="n">
         <f aca="false">SUM(J35,L35,N35,P35*2,R35*2)</f>
-        <v>1820</v>
+        <v>1785</v>
       </c>
       <c r="U35" s="2" t="n">
         <f aca="false">K35+SUM(L35:O35)+SUM(P35:S35)*2</f>
@@ -9743,15 +9756,6 @@
       <c r="Y35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z35" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA35" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AB35" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AC35" s="0" t="n">
         <v>32</v>
       </c>
@@ -9761,7 +9765,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>320</v>
@@ -9831,12 +9835,6 @@
         <f aca="false">U36+V36</f>
         <v>3210</v>
       </c>
-      <c r="AA36" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AB36" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AC36" s="0" t="n">
         <v>32</v>
       </c>
@@ -9846,7 +9844,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>320</v>
@@ -9925,38 +9923,53 @@
       <c r="Y37" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="Z37" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA37" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB37" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC37" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD37" s="0" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>365</v>
+        <v>320</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="J38" s="2" t="n">
         <f aca="false">SUM(B38,D38,F38*2,H38*2)</f>
-        <v>1185</v>
+        <v>1220</v>
       </c>
       <c r="K38" s="2" t="n">
         <f aca="false">SUM(B38:E38) + SUM(F38:I38)*2</f>
@@ -9988,24 +10001,21 @@
       </c>
       <c r="T38" s="2" t="n">
         <f aca="false">SUM(J38,L38,N38,P38*2,R38*2)</f>
-        <v>1785</v>
+        <v>1820</v>
       </c>
       <c r="U38" s="2" t="n">
         <f aca="false">K38+SUM(L38:O38)+SUM(P38:S38)*2</f>
         <v>3210</v>
       </c>
-      <c r="V38" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W38" s="1" t="n">
         <f aca="false">U38+V38</f>
         <v>3210</v>
       </c>
-      <c r="X38" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y38" s="1" t="s">
-        <v>26</v>
+      <c r="AA38" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB38" s="0" t="n">
+        <v>28</v>
       </c>
       <c r="AC38" s="0" t="n">
         <v>32</v>
@@ -10016,7 +10026,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>320</v>
@@ -10098,7 +10108,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>320</v>
@@ -10177,26 +10187,10 @@
       <c r="Y40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z40" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA40" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AB40" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC40" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="AD40" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>320</v>
@@ -10263,11 +10257,11 @@
         <v>3210</v>
       </c>
       <c r="V41" s="1" t="n">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="W41" s="1" t="n">
         <f aca="false">U41+V41</f>
-        <v>3540</v>
+        <v>3210</v>
       </c>
       <c r="X41" s="1" t="n">
         <v>39</v>
@@ -10275,16 +10269,26 @@
       <c r="Y41" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="Z41" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA41" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB41" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="AC41" s="0" t="n">
         <v>32</v>
       </c>
       <c r="AD41" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="AE41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>420</v>
@@ -10361,7 +10365,7 @@
         <v>1</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z42" s="0" t="n">
         <v>35</v>
@@ -10379,12 +10383,12 @@
         <v>35</v>
       </c>
       <c r="AE42" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>320</v>
@@ -10440,7 +10444,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="T43" s="2" t="n">
         <f aca="false">SUM(J43,L43,N43,P43*2,R43*2)</f>
@@ -10448,14 +10452,14 @@
       </c>
       <c r="U43" s="2" t="n">
         <f aca="false">K43+SUM(L43:O43)+SUM(P43:S43)*2</f>
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="V43" s="1" t="n">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="W43" s="1" t="n">
         <f aca="false">U43+V43</f>
-        <v>3260</v>
+        <v>3540</v>
       </c>
       <c r="X43" s="1" t="n">
         <v>39</v>
@@ -10463,79 +10467,72 @@
       <c r="Y43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z43" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA43" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AC43" s="0" t="n">
         <v>32</v>
       </c>
       <c r="AD43" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="AE43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B44" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D44" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="E44" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F44" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="D44" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="E44" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="G44" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J44" s="2" t="n">
         <f aca="false">SUM(B44,D44,F44*2,H44*2)</f>
-        <v>620</v>
+        <v>1220</v>
       </c>
       <c r="K44" s="2" t="n">
         <f aca="false">SUM(B44:E44) + SUM(F44:I44)*2</f>
-        <v>1170</v>
+        <v>2010</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M44" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N44" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q44" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R44" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S44" s="1" t="n">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="T44" s="2" t="n">
         <f aca="false">SUM(J44,L44,N44,P44*2,R44*2)</f>
@@ -10543,14 +10540,14 @@
       </c>
       <c r="U44" s="2" t="n">
         <f aca="false">K44+SUM(L44:O44)+SUM(P44:S44)*2</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="V44" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W44" s="1" t="n">
         <f aca="false">U44+V44</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="X44" s="1" t="n">
         <v>39</v>
@@ -10574,63 +10571,63 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="J45" s="2" t="n">
         <f aca="false">SUM(B45,D45,F45*2,H45*2)</f>
-        <v>1220</v>
+        <v>620</v>
       </c>
       <c r="K45" s="2" t="n">
         <f aca="false">SUM(B45:E45) + SUM(F45:I45)*2</f>
-        <v>2440</v>
+        <v>1170</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M45" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O45" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q45" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="R45" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S45" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="T45" s="2" t="n">
         <f aca="false">SUM(J45,L45,N45,P45*2,R45*2)</f>
@@ -10638,22 +10635,25 @@
       </c>
       <c r="U45" s="2" t="n">
         <f aca="false">K45+SUM(L45:O45)+SUM(P45:S45)*2</f>
-        <v>3340</v>
+        <v>3270</v>
       </c>
       <c r="V45" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W45" s="1" t="n">
         <f aca="false">U45+V45</f>
-        <v>3340</v>
+        <v>3270</v>
       </c>
       <c r="X45" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB45" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z45" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="AC45" s="0" t="n">
@@ -10662,98 +10662,108 @@
       <c r="AD45" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="AE45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>360</v>
+        <v>320</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="G46" s="1" t="n">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="J46" s="2" t="n">
         <f aca="false">SUM(B46,D46,F46*2,H46*2)</f>
-        <v>1460</v>
+        <v>1220</v>
       </c>
       <c r="K46" s="2" t="n">
         <f aca="false">SUM(B46:E46) + SUM(F46:I46)*2</f>
-        <v>2395</v>
+        <v>2440</v>
       </c>
       <c r="L46" s="0" t="n">
         <v>100</v>
       </c>
       <c r="M46" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N46" s="0" t="n">
         <v>100</v>
       </c>
       <c r="O46" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P46" s="0" t="n">
         <v>100</v>
       </c>
       <c r="Q46" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="R46" s="0" t="n">
         <v>100</v>
       </c>
       <c r="S46" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="T46" s="2" t="n">
         <f aca="false">SUM(J46,L46,N46,P46*2,R46*2)</f>
-        <v>2060</v>
+        <v>1820</v>
       </c>
       <c r="U46" s="2" t="n">
         <f aca="false">K46+SUM(L46:O46)+SUM(P46:S46)*2</f>
-        <v>3595</v>
+        <v>3340</v>
       </c>
       <c r="V46" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W46" s="1" t="n">
         <f aca="false">U46+V46</f>
-        <v>3595</v>
+        <v>3340</v>
       </c>
       <c r="X46" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>26</v>
+        <v>82</v>
+      </c>
+      <c r="AB46" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC46" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD46" s="0" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>360</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>260</v>
@@ -10765,7 +10775,7 @@
         <v>210</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>210</v>
@@ -10779,7 +10789,7 @@
       </c>
       <c r="K47" s="2" t="n">
         <f aca="false">SUM(B47:E47) + SUM(F47:I47)*2</f>
-        <v>2415</v>
+        <v>2395</v>
       </c>
       <c r="L47" s="0" t="n">
         <v>100</v>
@@ -10811,14 +10821,14 @@
       </c>
       <c r="U47" s="2" t="n">
         <f aca="false">K47+SUM(L47:O47)+SUM(P47:S47)*2</f>
-        <v>3615</v>
+        <v>3595</v>
       </c>
       <c r="V47" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W47" s="1" t="n">
         <f aca="false">U47+V47</f>
-        <v>3615</v>
+        <v>3595</v>
       </c>
       <c r="X47" s="1" t="n">
         <v>39</v>
@@ -10826,58 +10836,42 @@
       <c r="Y47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z47" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AA47" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="AB47" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AC47" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="AD47" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AE47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>500</v>
+        <v>360</v>
       </c>
       <c r="C48" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F48" s="0" t="n">
         <v>210</v>
       </c>
-      <c r="D48" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E48" s="1" t="n">
+      <c r="G48" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F48" s="0" t="n">
-        <v>290</v>
-      </c>
-      <c r="G48" s="1" t="n">
-        <v>110</v>
-      </c>
       <c r="H48" s="0" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="J48" s="2" t="n">
         <f aca="false">SUM(B48,D48,F48*2,H48*2)</f>
-        <v>1860</v>
+        <v>1460</v>
       </c>
       <c r="K48" s="2" t="n">
         <f aca="false">SUM(B48:E48) + SUM(F48:I48)*2</f>
-        <v>2650</v>
+        <v>2415</v>
       </c>
       <c r="L48" s="0" t="n">
         <v>100</v>
@@ -10905,18 +10899,18 @@
       </c>
       <c r="T48" s="2" t="n">
         <f aca="false">SUM(J48,L48,N48,P48*2,R48*2)</f>
-        <v>2460</v>
+        <v>2060</v>
       </c>
       <c r="U48" s="2" t="n">
         <f aca="false">K48+SUM(L48:O48)+SUM(P48:S48)*2</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="V48" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W48" s="1" t="n">
         <f aca="false">U48+V48</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="X48" s="1" t="n">
         <v>39</v>
@@ -10924,54 +10918,58 @@
       <c r="Y48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB48" s="0" t="s">
+      <c r="Z48" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA48" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="AB48" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="AC48" s="0" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AD48" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AE48" s="10" t="s">
-        <v>83</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="AE48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="J49" s="2" t="n">
         <f aca="false">SUM(B49,D49,F49*2,H49*2)</f>
-        <v>1820</v>
+        <v>1860</v>
       </c>
       <c r="K49" s="2" t="n">
         <f aca="false">SUM(B49:E49) + SUM(F49:I49)*2</f>
-        <v>2810</v>
+        <v>2650</v>
       </c>
       <c r="L49" s="0" t="n">
         <v>100</v>
@@ -10999,18 +10997,18 @@
       </c>
       <c r="T49" s="2" t="n">
         <f aca="false">SUM(J49,L49,N49,P49*2,R49*2)</f>
-        <v>2420</v>
+        <v>2460</v>
       </c>
       <c r="U49" s="2" t="n">
         <f aca="false">K49+SUM(L49:O49)+SUM(P49:S49)*2</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="V49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W49" s="1" t="n">
         <f aca="false">U49+V49</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="X49" s="1" t="n">
         <v>39</v>
@@ -11018,13 +11016,7 @@
       <c r="Y49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z49" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AA49" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AB49" s="0" t="n">
+      <c r="AB49" s="0" t="s">
         <v>42</v>
       </c>
       <c r="AC49" s="0" t="n">
@@ -11033,7 +11025,107 @@
       <c r="AD49" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="AE49" s="10"/>
+      <c r="AE49" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="G50" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <f aca="false">SUM(B50,D50,F50*2,H50*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <f aca="false">SUM(B50:E50) + SUM(F50:I50)*2</f>
+        <v>2810</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M50" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O50" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q50" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S50" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T50" s="2" t="n">
+        <f aca="false">SUM(J50,L50,N50,P50*2,R50*2)</f>
+        <v>2420</v>
+      </c>
+      <c r="U50" s="2" t="n">
+        <f aca="false">K50+SUM(L50:O50)+SUM(P50:S50)*2</f>
+        <v>4010</v>
+      </c>
+      <c r="V50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W50" s="1" t="n">
+        <f aca="false">U50+V50</f>
+        <v>4010</v>
+      </c>
+      <c r="X50" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z50" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA50" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB50" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC50" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD50" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AE50" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -11070,7 +11162,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1234DB59-155D-4C96-8051-A9F533F8A57B}</x14:id>
+          <x14:id>{93C2E754-8DB0-463F-8650-20F810209855}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11084,7 +11176,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{421B8842-1BC0-4478-8E22-AC531B215085}</x14:id>
+          <x14:id>{4F7798E0-30F0-4C2E-99DB-B26E59CA8895}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11098,12 +11190,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{18A25CA0-571E-44E6-B964-5092337EDF4B}</x14:id>
+          <x14:id>{B6DFCDE9-95DB-44C3-BB15-4F40BEAEA6C4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:AD49">
+  <conditionalFormatting sqref="Z3:AD70">
     <cfRule type="dataBar" priority="5">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="num" val="1"/>
@@ -11112,7 +11204,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EE21968A-B329-4FEA-94CB-9C56C3364940}</x14:id>
+          <x14:id>{586FCFA4-187F-4CFD-8960-633D6B2F70AA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11129,7 +11221,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1234DB59-155D-4C96-8051-A9F533F8A57B}">
+          <x14:cfRule type="dataBar" id="{93C2E754-8DB0-463F-8650-20F810209855}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11140,7 +11232,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{421B8842-1BC0-4478-8E22-AC531B215085}">
+          <x14:cfRule type="dataBar" id="{4F7798E0-30F0-4C2E-99DB-B26E59CA8895}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11151,7 +11243,7 @@
           <xm:sqref>T2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{18A25CA0-571E-44E6-B964-5092337EDF4B}">
+          <x14:cfRule type="dataBar" id="{B6DFCDE9-95DB-44C3-BB15-4F40BEAEA6C4}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11162,7 +11254,7 @@
           <xm:sqref>J2:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EE21968A-B329-4FEA-94CB-9C56C3364940}">
+          <x14:cfRule type="dataBar" id="{586FCFA4-187F-4CFD-8960-633D6B2F70AA}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11174,7 +11266,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Z3:AD49</xm:sqref>
+          <xm:sqref>Z3:AD70</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -11206,40 +11298,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11260,7 +11352,7 @@
       </c>
       <c r="I2" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B2-570)/6</f>
-        <v>690</v>
+        <v>710</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">MAX(B2:I2)</f>
@@ -11271,7 +11363,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11286,7 +11378,7 @@
       </c>
       <c r="I3" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$5:$G$5))+(2*SUM('Power Armor Sets'!$H$5:$I$5))+($B3-570)/6</f>
-        <v>730</v>
+        <v>750</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">MAX(B3:I3)</f>
@@ -11311,7 +11403,7 @@
       </c>
       <c r="I4" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B4-570)/6</f>
-        <v>770</v>
+        <v>870</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">MAX(B4:I4)</f>
@@ -11321,7 +11413,7 @@
         <v>1230</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11336,7 +11428,7 @@
       </c>
       <c r="I5" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$6:$G$6))+(2*SUM('Power Armor Sets'!$H$6:$I$6))+($B5-570)/6</f>
-        <v>810</v>
+        <v>910</v>
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">MAX(B5:I5)</f>
@@ -11362,7 +11454,7 @@
       </c>
       <c r="I6" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B6-570)/6</f>
-        <v>910</v>
+        <v>970</v>
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">MAX(B6:I6)</f>
@@ -11372,7 +11464,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11387,7 +11479,7 @@
       </c>
       <c r="I7" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$5:$E$5)+(2*SUM('Power Armor Sets'!$F$9:$G$9))+(2*SUM('Power Armor Sets'!$H$9:$I$9))+($B7-570)/6</f>
-        <v>950</v>
+        <v>1010</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">MAX(B7:I7)</f>
@@ -11413,7 +11505,7 @@
       </c>
       <c r="I8" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$13:$E$13)+(2*SUM('Power Armor Sets'!$F$13:$G$13))+(2*SUM('Power Armor Sets'!$H$15:$I$15))+($B8-570)/6</f>
-        <v>1140</v>
+        <v>1350</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">MAX(B8:I8)</f>
@@ -11423,7 +11515,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11439,7 +11531,7 @@
       </c>
       <c r="I9" s="13" t="n">
         <f aca="false">SUM('Power Armor Sets'!$B$4:$C$4)+SUM('Power Armor Sets'!$D$16:$E$16)+(2*SUM('Power Armor Sets'!$F$16:$G$16))+(2*SUM('Power Armor Sets'!$H$16:$I$16))+($B9-570)/6</f>
-        <v>1340</v>
+        <v>1380</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">MAX(B9:I9)</f>
@@ -11449,7 +11541,7 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11457,54 +11549,54 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -11540,49 +11632,49 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11898,84 +11990,84 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="L16" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="K16" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="M16" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12012,13 +12104,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12083,18 +12175,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -12129,43 +12221,43 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12367,76 +12459,76 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="16" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C19" s="16"/>
     </row>
@@ -12480,25 +12572,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add repair requirements for Classic Remnants Power Armor
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="127">
   <si>
     <t xml:space="preserve">Power Armor Set</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">X-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Remnants</t>
   </si>
   <si>
     <t xml:space="preserve">X-02 (Black Devil)</t>
@@ -733,7 +736,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1734,11 +1737,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="7857960"/>
-        <c:axId val="46576964"/>
+        <c:axId val="84048517"/>
+        <c:axId val="81402495"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7857960"/>
+        <c:axId val="84048517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,7 +1772,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46576964"/>
+        <c:crossAx val="81402495"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1777,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46576964"/>
+        <c:axId val="81402495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,7 +1820,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7857960"/>
+        <c:crossAx val="84048517"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1868,7 +1871,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3491,11 +3494,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="44903209"/>
-        <c:axId val="45990402"/>
+        <c:axId val="44565758"/>
+        <c:axId val="29746737"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44903209"/>
+        <c:axId val="44565758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3526,7 +3529,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45990402"/>
+        <c:crossAx val="29746737"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3534,7 +3537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45990402"/>
+        <c:axId val="29746737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3574,7 +3577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44903209"/>
+        <c:crossAx val="44565758"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3622,7 +3625,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3758,11 +3761,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="39963812"/>
-        <c:axId val="48547754"/>
+        <c:axId val="2349601"/>
+        <c:axId val="69778334"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39963812"/>
+        <c:axId val="2349601"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3793,7 +3796,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48547754"/>
+        <c:crossAx val="69778334"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3801,7 +3804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48547754"/>
+        <c:axId val="69778334"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3841,7 +3844,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39963812"/>
+        <c:crossAx val="2349601"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3892,7 +3895,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5256,11 +5259,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="93342942"/>
-        <c:axId val="14221353"/>
+        <c:axId val="53018299"/>
+        <c:axId val="60898876"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93342942"/>
+        <c:axId val="53018299"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5291,7 +5294,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14221353"/>
+        <c:crossAx val="60898876"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5299,7 +5302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14221353"/>
+        <c:axId val="60898876"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5339,7 +5342,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93342942"/>
+        <c:crossAx val="53018299"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5390,7 +5393,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6338,11 +6341,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="15834335"/>
-        <c:axId val="1536441"/>
+        <c:axId val="38877117"/>
+        <c:axId val="15603435"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15834335"/>
+        <c:axId val="38877117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6407,7 +6410,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1536441"/>
+        <c:crossAx val="15603435"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6415,7 +6418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1536441"/>
+        <c:axId val="15603435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6489,7 +6492,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15834335"/>
+        <c:crossAx val="38877117"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6551,9 +6554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>274680</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6562,7 +6565,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732400"/>
-        <a:ext cx="7781400" cy="4266000"/>
+        <a:ext cx="7781040" cy="4265640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6586,9 +6589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>376920</xdr:colOff>
+      <xdr:colOff>376560</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6597,7 +6600,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216960"/>
-        <a:ext cx="10422360" cy="4266000"/>
+        <a:ext cx="10434600" cy="4265640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6621,9 +6624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506880</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6632,7 +6635,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7822080" cy="4266000"/>
+        <a:ext cx="7831800" cy="4265640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6656,9 +6659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>66240</xdr:colOff>
+      <xdr:colOff>65880</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6667,7 +6670,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216960"/>
-        <a:ext cx="10404360" cy="4266000"/>
+        <a:ext cx="10415520" cy="4265640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6691,9 +6694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>58680</xdr:colOff>
+      <xdr:colOff>58320</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6702,7 +6705,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2632320"/>
-        <a:ext cx="8466120" cy="4704120"/>
+        <a:ext cx="8465760" cy="4703760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6720,17 +6723,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE53"/>
+  <dimension ref="A1:AE54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="W15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE15" activeCellId="0" sqref="AE15"/>
+      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="Z43" activeCellId="0" sqref="Z43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -10474,60 +10477,60 @@
         <v>77</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>310</v>
+        <v>210</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>240</v>
+        <v>140</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="G44" s="1" t="n">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="J44" s="2" t="n">
         <f aca="false">SUM(B44,D44,F44*2,H44*2)</f>
-        <v>1820</v>
+        <v>1220</v>
       </c>
       <c r="K44" s="2" t="n">
         <f aca="false">SUM(B44:E44) + SUM(F44:I44)*2</f>
-        <v>3210</v>
+        <v>2010</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M44" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N44" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q44" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R44" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S44" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T44" s="2" t="n">
         <f aca="false">SUM(J44,L44,N44,P44*2,R44*2)</f>
@@ -10545,89 +10548,87 @@
         <v>3210</v>
       </c>
       <c r="X44" s="1" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="Y44" s="1" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="Z44" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AA44" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AB44" s="0" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AC44" s="0" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="AD44" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AE44" s="0" t="s">
-        <v>79</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="AE44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="n">
+        <v>420</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="D45" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="E45" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="G45" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="D45" s="0" t="n">
-        <v>220</v>
-      </c>
-      <c r="E45" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="G45" s="1" t="n">
-        <v>110</v>
-      </c>
       <c r="H45" s="0" t="n">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="J45" s="2" t="n">
         <f aca="false">SUM(B45,D45,F45*2,H45*2)</f>
-        <v>1220</v>
+        <v>1820</v>
       </c>
       <c r="K45" s="2" t="n">
         <f aca="false">SUM(B45:E45) + SUM(F45:I45)*2</f>
-        <v>2010</v>
+        <v>3210</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M45" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O45" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R45" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S45" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="T45" s="2" t="n">
         <f aca="false">SUM(J45,L45,N45,P45*2,R45*2)</f>
@@ -10638,23 +10639,35 @@
         <v>3210</v>
       </c>
       <c r="V45" s="1" t="n">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="W45" s="1" t="n">
         <f aca="false">U45+V45</f>
-        <v>3540</v>
+        <v>3210</v>
       </c>
       <c r="X45" s="1" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="Y45" s="1" t="s">
-        <v>26</v>
+        <v>79</v>
+      </c>
+      <c r="Z45" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA45" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB45" s="0" t="n">
+        <v>35</v>
       </c>
       <c r="AC45" s="0" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AD45" s="0" t="n">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="AE45" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10715,7 +10728,7 @@
         <v>100</v>
       </c>
       <c r="S46" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="T46" s="2" t="n">
         <f aca="false">SUM(J46,L46,N46,P46*2,R46*2)</f>
@@ -10723,14 +10736,14 @@
       </c>
       <c r="U46" s="2" t="n">
         <f aca="false">K46+SUM(L46:O46)+SUM(P46:S46)*2</f>
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="V46" s="1" t="n">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="W46" s="1" t="n">
         <f aca="false">U46+V46</f>
-        <v>3260</v>
+        <v>3540</v>
       </c>
       <c r="X46" s="1" t="n">
         <v>39</v>
@@ -10738,79 +10751,72 @@
       <c r="Y46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z46" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AA46" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AC46" s="0" t="n">
         <v>32</v>
       </c>
       <c r="AD46" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="AE46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="D47" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="E47" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>170</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="E47" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="G47" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="I47" s="1" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J47" s="2" t="n">
         <f aca="false">SUM(B47,D47,F47*2,H47*2)</f>
-        <v>620</v>
+        <v>1220</v>
       </c>
       <c r="K47" s="2" t="n">
         <f aca="false">SUM(B47:E47) + SUM(F47:I47)*2</f>
-        <v>1170</v>
+        <v>2010</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M47" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="N47" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O47" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q47" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R47" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S47" s="1" t="n">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="T47" s="2" t="n">
         <f aca="false">SUM(J47,L47,N47,P47*2,R47*2)</f>
@@ -10818,14 +10824,14 @@
       </c>
       <c r="U47" s="2" t="n">
         <f aca="false">K47+SUM(L47:O47)+SUM(P47:S47)*2</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="V47" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W47" s="1" t="n">
         <f aca="false">U47+V47</f>
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="X47" s="1" t="n">
         <v>39</v>
@@ -10852,60 +10858,60 @@
         <v>83</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="J48" s="2" t="n">
         <f aca="false">SUM(B48,D48,F48*2,H48*2)</f>
-        <v>1220</v>
+        <v>620</v>
       </c>
       <c r="K48" s="2" t="n">
         <f aca="false">SUM(B48:E48) + SUM(F48:I48)*2</f>
-        <v>2440</v>
+        <v>1170</v>
       </c>
       <c r="L48" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M48" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="N48" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O48" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q48" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="R48" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S48" s="1" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="T48" s="2" t="n">
         <f aca="false">SUM(J48,L48,N48,P48*2,R48*2)</f>
@@ -10913,22 +10919,25 @@
       </c>
       <c r="U48" s="2" t="n">
         <f aca="false">K48+SUM(L48:O48)+SUM(P48:S48)*2</f>
-        <v>3340</v>
+        <v>3270</v>
       </c>
       <c r="V48" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W48" s="1" t="n">
         <f aca="false">U48+V48</f>
-        <v>3340</v>
+        <v>3270</v>
       </c>
       <c r="X48" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB48" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z48" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA48" s="0" t="n">
         <v>28</v>
       </c>
       <c r="AC48" s="0" t="n">
@@ -10937,87 +10946,88 @@
       <c r="AD48" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="AE48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>360</v>
+        <v>320</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>145</v>
+        <v>220</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="J49" s="2" t="n">
         <f aca="false">SUM(B49,D49,F49*2,H49*2)</f>
-        <v>1300</v>
+        <v>1220</v>
       </c>
       <c r="K49" s="2" t="n">
         <f aca="false">SUM(B49:E49) + SUM(F49:I49)*2</f>
-        <v>2165</v>
+        <v>2440</v>
       </c>
       <c r="L49" s="0" t="n">
         <v>100</v>
       </c>
       <c r="M49" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N49" s="0" t="n">
         <v>100</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P49" s="0" t="n">
         <v>100</v>
       </c>
       <c r="Q49" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="R49" s="0" t="n">
         <v>100</v>
       </c>
       <c r="S49" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="T49" s="2" t="n">
         <f aca="false">SUM(J49,L49,N49,P49*2,R49*2)</f>
-        <v>1900</v>
+        <v>1820</v>
       </c>
       <c r="U49" s="2" t="n">
         <f aca="false">K49+SUM(L49:O49)+SUM(P49:S49)*2</f>
-        <v>3365</v>
+        <v>3340</v>
       </c>
       <c r="V49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W49" s="1" t="n">
         <f aca="false">U49+V49</f>
-        <v>3365</v>
+        <v>3340</v>
       </c>
       <c r="X49" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="AB49" s="0" t="n">
         <v>28</v>
@@ -11037,33 +11047,33 @@
         <v>360</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="G50" s="1" t="n">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="J50" s="2" t="n">
         <f aca="false">SUM(B50,D50,F50*2,H50*2)</f>
-        <v>1460</v>
+        <v>1300</v>
       </c>
       <c r="K50" s="2" t="n">
         <f aca="false">SUM(B50:E50) + SUM(F50:I50)*2</f>
-        <v>2395</v>
+        <v>2165</v>
       </c>
       <c r="L50" s="0" t="n">
         <v>100</v>
@@ -11091,24 +11101,33 @@
       </c>
       <c r="T50" s="2" t="n">
         <f aca="false">SUM(J50,L50,N50,P50*2,R50*2)</f>
-        <v>2060</v>
+        <v>1900</v>
       </c>
       <c r="U50" s="2" t="n">
         <f aca="false">K50+SUM(L50:O50)+SUM(P50:S50)*2</f>
-        <v>3595</v>
+        <v>3365</v>
       </c>
       <c r="V50" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W50" s="1" t="n">
         <f aca="false">U50+V50</f>
-        <v>3595</v>
+        <v>3365</v>
       </c>
       <c r="X50" s="1" t="n">
         <v>39</v>
       </c>
       <c r="Y50" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AB50" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC50" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD50" s="0" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11119,7 +11138,7 @@
         <v>360</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>260</v>
@@ -11131,7 +11150,7 @@
         <v>210</v>
       </c>
       <c r="G51" s="1" t="n">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>210</v>
@@ -11145,7 +11164,7 @@
       </c>
       <c r="K51" s="2" t="n">
         <f aca="false">SUM(B51:E51) + SUM(F51:I51)*2</f>
-        <v>2415</v>
+        <v>2395</v>
       </c>
       <c r="L51" s="0" t="n">
         <v>100</v>
@@ -11177,14 +11196,14 @@
       </c>
       <c r="U51" s="2" t="n">
         <f aca="false">K51+SUM(L51:O51)+SUM(P51:S51)*2</f>
-        <v>3615</v>
+        <v>3595</v>
       </c>
       <c r="V51" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W51" s="1" t="n">
         <f aca="false">U51+V51</f>
-        <v>3615</v>
+        <v>3595</v>
       </c>
       <c r="X51" s="1" t="n">
         <v>39</v>
@@ -11192,58 +11211,42 @@
       <c r="Y51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z51" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AA51" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="AB51" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AC51" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="AD51" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="AE51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>88</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>500</v>
+        <v>360</v>
       </c>
       <c r="C52" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F52" s="0" t="n">
         <v>210</v>
       </c>
-      <c r="D52" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="E52" s="1" t="n">
+      <c r="G52" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F52" s="0" t="n">
-        <v>290</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>110</v>
-      </c>
       <c r="H52" s="0" t="n">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="J52" s="2" t="n">
         <f aca="false">SUM(B52,D52,F52*2,H52*2)</f>
-        <v>1860</v>
+        <v>1460</v>
       </c>
       <c r="K52" s="2" t="n">
         <f aca="false">SUM(B52:E52) + SUM(F52:I52)*2</f>
-        <v>2650</v>
+        <v>2415</v>
       </c>
       <c r="L52" s="0" t="n">
         <v>100</v>
@@ -11271,18 +11274,18 @@
       </c>
       <c r="T52" s="2" t="n">
         <f aca="false">SUM(J52,L52,N52,P52*2,R52*2)</f>
-        <v>2460</v>
+        <v>2060</v>
       </c>
       <c r="U52" s="2" t="n">
         <f aca="false">K52+SUM(L52:O52)+SUM(P52:S52)*2</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="V52" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W52" s="1" t="n">
         <f aca="false">U52+V52</f>
-        <v>3850</v>
+        <v>3615</v>
       </c>
       <c r="X52" s="1" t="n">
         <v>39</v>
@@ -11290,54 +11293,58 @@
       <c r="Y52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB52" s="0" t="s">
-        <v>42</v>
+      <c r="Z52" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA52" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AB52" s="0" t="n">
+        <v>35</v>
       </c>
       <c r="AC52" s="0" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AD52" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AE52" s="10" t="s">
-        <v>89</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="AE52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="G53" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H53" s="0" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="J53" s="2" t="n">
         <f aca="false">SUM(B53,D53,F53*2,H53*2)</f>
-        <v>1820</v>
+        <v>1860</v>
       </c>
       <c r="K53" s="2" t="n">
         <f aca="false">SUM(B53:E53) + SUM(F53:I53)*2</f>
-        <v>2810</v>
+        <v>2650</v>
       </c>
       <c r="L53" s="0" t="n">
         <v>100</v>
@@ -11365,18 +11372,18 @@
       </c>
       <c r="T53" s="2" t="n">
         <f aca="false">SUM(J53,L53,N53,P53*2,R53*2)</f>
-        <v>2420</v>
+        <v>2460</v>
       </c>
       <c r="U53" s="2" t="n">
         <f aca="false">K53+SUM(L53:O53)+SUM(P53:S53)*2</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="V53" s="1" t="n">
         <v>0</v>
       </c>
       <c r="W53" s="1" t="n">
         <f aca="false">U53+V53</f>
-        <v>4010</v>
+        <v>3850</v>
       </c>
       <c r="X53" s="1" t="n">
         <v>39</v>
@@ -11384,13 +11391,7 @@
       <c r="Y53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z53" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AA53" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AB53" s="0" t="n">
+      <c r="AB53" s="0" t="s">
         <v>42</v>
       </c>
       <c r="AC53" s="0" t="n">
@@ -11399,7 +11400,107 @@
       <c r="AD53" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="AE53" s="10"/>
+      <c r="AE53" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <f aca="false">SUM(B54,D54,F54*2,H54*2)</f>
+        <v>1820</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <f aca="false">SUM(B54:E54) + SUM(F54:I54)*2</f>
+        <v>2810</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M54" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O54" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q54" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S54" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T54" s="2" t="n">
+        <f aca="false">SUM(J54,L54,N54,P54*2,R54*2)</f>
+        <v>2420</v>
+      </c>
+      <c r="U54" s="2" t="n">
+        <f aca="false">K54+SUM(L54:O54)+SUM(P54:S54)*2</f>
+        <v>4010</v>
+      </c>
+      <c r="V54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" s="1" t="n">
+        <f aca="false">U54+V54</f>
+        <v>4010</v>
+      </c>
+      <c r="X54" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z54" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA54" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB54" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC54" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD54" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AE54" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -11436,7 +11537,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CF28141B-507F-4815-A0BF-6A1650405F82}</x14:id>
+          <x14:id>{4490C934-3CDC-4F5C-86F1-E06C562A7986}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11450,7 +11551,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1099D4EF-E12D-4094-9690-B00023D1135E}</x14:id>
+          <x14:id>{4C43C4D1-E5A8-4143-8F42-C0C439F6AAAC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11464,12 +11565,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A9CB3D42-C061-456E-B262-8648223378E0}</x14:id>
+          <x14:id>{B5CD5E16-2C96-41D7-9271-3134155A7A2A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:AD73">
+  <conditionalFormatting sqref="Z45:AD74 Z3:AD43">
     <cfRule type="dataBar" priority="5">
       <dataBar showValue="1" minLength="0" maxLength="100">
         <cfvo type="num" val="1"/>
@@ -11478,7 +11579,77 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D6B91C25-71E2-4E43-82E3-58852FE6F017}</x14:id>
+          <x14:id>{83C8DA16-AB87-4B72-9DAE-5D94D826E1F1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z44">
+    <cfRule type="dataBar" priority="6">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{198F25BA-55B7-4FE7-A531-3517FB115E71}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA44">
+    <cfRule type="dataBar" priority="7">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EDC6C94F-8290-42E3-805D-9D4EB01A2021}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB44">
+    <cfRule type="dataBar" priority="8">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{666E642C-2DBC-4EB5-926A-C3203A8BD9F0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC44">
+    <cfRule type="dataBar" priority="9">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F4D7127A-EA31-4AB8-96AA-6287FFBEC345}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD44">
+    <cfRule type="dataBar" priority="10">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{44475360-C633-4C58-96A9-CF4212145DD2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11495,7 +11666,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CF28141B-507F-4815-A0BF-6A1650405F82}">
+          <x14:cfRule type="dataBar" id="{4490C934-3CDC-4F5C-86F1-E06C562A7986}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11506,7 +11677,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1099D4EF-E12D-4094-9690-B00023D1135E}">
+          <x14:cfRule type="dataBar" id="{4C43C4D1-E5A8-4143-8F42-C0C439F6AAAC}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11517,7 +11688,7 @@
           <xm:sqref>T2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A9CB3D42-C061-456E-B262-8648223378E0}">
+          <x14:cfRule type="dataBar" id="{B5CD5E16-2C96-41D7-9271-3134155A7A2A}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11528,7 +11699,7 @@
           <xm:sqref>J2:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D6B91C25-71E2-4E43-82E3-58852FE6F017}">
+          <x14:cfRule type="dataBar" id="{83C8DA16-AB87-4B72-9DAE-5D94D826E1F1}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11540,7 +11711,82 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Z3:AD73</xm:sqref>
+          <xm:sqref>Z45:AD74 Z3:AD43</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{198F25BA-55B7-4FE7-A531-3517FB115E71}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Z44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EDC6C94F-8290-42E3-805D-9D4EB01A2021}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AA44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{666E642C-2DBC-4EB5-926A-C3203A8BD9F0}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AB44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F4D7127A-EA31-4AB8-96AA-6287FFBEC345}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AC44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{44475360-C633-4C58-96A9-CF4212145DD2}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AD44</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -11559,7 +11805,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.9"/>
@@ -11572,7 +11818,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>29</v>
@@ -11590,22 +11836,22 @@
         <v>59</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11637,7 +11883,7 @@
         <v>870</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11738,7 +11984,7 @@
         <v>1625</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11789,7 +12035,7 @@
         <v>1625</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11815,7 +12061,7 @@
         <v>1625</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11823,54 +12069,54 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -11896,7 +12142,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -11906,7 +12152,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>32</v>
@@ -11915,7 +12161,7 @@
         <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>38</v>
@@ -11927,28 +12173,28 @@
         <v>76</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12264,84 +12510,84 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12370,7 +12616,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -12378,13 +12624,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12449,18 +12695,18 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -12486,7 +12732,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -12495,7 +12741,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>32</v>
@@ -12510,28 +12756,28 @@
         <v>59</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>76</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12733,76 +12979,76 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>117</v>
-      </c>
       <c r="C17" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="L18" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="16"/>
     </row>
@@ -12832,7 +13078,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -12846,25 +13092,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>41</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add a patch for Porshet-5 power armor
* Lock the cellar door with a Master lock
* Make legendary and normal P-5 available for sale from The Collector
* Add an optional configuration for making P-5 available as a legendary drop (disabled by default)
* Add an optional configuration for making P-5 available for the Brotherhood of Steel (disabled by default)
</commit_message>
<xml_diff>
--- a/Balancing Data/Power Armor Stats.xlsx
+++ b/Balancing Data/Power Armor Stats.xlsx
@@ -1737,11 +1737,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84048517"/>
-        <c:axId val="81402495"/>
+        <c:axId val="28526606"/>
+        <c:axId val="95294392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84048517"/>
+        <c:axId val="28526606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1772,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81402495"/>
+        <c:crossAx val="95294392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81402495"/>
+        <c:axId val="95294392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1820,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84048517"/>
+        <c:crossAx val="28526606"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3494,11 +3494,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="44565758"/>
-        <c:axId val="29746737"/>
+        <c:axId val="85341511"/>
+        <c:axId val="35673429"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44565758"/>
+        <c:axId val="85341511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +3529,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29746737"/>
+        <c:crossAx val="35673429"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3537,7 +3537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29746737"/>
+        <c:axId val="35673429"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3577,7 +3577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44565758"/>
+        <c:crossAx val="85341511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3761,11 +3761,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="2349601"/>
-        <c:axId val="69778334"/>
+        <c:axId val="48571779"/>
+        <c:axId val="34425147"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2349601"/>
+        <c:axId val="48571779"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3796,7 +3796,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69778334"/>
+        <c:crossAx val="34425147"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3804,7 +3804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69778334"/>
+        <c:axId val="34425147"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3844,7 +3844,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2349601"/>
+        <c:crossAx val="48571779"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5259,11 +5259,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="53018299"/>
-        <c:axId val="60898876"/>
+        <c:axId val="39961325"/>
+        <c:axId val="85424633"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53018299"/>
+        <c:axId val="39961325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5294,7 +5294,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60898876"/>
+        <c:crossAx val="85424633"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5302,7 +5302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60898876"/>
+        <c:axId val="85424633"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5342,7 +5342,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53018299"/>
+        <c:crossAx val="39961325"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6341,11 +6341,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="38877117"/>
-        <c:axId val="15603435"/>
+        <c:axId val="11777580"/>
+        <c:axId val="36507352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38877117"/>
+        <c:axId val="11777580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6410,7 +6410,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15603435"/>
+        <c:crossAx val="36507352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6418,7 +6418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15603435"/>
+        <c:axId val="36507352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6492,7 +6492,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38877117"/>
+        <c:crossAx val="11777580"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6554,9 +6554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:colOff>273960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6565,7 +6565,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2732400"/>
-        <a:ext cx="7781040" cy="4265640"/>
+        <a:ext cx="7780680" cy="4265280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6589,9 +6589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>376560</xdr:colOff>
+      <xdr:colOff>376200</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6600,7 +6600,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216960"/>
-        <a:ext cx="10434600" cy="4265640"/>
+        <a:ext cx="10447200" cy="4265280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6624,9 +6624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>506880</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6635,7 +6635,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="2243160"/>
-        <a:ext cx="7831800" cy="4265640"/>
+        <a:ext cx="7841880" cy="4265280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6659,9 +6659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6670,7 +6670,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="468720" y="3216960"/>
-        <a:ext cx="10415520" cy="4265640"/>
+        <a:ext cx="10426680" cy="4265280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6694,9 +6694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>57960</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6705,7 +6705,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="260280" y="2632320"/>
-        <a:ext cx="8465760" cy="4703760"/>
+        <a:ext cx="8465400" cy="4703400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6726,14 +6726,14 @@
   <dimension ref="A1:AE54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="W15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="Q15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="Z43" activeCellId="0" sqref="Z43"/>
+      <selection pane="bottomRight" activeCell="AE33" activeCellId="0" sqref="AE33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.83"/>
@@ -9585,6 +9585,12 @@
       <c r="W33" s="1" t="n">
         <f aca="false">U33+V33</f>
         <v>3000</v>
+      </c>
+      <c r="AC33" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD33" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="AE33" s="10" t="s">
         <v>62</v>
@@ -11537,7 +11543,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4490C934-3CDC-4F5C-86F1-E06C562A7986}</x14:id>
+          <x14:id>{D0554C92-EE5E-4C89-B4D0-E0804AC630C5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11551,7 +11557,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4C43C4D1-E5A8-4143-8F42-C0C439F6AAAC}</x14:id>
+          <x14:id>{20E9A2F5-C4F0-48CB-AAD7-911CA5232B90}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11565,7 +11571,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B5CD5E16-2C96-41D7-9271-3134155A7A2A}</x14:id>
+          <x14:id>{BA5D8040-5346-47A0-AF75-1F7197117C99}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11579,7 +11585,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{83C8DA16-AB87-4B72-9DAE-5D94D826E1F1}</x14:id>
+          <x14:id>{219AEC8D-29A7-4AAF-941B-99DBB3EAE147}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11593,7 +11599,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{198F25BA-55B7-4FE7-A531-3517FB115E71}</x14:id>
+          <x14:id>{5B7AE096-95F4-4196-B4AF-B320C0C495E3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11607,7 +11613,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EDC6C94F-8290-42E3-805D-9D4EB01A2021}</x14:id>
+          <x14:id>{4049293D-3ADE-40E4-88B4-D1E147EEDD39}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11621,7 +11627,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{666E642C-2DBC-4EB5-926A-C3203A8BD9F0}</x14:id>
+          <x14:id>{E95DDE72-358C-45EB-A895-902D90A29764}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11635,7 +11641,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F4D7127A-EA31-4AB8-96AA-6287FFBEC345}</x14:id>
+          <x14:id>{1A232FDC-AFDA-4781-939E-66447ABDA4CA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11649,7 +11655,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{44475360-C633-4C58-96A9-CF4212145DD2}</x14:id>
+          <x14:id>{B77BEC4F-5AED-4A7A-A7F5-147B52DA9FED}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11666,7 +11672,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4490C934-3CDC-4F5C-86F1-E06C562A7986}">
+          <x14:cfRule type="dataBar" id="{D0554C92-EE5E-4C89-B4D0-E0804AC630C5}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11677,7 +11683,7 @@
           <xm:sqref>W2:W1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4C43C4D1-E5A8-4143-8F42-C0C439F6AAAC}">
+          <x14:cfRule type="dataBar" id="{20E9A2F5-C4F0-48CB-AAD7-911CA5232B90}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11688,7 +11694,7 @@
           <xm:sqref>T2:U1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B5CD5E16-2C96-41D7-9271-3134155A7A2A}">
+          <x14:cfRule type="dataBar" id="{BA5D8040-5346-47A0-AF75-1F7197117C99}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -11699,7 +11705,7 @@
           <xm:sqref>J2:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{83C8DA16-AB87-4B72-9DAE-5D94D826E1F1}">
+          <x14:cfRule type="dataBar" id="{219AEC8D-29A7-4AAF-941B-99DBB3EAE147}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11714,7 +11720,7 @@
           <xm:sqref>Z45:AD74 Z3:AD43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{198F25BA-55B7-4FE7-A531-3517FB115E71}">
+          <x14:cfRule type="dataBar" id="{5B7AE096-95F4-4196-B4AF-B320C0C495E3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11729,7 +11735,7 @@
           <xm:sqref>Z44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EDC6C94F-8290-42E3-805D-9D4EB01A2021}">
+          <x14:cfRule type="dataBar" id="{4049293D-3ADE-40E4-88B4-D1E147EEDD39}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11744,7 +11750,7 @@
           <xm:sqref>AA44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{666E642C-2DBC-4EB5-926A-C3203A8BD9F0}">
+          <x14:cfRule type="dataBar" id="{E95DDE72-358C-45EB-A895-902D90A29764}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11759,7 +11765,7 @@
           <xm:sqref>AB44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F4D7127A-EA31-4AB8-96AA-6287FFBEC345}">
+          <x14:cfRule type="dataBar" id="{1A232FDC-AFDA-4781-939E-66447ABDA4CA}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11774,7 +11780,7 @@
           <xm:sqref>AC44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{44475360-C633-4C58-96A9-CF4212145DD2}">
+          <x14:cfRule type="dataBar" id="{B77BEC4F-5AED-4A7A-A7F5-147B52DA9FED}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>1</xm:f>
@@ -11805,7 +11811,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.9"/>
@@ -12142,7 +12148,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
@@ -12616,7 +12622,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.55"/>
@@ -12732,7 +12738,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="15.46"/>
@@ -13078,7 +13084,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>

</xml_diff>